<commit_message>
Refactored Test Suites for Choose Modem
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -27,10 +27,38 @@
     <t>Excel Worksheet Name</t>
   </si>
   <si>
+    <t>Export Summary</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
     <t>Testdata</t>
   </si>
   <si>
-    <t>Table 1</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Testdata</t>
+    </r>
+  </si>
+  <si>
+    <t>Locators</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Locators</t>
+    </r>
   </si>
   <si>
     <t>TCName</t>
@@ -39,7 +67,7 @@
     <t>verifyGetStartedPages</t>
   </si>
   <si>
-    <t>text1=Welcome to Globe myBusiness</t>
+    <t>text1=Welcometo Globe myBusiness</t>
   </si>
   <si>
     <t>text2=Manage your myBusiness Prepaid Internet number</t>
@@ -69,15 +97,9 @@
     <t>verifyChooseModemOne</t>
   </si>
   <si>
-    <t>text1=Welcometo Globe myBusiness</t>
-  </si>
-  <si>
     <t>nickname=Abe</t>
   </si>
   <si>
-    <t>Locators</t>
-  </si>
-  <si>
     <t>Page</t>
   </si>
   <si>
@@ -153,48 +175,49 @@
     <t>letsGoButton</t>
   </si>
   <si>
-    <t xml:space="preserve">//android.widget.Button[@resource-id='ph.com.globe.mybusiness:id/btn_next']
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skipBtn
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//android.widget.TextView[@resource-id='ph.com.globe.mybusiness:id/tv_skip']
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">closeModalBtn
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//android.widget.RelativeLayout[@resource-id='ph.com.globe.mybusiness:id/rl_dialog_button_container']
-</t>
+    <t>//android.widget.Button[@resource-id='ph.com.globe.mybusiness:id/btn_next']</t>
+  </si>
+  <si>
+    <t>skipBtn</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/tv_skip</t>
+  </si>
+  <si>
+    <t>modalPopOut</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/action_bar_root</t>
+  </si>
+  <si>
+    <t>closeModalBtn</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='ph.com.globe.mybusiness:id/btn_positive']</t>
   </si>
   <si>
     <t>modemOneBtn</t>
   </si>
   <si>
-    <t>//android.widget.ImageView)[1]</t>
+    <t>(//android.widget.ImageView)[1]</t>
   </si>
   <si>
     <t>modemTwoBtn</t>
   </si>
   <si>
-    <t>//android.widget.ImageView)[2]</t>
+    <t>(//android.widget.ImageView)[2]</t>
   </si>
   <si>
     <t>modemThreeBtn</t>
   </si>
   <si>
-    <t>//android.widget.ImageView)[3]</t>
+    <t>(//android.widget.ImageView)[3]</t>
   </si>
   <si>
     <t>modemFourBtn</t>
   </si>
   <si>
-    <t>//android.widget.ImageView)[4]</t>
+    <t>(//android.widget.ImageView)[4]</t>
   </si>
   <si>
     <t>policyCheckbox</t>
@@ -254,7 +277,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,8 +296,26 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -284,49 +325,55 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
+      <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom/>
@@ -334,13 +381,85 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -349,7 +468,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -371,40 +490,100 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -427,7 +606,10 @@
       <rgbColor rgb="015e88b1"/>
       <rgbColor rgb="01eef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -626,12 +808,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -664,10 +846,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -915,12 +1097,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1235,10 +1417,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1489,73 +1671,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" style="6" customWidth="1"/>
     <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="2" max="2" width="33.6719" style="6" customWidth="1"/>
+    <col min="3" max="3" width="33.6719" style="6" customWidth="1"/>
+    <col min="4" max="4" width="33.6719" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="256" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="13.65" customHeight="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s" s="13">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="14">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="14">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="14">
         <v>3</v>
       </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9">
-      <c r="B9" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="10"/>
+      <c r="B9" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="17"/>
+      <c r="C10" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="D10" t="s" s="19">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="10"/>
       <c r="B11" t="s" s="3">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" ht="13" customHeight="1">
+      <c r="A12" s="20"/>
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>20</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" ht="13" customHeight="1">
+      <c r="A13" s="7"/>
+      <c r="B13" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" ht="13" customHeight="1">
+      <c r="A14" s="20"/>
+      <c r="B14" s="4"/>
+      <c r="C14" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s" s="5">
+        <v>8</v>
+      </c>
+      <c r="E14" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
+    <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
-    <hyperlink ref="D12" location="'Locators'!R1C1" tooltip="" display="Locators"/>
+    <hyperlink ref="D12" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
+    <hyperlink ref="D14" location="'Locators'!R1C1" tooltip="" display="Locators"/>
+    <hyperlink ref="D12" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
+    <hyperlink ref="D14" location="'Locators'!R1C1" tooltip="" display="Locators"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1567,143 +1843,143 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="25.3516" style="6" customWidth="1"/>
-    <col min="2" max="2" width="32.8516" style="6" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.6719" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24.3516" style="6" customWidth="1"/>
-    <col min="6" max="6" width="15" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="6" customWidth="1"/>
-    <col min="8" max="256" width="14.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="25.3516" style="25" customWidth="1"/>
+    <col min="2" max="2" width="32.8516" style="25" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="25" customWidth="1"/>
+    <col min="4" max="4" width="23.6719" style="25" customWidth="1"/>
+    <col min="5" max="5" width="24.3516" style="25" customWidth="1"/>
+    <col min="6" max="6" width="15" style="25" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="25" customWidth="1"/>
+    <col min="8" max="256" width="14.5" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" t="s" s="7">
+      <c r="A1" t="s" s="26">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s" s="27">
         <v>6</v>
       </c>
-      <c r="B1" t="s" s="8">
-        <v>4</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s" s="7">
+      <c r="A2" t="s" s="26">
         <v>11</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="B2" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s" s="26">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s" s="26">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s" s="26">
+        <v>15</v>
+      </c>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" t="s" s="7">
+      <c r="A3" t="s" s="26">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s" s="26">
+        <v>19</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" t="s" s="26">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="26">
         <v>12</v>
       </c>
-      <c r="B3" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="C5" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="D5" t="s" s="26">
         <v>18</v>
       </c>
-      <c r="C5" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="E5" t="s" s="26">
+        <v>22</v>
+      </c>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1725,470 +2001,466 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.3516" style="10" customWidth="1"/>
-    <col min="2" max="2" width="19" style="10" customWidth="1"/>
-    <col min="3" max="3" width="19.3516" style="10" customWidth="1"/>
-    <col min="4" max="4" width="77.8516" style="10" customWidth="1"/>
-    <col min="5" max="5" width="21.3516" style="10" customWidth="1"/>
-    <col min="6" max="6" width="11.3516" style="10" customWidth="1"/>
-    <col min="7" max="256" width="14.5" style="10" customWidth="1"/>
+    <col min="1" max="1" width="19.3516" style="29" customWidth="1"/>
+    <col min="2" max="2" width="19" style="29" customWidth="1"/>
+    <col min="3" max="3" width="19.3516" style="29" customWidth="1"/>
+    <col min="4" max="4" width="77.8516" style="29" customWidth="1"/>
+    <col min="5" max="5" width="21.3516" style="29" customWidth="1"/>
+    <col min="6" max="6" width="11.3516" style="29" customWidth="1"/>
+    <col min="7" max="256" width="14.5" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s" s="7">
+      <c r="A1" t="s" s="26">
         <v>23</v>
       </c>
-      <c r="D1" t="s" s="7">
+      <c r="B1" t="s" s="26">
         <v>24</v>
       </c>
-      <c r="E1" t="s" s="7">
+      <c r="C1" t="s" s="26">
         <v>25</v>
       </c>
-      <c r="F1" t="s" s="7">
+      <c r="D1" t="s" s="26">
         <v>26</v>
       </c>
+      <c r="E1" t="s" s="26">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s" s="26">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s" s="7">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s" s="7">
+      <c r="A2" t="s" s="26">
         <v>29</v>
       </c>
-      <c r="D2" t="s" s="7">
+      <c r="B2" t="s" s="26">
         <v>30</v>
       </c>
-      <c r="E2" t="s" s="7">
+      <c r="C2" t="s" s="26">
         <v>31</v>
       </c>
-      <c r="F2" t="s" s="7">
+      <c r="D2" t="s" s="26">
         <v>32</v>
       </c>
+      <c r="E2" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s" s="26">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" t="s" s="7">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s" s="7">
+      <c r="A3" t="s" s="26">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s" s="26">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s" s="26">
         <v>33</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="D3" t="s" s="26">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s" s="26">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1">
+      <c r="A4" t="s" s="26">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s" s="26">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s" s="26">
         <v>31</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="D4" t="s" s="30">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s" s="26">
         <v>34</v>
       </c>
-      <c r="E3" t="s" s="7">
+    </row>
+    <row r="5" ht="12.75" customHeight="1">
+      <c r="A5" t="s" s="26">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s" s="30">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s" s="26">
         <v>31</v>
       </c>
-      <c r="F3" t="s" s="7">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s" s="11">
+      <c r="D5" t="s" s="30">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s" s="31">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1">
+      <c r="A6" t="s" s="26">
         <v>37</v>
       </c>
-      <c r="E4" t="s" s="7">
+      <c r="B6" t="s" s="30">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s" s="30">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s" s="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1">
+      <c r="A7" t="s" s="26">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s" s="30">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s" s="26">
         <v>31</v>
       </c>
-      <c r="F4" t="s" s="7">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s" s="11">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s" s="11">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s" s="7">
+      <c r="D7" t="s" s="30">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s" s="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="1">
+      <c r="A8" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s" s="26">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s" s="34">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s" s="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="1">
+      <c r="A9" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s" s="34">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s" s="26">
         <v>31</v>
       </c>
-      <c r="F5" t="s" s="12">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s" s="11">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s" s="7">
+      <c r="D9" t="s" s="34">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s" s="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" ht="12.75" customHeight="1">
+      <c r="A10" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s" s="26">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s" s="26">
         <v>31</v>
       </c>
-      <c r="D6" t="s" s="11">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s" s="13">
+      <c r="D10" t="s" s="26">
+        <v>52</v>
+      </c>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
+    </row>
+    <row r="11" ht="12.75" customHeight="1">
+      <c r="A11" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s" s="34">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s" s="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" ht="12.75" customHeight="1">
+      <c r="A12" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s" s="26">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s" s="26">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s" s="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" ht="12.75" customHeight="1">
+      <c r="A13" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s" s="26">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s" s="26">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s" s="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" ht="12.75" customHeight="1">
+      <c r="A14" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s" s="26">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s" s="26">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s" s="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" ht="12.75" customHeight="1">
+      <c r="A15" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s" s="26">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s" s="26">
+        <v>62</v>
+      </c>
+      <c r="E15" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="F15" t="s" s="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" ht="12.75" customHeight="1">
+      <c r="A16" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s" s="26">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s" s="26">
+        <v>64</v>
+      </c>
+      <c r="E16" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="F16" t="s" s="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s" s="26">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s" s="26">
         <v>31</v>
       </c>
-      <c r="F6" t="s" s="14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s" s="11">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s" s="11">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="F7" t="s" s="14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="B8" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s" s="15">
-        <v>46</v>
-      </c>
-      <c r="E8" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="F8" t="s" s="14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s" s="15">
-        <v>47</v>
-      </c>
-      <c r="C9" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s" s="15">
-        <v>48</v>
-      </c>
-      <c r="E9" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s" s="14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s" s="15">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s" s="15">
-        <v>50</v>
-      </c>
-      <c r="E10" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="F10" t="s" s="14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s" s="7">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s" s="7">
-        <v>52</v>
-      </c>
-      <c r="E11" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="F11" t="s" s="14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="B12" t="s" s="7">
-        <v>53</v>
-      </c>
-      <c r="C12" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s" s="7">
-        <v>54</v>
-      </c>
-      <c r="E12" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="F12" t="s" s="14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="B13" t="s" s="7">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s" s="7">
-        <v>56</v>
-      </c>
-      <c r="E13" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="F13" t="s" s="14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="B14" t="s" s="7">
-        <v>57</v>
-      </c>
-      <c r="C14" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s" s="7">
-        <v>58</v>
-      </c>
-      <c r="E14" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="F14" t="s" s="14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="B15" t="s" s="7">
-        <v>59</v>
-      </c>
-      <c r="C15" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s" s="7">
-        <v>60</v>
-      </c>
-      <c r="E15" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="F15" t="s" s="14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="B16" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D16" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="E16" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="F16" t="s" s="16">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s" s="7">
-        <v>61</v>
-      </c>
-      <c r="C17" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D17" t="s" s="7">
-        <v>62</v>
-      </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
+      <c r="D17" t="s" s="26">
+        <v>66</v>
+      </c>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="36"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="18"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="18"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="36"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="18"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="36"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="18"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="18"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="18"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="18"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="18"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="36"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="18"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="36"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="18"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="36"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="18"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Added HomePage Test Suites
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -98,6 +98,24 @@
   </si>
   <si>
     <t>nickname=Abe</t>
+  </si>
+  <si>
+    <t>verifyChooseModemTwo</t>
+  </si>
+  <si>
+    <t>nickname=Abraham</t>
+  </si>
+  <si>
+    <t>verifyChooseModemThree</t>
+  </si>
+  <si>
+    <t>nickname=Ham</t>
+  </si>
+  <si>
+    <t>verifyChooseModemFour</t>
+  </si>
+  <si>
+    <t>nickname=Honestabe</t>
   </si>
   <si>
     <t>Page</t>
@@ -1937,29 +1955,59 @@
       <c r="G5" s="28"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="A6" t="s" s="26">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s" s="26">
+        <v>24</v>
+      </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="A7" t="s" s="26">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s" s="26">
+        <v>26</v>
+      </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="A8" t="s" s="26">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s" s="26">
+        <v>28</v>
+      </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
     </row>
@@ -2012,332 +2060,332 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" t="s" s="26">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s" s="26">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s" s="26">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s" s="26">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s" s="26">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s" s="26">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" t="s" s="26">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s" s="26">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s" s="26">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s" s="26">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s" s="26">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s" s="26">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" t="s" s="26">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s" s="26">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s" s="26">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s" s="26">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s" s="26">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s" s="26">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" t="s" s="26">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s" s="26">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s" s="26">
         <v>37</v>
       </c>
-      <c r="B4" t="s" s="26">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s" s="26">
-        <v>31</v>
-      </c>
       <c r="D4" t="s" s="30">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s" s="26">
         <v>39</v>
       </c>
-      <c r="E4" t="s" s="26">
-        <v>33</v>
-      </c>
       <c r="F4" t="s" s="26">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" t="s" s="26">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s" s="30">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s" s="26">
         <v>37</v>
       </c>
-      <c r="B5" t="s" s="30">
+      <c r="D5" t="s" s="30">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s" s="26">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s" s="31">
         <v>40</v>
-      </c>
-      <c r="C5" t="s" s="26">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s" s="30">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s" s="26">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s" s="31">
-        <v>34</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" t="s" s="26">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s" s="30">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s" s="26">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s" s="30">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s" s="32">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s" s="33">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" t="s" s="26">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s" s="30">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s" s="26">
         <v>37</v>
       </c>
-      <c r="B7" t="s" s="30">
-        <v>44</v>
-      </c>
-      <c r="C7" t="s" s="26">
-        <v>31</v>
-      </c>
       <c r="D7" t="s" s="30">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s" s="32">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s" s="33">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" t="s" s="26">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s" s="26">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s" s="26">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s" s="34">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s" s="32">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s" s="33">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" t="s" s="26">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s" s="34">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s" s="26">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s" s="34">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s" s="32">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s" s="33">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" t="s" s="26">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s" s="26">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s" s="26">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s" s="26">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="36"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" t="s" s="26">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s" s="34">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s" s="26">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s" s="34">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s" s="32">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s" s="33">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" t="s" s="26">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s" s="26">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s" s="26">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s" s="26">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s" s="32">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s" s="33">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" t="s" s="26">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s" s="26">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s" s="26">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s" s="32">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s" s="33">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" t="s" s="26">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s" s="26">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s" s="26">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s" s="26">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s" s="32">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s" s="33">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" t="s" s="26">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s" s="26">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s" s="26">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s" s="26">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s" s="32">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F15" t="s" s="33">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" t="s" s="26">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s" s="26">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s" s="26">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s" s="26">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s" s="32">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s" s="33">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" t="s" s="26">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s" s="26">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s" s="26">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s" s="26">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="36"/>

</xml_diff>

<commit_message>
Added Modem Configuration Page Test
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -118,6 +118,12 @@
     <t>nickname=Honestabe</t>
   </si>
   <si>
+    <t>verifyUserAlreadyConnected</t>
+  </si>
+  <si>
+    <t>nickname=Hendrix</t>
+  </si>
+  <si>
     <t>Page</t>
   </si>
   <si>
@@ -248,6 +254,15 @@
   </si>
   <si>
     <t>ph.com.globe.mybusiness:id/spet_acct</t>
+  </si>
+  <si>
+    <t>ModemConfigurationPage</t>
+  </si>
+  <si>
+    <t>imAlreadyConnBtn</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/btn_already_connected</t>
   </si>
 </sst>
 </file>
@@ -486,7 +501,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -597,6 +612,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -2012,11 +2030,21 @@
       <c r="G8" s="28"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
+      <c r="A9" t="s" s="26">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s" s="26">
+        <v>30</v>
+      </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
     </row>
@@ -2060,342 +2088,350 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" t="s" s="26">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s" s="26">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s" s="26">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s" s="26">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s" s="26">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s" s="26">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" t="s" s="26">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s" s="26">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s" s="26">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s" s="26">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s" s="26">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s" s="26">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" t="s" s="26">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s" s="26">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s" s="26">
         <v>41</v>
       </c>
-      <c r="C3" t="s" s="26">
-        <v>39</v>
-      </c>
       <c r="D3" t="s" s="26">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s" s="26">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s" s="26">
         <v>42</v>
-      </c>
-      <c r="E3" t="s" s="26">
-        <v>39</v>
-      </c>
-      <c r="F3" t="s" s="26">
-        <v>40</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" t="s" s="26">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s" s="26">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s" s="26">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s" s="30">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s" s="26">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s" s="26">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" t="s" s="26">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s" s="30">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s" s="26">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s" s="30">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s" s="26">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s" s="31">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" t="s" s="26">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s" s="30">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s" s="26">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s" s="30">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s" s="32">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s" s="33">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" t="s" s="26">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s" s="30">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s" s="26">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s" s="30">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s" s="32">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s" s="33">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" t="s" s="26">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s" s="26">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s" s="26">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s" s="34">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s" s="32">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s" s="33">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" t="s" s="26">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s" s="34">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s" s="26">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s" s="34">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s" s="32">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s" s="33">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" t="s" s="26">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s" s="26">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s" s="26">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="36"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" t="s" s="26">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s" s="34">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s" s="26">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s" s="34">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s" s="32">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s" s="33">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" t="s" s="26">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s" s="26">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s" s="26">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s" s="26">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s" s="32">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s" s="33">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" t="s" s="26">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s" s="26">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s" s="26">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s" s="26">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s" s="32">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s" s="33">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" t="s" s="26">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s" s="26">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s" s="26">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s" s="26">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s" s="32">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s" s="33">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" t="s" s="26">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s" s="26">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s" s="26">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s" s="26">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s" s="32">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s" s="33">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" t="s" s="26">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s" s="26">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s" s="26">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s" s="26">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s" s="32">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F16" t="s" s="33">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" t="s" s="26">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s" s="26">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s" s="26">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s" s="26">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="36"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="35"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
+      <c r="A18" t="s" s="32">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s" s="37">
+        <v>76</v>
+      </c>
+      <c r="C18" t="s" s="37">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s" s="37">
+        <v>77</v>
+      </c>
+      <c r="E18" s="38"/>
       <c r="F18" s="12"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
@@ -2508,7 +2544,7 @@
       <c r="C32" s="28"/>
       <c r="D32" s="28"/>
       <c r="E32" s="35"/>
-      <c r="F32" s="38"/>
+      <c r="F32" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Create some changes in ChooseModemPage
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="75">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -27,101 +27,76 @@
     <t>Excel Worksheet Name</t>
   </si>
   <si>
-    <t>Export Summary</t>
+    <t>Testdata</t>
   </si>
   <si>
     <t>Table 1</t>
   </si>
   <si>
-    <t>Testdata</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="11"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Testdata</t>
-    </r>
+    <t>TCName</t>
+  </si>
+  <si>
+    <t>verifyGetStartedPages</t>
+  </si>
+  <si>
+    <t>text1=Welcometo Globe myBusiness</t>
+  </si>
+  <si>
+    <t>text2=Manage your myBusiness Prepaid Internet number</t>
+  </si>
+  <si>
+    <t>text3=Track your data usage</t>
+  </si>
+  <si>
+    <t>text4=Get more data</t>
+  </si>
+  <si>
+    <t>customerProfileEnterNickname</t>
+  </si>
+  <si>
+    <t>mobileNumber=09271080510</t>
+  </si>
+  <si>
+    <t>pin=1111</t>
+  </si>
+  <si>
+    <t>nickname=Lexter</t>
+  </si>
+  <si>
+    <t>customerProfileSkipEnterNickname</t>
+  </si>
+  <si>
+    <t>verifyChooseModemOne</t>
+  </si>
+  <si>
+    <t>nickname=Rafaela</t>
+  </si>
+  <si>
+    <t>verifyChooseModemTwo</t>
+  </si>
+  <si>
+    <t>nickname=Franco</t>
+  </si>
+  <si>
+    <t>verifyChooseModemThree</t>
+  </si>
+  <si>
+    <t>nickname=Atlas</t>
+  </si>
+  <si>
+    <t>verifyChooseModemFour</t>
+  </si>
+  <si>
+    <t>nickname=Chang’e</t>
+  </si>
+  <si>
+    <t>verifyUserAlreadyConnected</t>
+  </si>
+  <si>
+    <t>nickname=Hendrix</t>
   </si>
   <si>
     <t>Locators</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="11"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Locators</t>
-    </r>
-  </si>
-  <si>
-    <t>TCName</t>
-  </si>
-  <si>
-    <t>verifyGetStartedPages</t>
-  </si>
-  <si>
-    <t>text1=Welcometo Globe myBusiness</t>
-  </si>
-  <si>
-    <t>text2=Manage your myBusiness Prepaid Internet number</t>
-  </si>
-  <si>
-    <t>text3=Track your data usage</t>
-  </si>
-  <si>
-    <t>text4=Get more data</t>
-  </si>
-  <si>
-    <t>customerProfileEnterNickname</t>
-  </si>
-  <si>
-    <t>mobileNumber=09271080510</t>
-  </si>
-  <si>
-    <t>pin=1111</t>
-  </si>
-  <si>
-    <t>nickname=Lexter</t>
-  </si>
-  <si>
-    <t>customerProfileSkipEnterNickname</t>
-  </si>
-  <si>
-    <t>verifyChooseModemOne</t>
-  </si>
-  <si>
-    <t>nickname=Abe</t>
-  </si>
-  <si>
-    <t>verifyChooseModemTwo</t>
-  </si>
-  <si>
-    <t>nickname=Abraham</t>
-  </si>
-  <si>
-    <t>verifyChooseModemThree</t>
-  </si>
-  <si>
-    <t>nickname=Ham</t>
-  </si>
-  <si>
-    <t>verifyChooseModemFour</t>
-  </si>
-  <si>
-    <t>nickname=Honestabe</t>
-  </si>
-  <si>
-    <t>verifyUserAlreadyConnected</t>
-  </si>
-  <si>
-    <t>nickname=Hendrix</t>
   </si>
   <si>
     <t>Page</t>
@@ -272,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -305,12 +280,17 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,26 +309,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="14"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="15"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -358,86 +320,29 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
       <bottom style="thin">
         <color indexed="13"/>
       </bottom>
@@ -463,35 +368,159 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
       </right>
       <top style="thin">
         <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,7 +530,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -523,103 +552,79 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -642,10 +647,8 @@
       <rgbColor rgb="015e88b1"/>
       <rgbColor rgb="01eef3f4"/>
       <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff5e88b1"/>
-      <rgbColor rgb="ffeef3f4"/>
+      <rgbColor rgb="ff9a9a9a"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -844,12 +847,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -882,10 +885,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1133,12 +1136,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1453,10 +1456,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1707,167 +1710,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="1" max="1" width="2" style="6" customWidth="1"/>
     <col min="2" max="4" width="33.6016" customWidth="1"/>
-    <col min="2" max="2" width="33.6719" style="6" customWidth="1"/>
-    <col min="3" max="3" width="33.6719" style="6" customWidth="1"/>
-    <col min="4" max="4" width="33.6719" style="6" customWidth="1"/>
-    <col min="5" max="5" width="10" style="6" customWidth="1"/>
-    <col min="6" max="256" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-    </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" t="s" s="13">
+      <c r="B3" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
+      <c r="C3"/>
+      <c r="D3"/>
     </row>
     <row r="7">
-      <c r="A7" s="10"/>
-      <c r="B7" t="s" s="14">
+      <c r="B7" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="14">
+      <c r="C7" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="14">
+      <c r="D7" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
     </row>
     <row r="9">
-      <c r="A9" s="10"/>
-      <c r="B9" t="s" s="15">
-        <v>6</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="12"/>
+      <c r="B9" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10">
-      <c r="A10" s="10"/>
-      <c r="B10" s="17"/>
-      <c r="C10" t="s" s="18">
+      <c r="B10" s="4"/>
+      <c r="C10" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="19">
-        <v>7</v>
-      </c>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" ht="13" customHeight="1">
-      <c r="A11" s="10"/>
+      <c r="D10" t="s" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="B11" t="s" s="3">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" ht="13" customHeight="1">
-      <c r="A12" s="20"/>
+    </row>
+    <row r="12">
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="E12" s="21"/>
-    </row>
-    <row r="13" ht="13" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" t="s" s="3">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" ht="13" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="4"/>
-      <c r="C14" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s" s="5">
-        <v>8</v>
-      </c>
-      <c r="E14" s="21"/>
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:D3"/>
+  <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
-    <hyperlink ref="D12" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
-    <hyperlink ref="D14" location="'Locators'!R1C1" tooltip="" display="Locators"/>
-    <hyperlink ref="D12" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
-    <hyperlink ref="D14" location="'Locators'!R1C1" tooltip="" display="Locators"/>
+    <hyperlink ref="D12" location="'Locators'!R1C1" tooltip="" display="Locators"/>
   </hyperlinks>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -1879,183 +1788,183 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="25.3516" style="25" customWidth="1"/>
-    <col min="2" max="2" width="32.8516" style="25" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="25" customWidth="1"/>
-    <col min="4" max="4" width="23.6719" style="25" customWidth="1"/>
-    <col min="5" max="5" width="24.3516" style="25" customWidth="1"/>
-    <col min="6" max="6" width="15" style="25" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="25" customWidth="1"/>
-    <col min="8" max="256" width="14.5" style="25" customWidth="1"/>
+    <col min="1" max="1" width="25.3516" style="6" customWidth="1"/>
+    <col min="2" max="2" width="32.8516" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.6719" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.3516" style="6" customWidth="1"/>
+    <col min="6" max="6" width="15" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="6" customWidth="1"/>
+    <col min="8" max="256" width="14.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" t="s" s="26">
+      <c r="A1" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s" s="7">
         <v>10</v>
       </c>
-      <c r="B1" t="s" s="27">
-        <v>6</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="26">
+      <c r="E2" t="s" s="7">
         <v>11</v>
       </c>
-      <c r="B2" t="s" s="26">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" t="s" s="7">
         <v>12</v>
       </c>
-      <c r="C2" t="s" s="26">
+      <c r="B3" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="D2" t="s" s="26">
+      <c r="C3" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="E2" t="s" s="26">
+      <c r="D3" t="s" s="7">
         <v>15</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" t="s" s="26">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" t="s" s="7">
         <v>16</v>
       </c>
-      <c r="B3" t="s" s="26">
+      <c r="B4" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="C3" t="s" s="26">
+      <c r="B5" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="10">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s" s="10">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s" s="10">
         <v>18</v>
       </c>
-      <c r="D3" t="s" s="26">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" t="s" s="10">
         <v>19</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" t="s" s="26">
+      <c r="B6" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s" s="10">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s" s="10">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s" s="10">
         <v>20</v>
       </c>
-      <c r="B4" t="s" s="26">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s" s="26">
-        <v>18</v>
-      </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" t="s" s="26">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" t="s" s="10">
         <v>21</v>
       </c>
-      <c r="B5" t="s" s="26">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s" s="26">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s" s="26">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s" s="26">
+      <c r="B7" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s" s="10">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s" s="10">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s" s="10">
         <v>22</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" t="s" s="26">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" t="s" s="11">
         <v>23</v>
       </c>
-      <c r="B6" t="s" s="26">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s" s="26">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s" s="26">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s" s="26">
+      <c r="B8" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s" s="11">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s" s="11">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s" s="11">
         <v>24</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" t="s" s="26">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" t="s" s="12">
         <v>25</v>
       </c>
-      <c r="B7" t="s" s="26">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s" s="26">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s" s="26">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s" s="26">
+      <c r="B9" t="s" s="12">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s" s="12">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s" s="12">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s" s="12">
         <v>26</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" t="s" s="26">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s" s="26">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s" s="26">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s" s="26">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s" s="26">
-        <v>28</v>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" t="s" s="26">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s" s="26">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s" s="26">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s" s="26">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s" s="26">
-        <v>30</v>
-      </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2071,480 +1980,380 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.3516" style="29" customWidth="1"/>
-    <col min="2" max="2" width="19" style="29" customWidth="1"/>
-    <col min="3" max="3" width="19.3516" style="29" customWidth="1"/>
-    <col min="4" max="4" width="77.8516" style="29" customWidth="1"/>
-    <col min="5" max="5" width="21.3516" style="29" customWidth="1"/>
-    <col min="6" max="6" width="11.3516" style="29" customWidth="1"/>
-    <col min="7" max="256" width="14.5" style="29" customWidth="1"/>
+    <col min="1" max="1" width="19.3516" style="15" customWidth="1"/>
+    <col min="2" max="2" width="19" style="15" customWidth="1"/>
+    <col min="3" max="3" width="19.3516" style="15" customWidth="1"/>
+    <col min="4" max="4" width="83.8516" style="15" customWidth="1"/>
+    <col min="5" max="5" width="21.3516" style="15" customWidth="1"/>
+    <col min="6" max="6" width="11.3516" style="15" customWidth="1"/>
+    <col min="7" max="256" width="14.5" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" t="s" s="26">
+      <c r="A1" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="B1" t="s" s="26">
+      <c r="E1" t="s" s="7">
         <v>32</v>
       </c>
-      <c r="C1" t="s" s="26">
+      <c r="F1" t="s" s="7">
         <v>33</v>
       </c>
-      <c r="D1" t="s" s="26">
+    </row>
+    <row r="2" ht="12.75" customHeight="1">
+      <c r="A2" t="s" s="7">
         <v>34</v>
       </c>
-      <c r="E1" t="s" s="26">
+      <c r="B2" t="s" s="7">
         <v>35</v>
       </c>
-      <c r="F1" t="s" s="26">
+      <c r="C2" t="s" s="7">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s" s="26">
+      <c r="D2" t="s" s="7">
         <v>37</v>
       </c>
-      <c r="B2" t="s" s="26">
-        <v>38</v>
-      </c>
-      <c r="C2" t="s" s="26">
+      <c r="E2" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s" s="7">
         <v>39</v>
       </c>
-      <c r="D2" t="s" s="26">
+    </row>
+    <row r="3" ht="12.75" customHeight="1">
+      <c r="A3" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s" s="7">
         <v>40</v>
       </c>
-      <c r="E2" t="s" s="26">
+      <c r="C3" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s" s="7">
         <v>41</v>
       </c>
-      <c r="F2" t="s" s="26">
+      <c r="E3" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s" s="7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1">
+      <c r="A4" t="s" s="7">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" t="s" s="26">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s" s="26">
+      <c r="B4" t="s" s="7">
         <v>43</v>
       </c>
-      <c r="C3" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s" s="26">
+      <c r="C4" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E3" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="F3" t="s" s="26">
+      <c r="E4" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s" s="7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1">
+      <c r="A5" t="s" s="7">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" t="s" s="26">
+      <c r="B5" t="s" s="16">
         <v>45</v>
       </c>
-      <c r="B4" t="s" s="26">
+      <c r="C5" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s" s="16">
         <v>46</v>
       </c>
-      <c r="C4" t="s" s="26">
+      <c r="E5" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s" s="17">
         <v>39</v>
       </c>
-      <c r="D4" t="s" s="30">
+    </row>
+    <row r="6" ht="12.75" customHeight="1">
+      <c r="A6" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s" s="16">
         <v>47</v>
       </c>
-      <c r="E4" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s" s="26">
+      <c r="C6" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s" s="16">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s" s="18">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1">
+      <c r="A7" t="s" s="7">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s" s="30">
-        <v>48</v>
-      </c>
-      <c r="C5" t="s" s="26">
+      <c r="B7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s" s="20">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s" s="18">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s" s="19">
         <v>39</v>
       </c>
-      <c r="D5" t="s" s="30">
-        <v>49</v>
-      </c>
-      <c r="E5" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s" s="31">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="B6" t="s" s="30">
-        <v>50</v>
-      </c>
-      <c r="C6" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s" s="30">
+    </row>
+    <row r="8" ht="12.75" customHeight="1">
+      <c r="A8" t="s" s="10">
         <v>51</v>
       </c>
-      <c r="E6" t="s" s="32">
-        <v>41</v>
-      </c>
-      <c r="F6" t="s" s="33">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="B7" t="s" s="30">
+      <c r="B8" t="s" s="21">
         <v>52</v>
       </c>
-      <c r="C7" t="s" s="26">
+      <c r="C8" t="s" s="22">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s" s="23">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s" s="24">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s" s="19">
         <v>39</v>
       </c>
-      <c r="D7" t="s" s="30">
-        <v>53</v>
-      </c>
-      <c r="E7" t="s" s="32">
-        <v>41</v>
-      </c>
-      <c r="F7" t="s" s="33">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" t="s" s="26">
+    </row>
+    <row r="9" ht="12.75" customHeight="1">
+      <c r="A9" t="s" s="22">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s" s="23">
         <v>54</v>
       </c>
-      <c r="B8" t="s" s="26">
+      <c r="C9" t="s" s="25">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s" s="23">
         <v>55</v>
       </c>
-      <c r="C8" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D8" t="s" s="34">
+      <c r="E9" t="s" s="24">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" ht="12.75" customHeight="1">
+      <c r="A10" t="s" s="10">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s" s="26">
         <v>56</v>
       </c>
-      <c r="E8" t="s" s="32">
-        <v>41</v>
-      </c>
-      <c r="F8" t="s" s="33">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" t="s" s="26">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s" s="34">
+      <c r="C10" t="s" s="10">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s" s="26">
         <v>57</v>
       </c>
-      <c r="C9" t="s" s="26">
+      <c r="E10" t="s" s="18">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s" s="19">
         <v>39</v>
       </c>
-      <c r="D9" t="s" s="34">
+    </row>
+    <row r="11" ht="12.75" customHeight="1">
+      <c r="A11" t="s" s="22">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s" s="23">
         <v>58</v>
       </c>
-      <c r="E9" t="s" s="32">
-        <v>41</v>
-      </c>
-      <c r="F9" t="s" s="33">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" t="s" s="26">
-        <v>54</v>
-      </c>
-      <c r="B10" t="s" s="26">
+      <c r="C11" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s" s="23">
         <v>59</v>
       </c>
-      <c r="C10" t="s" s="26">
+      <c r="E11" t="s" s="24">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s" s="19">
         <v>39</v>
       </c>
-      <c r="D10" t="s" s="26">
+    </row>
+    <row r="12" ht="12.75" customHeight="1">
+      <c r="A12" t="s" s="10">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s" s="27">
         <v>60</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
-    </row>
-    <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" t="s" s="26">
-        <v>54</v>
-      </c>
-      <c r="B11" t="s" s="34">
+      <c r="C12" t="s" s="10">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s" s="27">
         <v>61</v>
       </c>
-      <c r="C11" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s" s="34">
+      <c r="E12" t="s" s="18">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" ht="12.75" customHeight="1">
+      <c r="A13" t="s" s="10">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s" s="10">
         <v>62</v>
       </c>
-      <c r="E11" t="s" s="32">
-        <v>41</v>
-      </c>
-      <c r="F11" t="s" s="33">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" t="s" s="26">
-        <v>54</v>
-      </c>
-      <c r="B12" t="s" s="26">
+      <c r="C13" t="s" s="10">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s" s="10">
         <v>63</v>
       </c>
-      <c r="C12" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D12" t="s" s="26">
+      <c r="E13" t="s" s="18">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" ht="12.75" customHeight="1">
+      <c r="A14" t="s" s="10">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s" s="10">
         <v>64</v>
       </c>
-      <c r="E12" t="s" s="32">
-        <v>41</v>
-      </c>
-      <c r="F12" t="s" s="33">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" t="s" s="26">
-        <v>54</v>
-      </c>
-      <c r="B13" t="s" s="26">
+      <c r="C14" t="s" s="10">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s" s="10">
         <v>65</v>
       </c>
-      <c r="C13" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s" s="26">
+      <c r="E14" t="s" s="18">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" ht="12.75" customHeight="1">
+      <c r="A15" t="s" s="10">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s" s="10">
         <v>66</v>
       </c>
-      <c r="E13" t="s" s="32">
-        <v>41</v>
-      </c>
-      <c r="F13" t="s" s="33">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" t="s" s="26">
-        <v>54</v>
-      </c>
-      <c r="B14" t="s" s="26">
+      <c r="C15" t="s" s="10">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s" s="10">
         <v>67</v>
       </c>
-      <c r="C14" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s" s="26">
+      <c r="E15" t="s" s="18">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" ht="12.75" customHeight="1">
+      <c r="A16" t="s" s="10">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s" s="10">
         <v>68</v>
       </c>
-      <c r="E14" t="s" s="32">
-        <v>41</v>
-      </c>
-      <c r="F14" t="s" s="33">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" t="s" s="26">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s" s="26">
+      <c r="C16" t="s" s="10">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s" s="10">
         <v>69</v>
       </c>
-      <c r="C15" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s" s="26">
+      <c r="E16" t="s" s="18">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" t="s" s="28">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s" s="28">
         <v>70</v>
       </c>
-      <c r="E15" t="s" s="32">
-        <v>41</v>
-      </c>
-      <c r="F15" t="s" s="33">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" t="s" s="26">
-        <v>54</v>
-      </c>
-      <c r="B16" t="s" s="26">
+      <c r="C17" t="s" s="28">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s" s="28">
         <v>71</v>
       </c>
-      <c r="C16" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s" s="26">
+      <c r="E17" t="s" s="18">
+        <v>38</v>
+      </c>
+      <c r="F17" t="s" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" ht="12.75" customHeight="1">
+      <c r="A18" t="s" s="29">
         <v>72</v>
       </c>
-      <c r="E16" t="s" s="32">
-        <v>41</v>
-      </c>
-      <c r="F16" t="s" s="33">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" t="s" s="26">
-        <v>54</v>
-      </c>
-      <c r="B17" t="s" s="26">
+      <c r="B18" t="s" s="29">
         <v>73</v>
       </c>
-      <c r="C17" t="s" s="26">
+      <c r="C18" t="s" s="29">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s" s="29">
+        <v>74</v>
+      </c>
+      <c r="E18" t="s" s="30">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s" s="31">
         <v>39</v>
       </c>
-      <c r="D17" t="s" s="26">
-        <v>74</v>
-      </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="36"/>
-    </row>
-    <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" t="s" s="32">
-        <v>75</v>
-      </c>
-      <c r="B18" t="s" s="37">
-        <v>76</v>
-      </c>
-      <c r="C18" t="s" s="37">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s" s="37">
-        <v>77</v>
-      </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36"/>
-    </row>
-    <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-    </row>
-    <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
-    </row>
-    <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="36"/>
-    </row>
-    <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="36"/>
-    </row>
-    <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
-    </row>
-    <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
-    </row>
-    <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
-    </row>
-    <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
-    </row>
-    <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
-    </row>
-    <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="36"/>
-    </row>
-    <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="36"/>
-    </row>
-    <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
-    </row>
-    <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Added Test Cases for Modem Configuration Page
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -96,6 +96,12 @@
     <t>nickname=Hendrix</t>
   </si>
   <si>
+    <t>verifyShowMeHowToConnect</t>
+  </si>
+  <si>
+    <t>nickname=Pillows</t>
+  </si>
+  <si>
     <t>Locators</t>
   </si>
   <si>
@@ -238,6 +244,27 @@
   </si>
   <si>
     <t>ph.com.globe.mybusiness:id/btn_already_connected</t>
+  </si>
+  <si>
+    <t>showMeHowToConnBtn</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/btn_show_me</t>
+  </si>
+  <si>
+    <t>btnNextSTep1</t>
+  </si>
+  <si>
+    <t>//android.widget.Button[@text=‘NEXT STEP’]</t>
+  </si>
+  <si>
+    <t>btnNextSTep2</t>
+  </si>
+  <si>
+    <t>btnConnectNow</t>
+  </si>
+  <si>
+    <t>//android.widget.Button[@text=‘CONNECT NOW’]</t>
   </si>
 </sst>
 </file>
@@ -310,7 +337,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -372,21 +399,6 @@
       </right>
       <top style="thin">
         <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="12"/>
@@ -514,6 +526,51 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="12"/>
@@ -530,7 +587,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -573,39 +630,39 @@
     <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -618,13 +675,28 @@
     <xf numFmtId="49" fontId="6" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1755,7 +1827,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1766,7 +1838,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1958,12 +2030,22 @@
       <c r="G9" s="9"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="9"/>
+      <c r="A10" t="s" s="12">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s" s="12">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s" s="12">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s" s="12">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s" s="12">
+        <v>28</v>
+      </c>
+      <c r="F10" s="13"/>
       <c r="G10" s="9"/>
     </row>
   </sheetData>
@@ -1980,380 +2062,476 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.3516" style="15" customWidth="1"/>
-    <col min="2" max="2" width="19" style="15" customWidth="1"/>
-    <col min="3" max="3" width="19.3516" style="15" customWidth="1"/>
-    <col min="4" max="4" width="83.8516" style="15" customWidth="1"/>
-    <col min="5" max="5" width="21.3516" style="15" customWidth="1"/>
-    <col min="6" max="6" width="11.3516" style="15" customWidth="1"/>
-    <col min="7" max="256" width="14.5" style="15" customWidth="1"/>
+    <col min="1" max="1" width="19.3516" style="14" customWidth="1"/>
+    <col min="2" max="2" width="19" style="14" customWidth="1"/>
+    <col min="3" max="3" width="19.3516" style="14" customWidth="1"/>
+    <col min="4" max="4" width="83.8516" style="14" customWidth="1"/>
+    <col min="5" max="5" width="21.3516" style="14" customWidth="1"/>
+    <col min="6" max="6" width="11.3516" style="14" customWidth="1"/>
+    <col min="7" max="256" width="14.5" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" t="s" s="7">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s" s="7">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s" s="7">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s" s="7">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s" s="7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" t="s" s="7">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s" s="7">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s" s="7">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s" s="7">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" t="s" s="7">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s" s="7">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s" s="7">
         <v>41</v>
-      </c>
-      <c r="E3" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s" s="7">
-        <v>39</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" t="s" s="7">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s" s="7">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s" s="16">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="D4" t="s" s="15">
+        <v>46</v>
       </c>
       <c r="E4" t="s" s="7">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s" s="7">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s" s="16">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="B5" t="s" s="15">
+        <v>47</v>
       </c>
       <c r="C5" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s" s="16">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="D5" t="s" s="15">
+        <v>48</v>
       </c>
       <c r="E5" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s" s="17">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="F5" t="s" s="16">
+        <v>41</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s" s="16">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="B6" t="s" s="15">
+        <v>49</v>
       </c>
       <c r="C6" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s" s="16">
-        <v>48</v>
-      </c>
-      <c r="E6" t="s" s="18">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s" s="19">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="D6" t="s" s="15">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s" s="17">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s" s="18">
+        <v>41</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s" s="16">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="B7" t="s" s="15">
+        <v>51</v>
       </c>
       <c r="C7" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s" s="20">
-        <v>50</v>
-      </c>
-      <c r="E7" t="s" s="18">
         <v>38</v>
       </c>
-      <c r="F7" t="s" s="19">
-        <v>39</v>
+      <c r="D7" t="s" s="19">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s" s="17">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s" s="18">
+        <v>41</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" t="s" s="10">
-        <v>51</v>
-      </c>
-      <c r="B8" t="s" s="21">
-        <v>52</v>
-      </c>
-      <c r="C8" t="s" s="22">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s" s="20">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s" s="21">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s" s="22">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s" s="23">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s" s="18">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="1">
+      <c r="A9" t="s" s="21">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s" s="22">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s" s="24">
         <v>38</v>
       </c>
-      <c r="D8" t="s" s="23">
-        <v>53</v>
-      </c>
-      <c r="E8" t="s" s="24">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s" s="19">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" t="s" s="22">
-        <v>51</v>
-      </c>
-      <c r="B9" t="s" s="23">
-        <v>54</v>
-      </c>
-      <c r="C9" t="s" s="25">
-        <v>36</v>
-      </c>
-      <c r="D9" t="s" s="23">
-        <v>55</v>
-      </c>
-      <c r="E9" t="s" s="24">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s" s="19">
-        <v>39</v>
+      <c r="D9" t="s" s="22">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s" s="23">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s" s="18">
+        <v>41</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" t="s" s="10">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s" s="26">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="B10" t="s" s="25">
+        <v>58</v>
       </c>
       <c r="C10" t="s" s="10">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s" s="26">
-        <v>57</v>
-      </c>
-      <c r="E10" t="s" s="18">
         <v>38</v>
       </c>
-      <c r="F10" t="s" s="19">
-        <v>39</v>
+      <c r="D10" t="s" s="25">
+        <v>59</v>
+      </c>
+      <c r="E10" t="s" s="17">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s" s="18">
+        <v>41</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" t="s" s="22">
-        <v>51</v>
-      </c>
-      <c r="B11" t="s" s="23">
-        <v>58</v>
-      </c>
-      <c r="C11" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s" s="23">
-        <v>59</v>
-      </c>
-      <c r="E11" t="s" s="24">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s" s="19">
-        <v>39</v>
+      <c r="A11" t="s" s="21">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s" s="22">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s" s="24">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s" s="22">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s" s="23">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s" s="18">
+        <v>41</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" t="s" s="10">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s" s="27">
-        <v>60</v>
+        <v>53</v>
+      </c>
+      <c r="B12" t="s" s="26">
+        <v>62</v>
       </c>
       <c r="C12" t="s" s="10">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s" s="27">
-        <v>61</v>
-      </c>
-      <c r="E12" t="s" s="18">
-        <v>38</v>
-      </c>
-      <c r="F12" t="s" s="19">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="D12" t="s" s="26">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s" s="17">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s" s="18">
+        <v>41</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" t="s" s="10">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s" s="10">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s" s="10">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s" s="10">
-        <v>63</v>
-      </c>
-      <c r="E13" t="s" s="18">
-        <v>38</v>
-      </c>
-      <c r="F13" t="s" s="19">
-        <v>39</v>
+        <v>65</v>
+      </c>
+      <c r="E13" t="s" s="17">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s" s="18">
+        <v>41</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" t="s" s="10">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s" s="10">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s" s="10">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s" s="10">
-        <v>65</v>
-      </c>
-      <c r="E14" t="s" s="18">
-        <v>38</v>
-      </c>
-      <c r="F14" t="s" s="19">
-        <v>39</v>
+        <v>67</v>
+      </c>
+      <c r="E14" t="s" s="17">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s" s="18">
+        <v>41</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" t="s" s="10">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s" s="10">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s" s="10">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s" s="10">
-        <v>67</v>
-      </c>
-      <c r="E15" t="s" s="18">
-        <v>38</v>
-      </c>
-      <c r="F15" t="s" s="19">
-        <v>39</v>
+        <v>69</v>
+      </c>
+      <c r="E15" t="s" s="17">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s" s="18">
+        <v>41</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" t="s" s="10">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s" s="10">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s" s="10">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s" s="10">
+        <v>71</v>
+      </c>
+      <c r="E16" t="s" s="17">
+        <v>40</v>
+      </c>
+      <c r="F16" t="s" s="18">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" t="s" s="27">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s" s="27">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s" s="27">
         <v>38</v>
       </c>
-      <c r="D16" t="s" s="10">
-        <v>69</v>
-      </c>
-      <c r="E16" t="s" s="18">
+      <c r="D17" t="s" s="27">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s" s="17">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s" s="18">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" ht="12.75" customHeight="1">
+      <c r="A18" t="s" s="28">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s" s="28">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s" s="28">
         <v>38</v>
       </c>
-      <c r="F16" t="s" s="19">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" t="s" s="28">
-        <v>51</v>
-      </c>
-      <c r="B17" t="s" s="28">
-        <v>70</v>
-      </c>
-      <c r="C17" t="s" s="28">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s" s="28">
-        <v>71</v>
-      </c>
-      <c r="E17" t="s" s="18">
+      <c r="D18" t="s" s="28">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s" s="29">
+        <v>40</v>
+      </c>
+      <c r="F18" t="s" s="18">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" ht="12.75" customHeight="1">
+      <c r="A19" t="s" s="28">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s" s="28">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s" s="28">
         <v>38</v>
       </c>
-      <c r="F17" t="s" s="19">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" t="s" s="29">
-        <v>72</v>
-      </c>
-      <c r="B18" t="s" s="29">
-        <v>73</v>
-      </c>
-      <c r="C18" t="s" s="29">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s" s="29">
+      <c r="D19" t="s" s="28">
+        <v>78</v>
+      </c>
+      <c r="E19" s="30"/>
+      <c r="F19" s="31"/>
+    </row>
+    <row r="20" ht="12.75" customHeight="1">
+      <c r="A20" t="s" s="28">
         <v>74</v>
       </c>
-      <c r="E18" t="s" s="30">
-        <v>38</v>
-      </c>
-      <c r="F18" t="s" s="31">
-        <v>39</v>
-      </c>
+      <c r="B20" t="s" s="28">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s" s="32">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s" s="28">
+        <v>80</v>
+      </c>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
+    </row>
+    <row r="21" ht="12.75" customHeight="1">
+      <c r="A21" t="s" s="28">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s" s="28">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s" s="33">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s" s="28">
+        <v>80</v>
+      </c>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
+    </row>
+    <row r="22" ht="12.75" customHeight="1">
+      <c r="A22" t="s" s="28">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s" s="28">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s" s="34">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
+    </row>
+    <row r="23" ht="12.75" customHeight="1">
+      <c r="A23" s="35"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
+    </row>
+    <row r="24" ht="12.75" customHeight="1">
+      <c r="A24" s="35"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
+    </row>
+    <row r="25" ht="12.75" customHeight="1">
+      <c r="A25" s="35"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31"/>
+    </row>
+    <row r="26" ht="12.75" customHeight="1">
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Completed test case verifyShowMeHowToConnect
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -280,13 +280,16 @@
     <t>btnNextStep1</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t>ph.com.globe.mybusiness:id/btn_next</t>
   </si>
   <si>
     <t>Get Timing</t>
+  </si>
+  <si>
+    <t>btnNextStep2</t>
+  </si>
+  <si>
+    <t>btnConnectNow</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -377,7 +380,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -387,11 +390,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -400,7 +403,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -408,17 +411,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
@@ -435,7 +438,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom/>
@@ -443,12 +446,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -457,45 +471,34 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="16"/>
@@ -522,39 +525,39 @@
         <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -562,19 +565,19 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom/>
@@ -582,26 +585,26 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -629,10 +632,23 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,46 +663,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -698,7 +675,7 @@
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -711,7 +688,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -733,28 +710,28 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -772,20 +749,20 @@
     <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -871,19 +848,13 @@
     <xf numFmtId="49" fontId="6" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -906,8 +877,8 @@
       <rgbColor rgb="015e88b1"/>
       <rgbColor rgb="01eef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff9a9a9a"/>
@@ -1975,7 +1946,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2093,16 +2064,19 @@
       <c r="D12" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="E12" s="24"/>
-    </row>
-    <row r="13">
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" ht="13" customHeight="1">
+      <c r="A13" s="7"/>
       <c r="B13" t="s" s="3">
         <v>8</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14">
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" ht="13" customHeight="1">
+      <c r="A14" s="20"/>
       <c r="B14" s="4"/>
       <c r="C14" t="s" s="4">
         <v>5</v>
@@ -2110,6 +2084,7 @@
       <c r="D14" t="s" s="5">
         <v>8</v>
       </c>
+      <c r="E14" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2119,7 +2094,8 @@
   <hyperlinks>
     <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
-    <hyperlink ref="D12" location="'Locators'!R1C1" tooltip="" display="Locators"/>
+    <hyperlink ref="D12" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
+    <hyperlink ref="D14" location="'Locators'!R1C1" tooltip="" display="Locators"/>
     <hyperlink ref="D12" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
     <hyperlink ref="D14" location="'Locators'!R1C1" tooltip="" display="Locators"/>
   </hyperlinks>
@@ -2739,64 +2715,84 @@
       <c r="B20" t="s" s="47">
         <v>82</v>
       </c>
-      <c r="C20" t="s" s="51">
+      <c r="C20" t="s" s="47">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s" s="51">
         <v>83</v>
       </c>
-      <c r="D20" t="s" s="52">
+      <c r="E20" t="s" s="42">
         <v>84</v>
       </c>
-      <c r="E20" t="s" s="42">
+      <c r="F20" s="50"/>
+    </row>
+    <row r="21" ht="12.75" customHeight="1">
+      <c r="A21" t="s" s="47">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s" s="47">
         <v>85</v>
       </c>
-      <c r="F20" s="50"/>
-    </row>
-    <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="47"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="49"/>
+      <c r="C21" t="s" s="47">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s" s="51">
+        <v>83</v>
+      </c>
+      <c r="E21" t="s" s="42">
+        <v>84</v>
+      </c>
       <c r="F21" s="50"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="47"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="49"/>
+      <c r="A22" t="s" s="47">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s" s="47">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s" s="52">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s" s="51">
+        <v>83</v>
+      </c>
+      <c r="E22" t="s" s="42">
+        <v>84</v>
+      </c>
       <c r="F22" s="50"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="56"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
+      <c r="A23" s="53"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="53"/>
       <c r="E23" s="49"/>
       <c r="F23" s="50"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="56"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
+      <c r="A24" s="53"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
       <c r="E24" s="49"/>
       <c r="F24" s="50"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="56"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
+      <c r="A25" s="53"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="49"/>
       <c r="F25" s="50"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="56"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
+      <c r="A26" s="53"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
       <c r="E26" s="49"/>
-      <c r="F26" s="57"/>
+      <c r="F26" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Added scripts for verifyUserAlreadyConnected test case
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -291,6 +291,18 @@
   <si>
     <t>btnConnectNow</t>
   </si>
+  <si>
+    <t>btnManuallyVerifyAccnt</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/btn_manual_verif</t>
+  </si>
+  <si>
+    <t>btnSkipForNow</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/sptxt_skip</t>
+  </si>
 </sst>
 </file>
 
@@ -299,7 +311,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -335,11 +347,6 @@
       <sz val="8"/>
       <color indexed="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="7">
@@ -688,7 +695,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -791,9 +798,6 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -803,34 +807,22 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -842,16 +834,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2109,7 +2101,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2302,6 +2294,96 @@
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="28"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="28"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="28"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="28"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="28"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="28"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="28"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="28"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="28"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2402,7 +2484,7 @@
       <c r="C4" t="s" s="26">
         <v>41</v>
       </c>
-      <c r="D4" t="s" s="34">
+      <c r="D4" t="s" s="26">
         <v>49</v>
       </c>
       <c r="E4" t="s" s="26">
@@ -2416,19 +2498,19 @@
       <c r="A5" t="s" s="26">
         <v>47</v>
       </c>
-      <c r="B5" t="s" s="34">
+      <c r="B5" t="s" s="26">
         <v>50</v>
       </c>
       <c r="C5" t="s" s="26">
         <v>41</v>
       </c>
-      <c r="D5" t="s" s="34">
+      <c r="D5" t="s" s="26">
         <v>51</v>
       </c>
       <c r="E5" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="F5" t="s" s="35">
+      <c r="F5" t="s" s="34">
         <v>44</v>
       </c>
     </row>
@@ -2436,19 +2518,19 @@
       <c r="A6" t="s" s="26">
         <v>47</v>
       </c>
-      <c r="B6" t="s" s="34">
+      <c r="B6" t="s" s="26">
         <v>52</v>
       </c>
       <c r="C6" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="D6" t="s" s="34">
+      <c r="D6" t="s" s="26">
         <v>53</v>
       </c>
-      <c r="E6" t="s" s="36">
+      <c r="E6" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="F6" t="s" s="37">
+      <c r="F6" t="s" s="36">
         <v>44</v>
       </c>
     </row>
@@ -2456,343 +2538,361 @@
       <c r="A7" t="s" s="26">
         <v>47</v>
       </c>
-      <c r="B7" t="s" s="34">
+      <c r="B7" t="s" s="26">
         <v>54</v>
       </c>
       <c r="C7" t="s" s="26">
         <v>41</v>
       </c>
-      <c r="D7" t="s" s="38">
+      <c r="D7" t="s" s="34">
         <v>55</v>
       </c>
-      <c r="E7" t="s" s="36">
+      <c r="E7" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="F7" t="s" s="37">
+      <c r="F7" t="s" s="36">
         <v>44</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" t="s" s="29">
+      <c r="A8" t="s" s="26">
         <v>56</v>
       </c>
-      <c r="B8" t="s" s="39">
+      <c r="B8" t="s" s="34">
         <v>57</v>
       </c>
-      <c r="C8" t="s" s="40">
+      <c r="C8" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="D8" t="s" s="41">
+      <c r="D8" t="s" s="37">
         <v>58</v>
       </c>
-      <c r="E8" t="s" s="42">
+      <c r="E8" t="s" s="38">
         <v>43</v>
       </c>
-      <c r="F8" t="s" s="37">
+      <c r="F8" t="s" s="36">
         <v>44</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" t="s" s="40">
+      <c r="A9" t="s" s="35">
         <v>56</v>
       </c>
-      <c r="B9" t="s" s="41">
+      <c r="B9" t="s" s="37">
         <v>59</v>
       </c>
-      <c r="C9" t="s" s="43">
+      <c r="C9" t="s" s="38">
         <v>41</v>
       </c>
-      <c r="D9" t="s" s="41">
+      <c r="D9" t="s" s="37">
         <v>60</v>
       </c>
-      <c r="E9" t="s" s="42">
+      <c r="E9" t="s" s="38">
         <v>43</v>
       </c>
-      <c r="F9" t="s" s="37">
+      <c r="F9" t="s" s="36">
         <v>44</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" t="s" s="29">
+      <c r="A10" t="s" s="26">
         <v>56</v>
       </c>
-      <c r="B10" t="s" s="44">
+      <c r="B10" t="s" s="39">
         <v>61</v>
       </c>
-      <c r="C10" t="s" s="29">
+      <c r="C10" t="s" s="26">
         <v>41</v>
       </c>
-      <c r="D10" t="s" s="44">
+      <c r="D10" t="s" s="39">
         <v>62</v>
       </c>
-      <c r="E10" t="s" s="36">
+      <c r="E10" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="F10" t="s" s="37">
+      <c r="F10" t="s" s="36">
         <v>44</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" t="s" s="40">
+      <c r="A11" t="s" s="35">
         <v>56</v>
       </c>
-      <c r="B11" t="s" s="41">
+      <c r="B11" t="s" s="37">
         <v>63</v>
       </c>
-      <c r="C11" t="s" s="43">
+      <c r="C11" t="s" s="38">
         <v>43</v>
       </c>
-      <c r="D11" t="s" s="41">
+      <c r="D11" t="s" s="37">
         <v>64</v>
       </c>
-      <c r="E11" t="s" s="42">
+      <c r="E11" t="s" s="38">
         <v>43</v>
       </c>
-      <c r="F11" t="s" s="37">
+      <c r="F11" t="s" s="36">
         <v>44</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" t="s" s="29">
+      <c r="A12" t="s" s="26">
         <v>56</v>
       </c>
-      <c r="B12" t="s" s="45">
+      <c r="B12" t="s" s="40">
         <v>65</v>
       </c>
-      <c r="C12" t="s" s="29">
+      <c r="C12" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="D12" t="s" s="45">
+      <c r="D12" t="s" s="40">
         <v>66</v>
       </c>
-      <c r="E12" t="s" s="36">
+      <c r="E12" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="F12" t="s" s="37">
+      <c r="F12" t="s" s="36">
         <v>44</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" t="s" s="29">
+      <c r="A13" t="s" s="26">
         <v>56</v>
       </c>
-      <c r="B13" t="s" s="29">
+      <c r="B13" t="s" s="26">
         <v>67</v>
       </c>
-      <c r="C13" t="s" s="29">
+      <c r="C13" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="D13" t="s" s="29">
+      <c r="D13" t="s" s="26">
         <v>68</v>
       </c>
-      <c r="E13" t="s" s="36">
+      <c r="E13" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="F13" t="s" s="37">
+      <c r="F13" t="s" s="36">
         <v>44</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" t="s" s="29">
+      <c r="A14" t="s" s="26">
         <v>56</v>
       </c>
-      <c r="B14" t="s" s="29">
+      <c r="B14" t="s" s="26">
         <v>69</v>
       </c>
-      <c r="C14" t="s" s="29">
+      <c r="C14" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="D14" t="s" s="29">
+      <c r="D14" t="s" s="26">
         <v>70</v>
       </c>
-      <c r="E14" t="s" s="36">
+      <c r="E14" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="F14" t="s" s="37">
+      <c r="F14" t="s" s="36">
         <v>44</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" t="s" s="29">
+      <c r="A15" t="s" s="26">
         <v>56</v>
       </c>
-      <c r="B15" t="s" s="29">
+      <c r="B15" t="s" s="26">
         <v>71</v>
       </c>
-      <c r="C15" t="s" s="29">
+      <c r="C15" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="D15" t="s" s="29">
+      <c r="D15" t="s" s="26">
         <v>72</v>
       </c>
-      <c r="E15" t="s" s="36">
+      <c r="E15" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="F15" t="s" s="37">
+      <c r="F15" t="s" s="36">
         <v>44</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" t="s" s="29">
+      <c r="A16" t="s" s="26">
         <v>56</v>
       </c>
-      <c r="B16" t="s" s="29">
+      <c r="B16" t="s" s="26">
         <v>73</v>
       </c>
-      <c r="C16" t="s" s="29">
+      <c r="C16" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="D16" t="s" s="29">
+      <c r="D16" t="s" s="26">
         <v>74</v>
       </c>
-      <c r="E16" t="s" s="36">
+      <c r="E16" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="F16" t="s" s="37">
+      <c r="F16" t="s" s="36">
         <v>44</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" t="s" s="46">
+      <c r="A17" t="s" s="41">
         <v>56</v>
       </c>
-      <c r="B17" t="s" s="46">
+      <c r="B17" t="s" s="41">
         <v>75</v>
       </c>
-      <c r="C17" t="s" s="46">
+      <c r="C17" t="s" s="41">
         <v>41</v>
       </c>
-      <c r="D17" t="s" s="46">
+      <c r="D17" t="s" s="41">
         <v>76</v>
       </c>
-      <c r="E17" t="s" s="36">
+      <c r="E17" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="F17" t="s" s="37">
+      <c r="F17" t="s" s="36">
         <v>44</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" t="s" s="47">
+      <c r="A18" t="s" s="42">
         <v>77</v>
       </c>
-      <c r="B18" t="s" s="47">
+      <c r="B18" t="s" s="42">
         <v>78</v>
       </c>
-      <c r="C18" t="s" s="47">
+      <c r="C18" t="s" s="42">
         <v>41</v>
       </c>
-      <c r="D18" t="s" s="47">
+      <c r="D18" t="s" s="42">
         <v>79</v>
       </c>
-      <c r="E18" t="s" s="48">
+      <c r="E18" t="s" s="43">
         <v>43</v>
       </c>
-      <c r="F18" t="s" s="37">
+      <c r="F18" t="s" s="36">
         <v>44</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" t="s" s="47">
+      <c r="A19" t="s" s="42">
         <v>77</v>
       </c>
-      <c r="B19" t="s" s="47">
+      <c r="B19" t="s" s="42">
         <v>80</v>
       </c>
-      <c r="C19" t="s" s="47">
+      <c r="C19" t="s" s="42">
         <v>41</v>
       </c>
-      <c r="D19" t="s" s="47">
+      <c r="D19" t="s" s="42">
         <v>81</v>
       </c>
-      <c r="E19" s="49"/>
-      <c r="F19" s="50"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="45"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" t="s" s="47">
+      <c r="A20" t="s" s="42">
         <v>77</v>
       </c>
-      <c r="B20" t="s" s="47">
+      <c r="B20" t="s" s="42">
         <v>82</v>
       </c>
-      <c r="C20" t="s" s="47">
+      <c r="C20" t="s" s="42">
         <v>41</v>
       </c>
-      <c r="D20" t="s" s="51">
+      <c r="D20" t="s" s="46">
         <v>83</v>
       </c>
-      <c r="E20" t="s" s="42">
+      <c r="E20" t="s" s="38">
         <v>84</v>
       </c>
-      <c r="F20" s="50"/>
+      <c r="F20" s="45"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" t="s" s="47">
+      <c r="A21" t="s" s="42">
         <v>77</v>
       </c>
-      <c r="B21" t="s" s="47">
+      <c r="B21" t="s" s="42">
         <v>85</v>
       </c>
-      <c r="C21" t="s" s="47">
+      <c r="C21" t="s" s="42">
         <v>41</v>
       </c>
-      <c r="D21" t="s" s="51">
+      <c r="D21" t="s" s="46">
         <v>83</v>
       </c>
-      <c r="E21" t="s" s="42">
+      <c r="E21" t="s" s="38">
         <v>84</v>
       </c>
-      <c r="F21" s="50"/>
+      <c r="F21" s="45"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" t="s" s="47">
+      <c r="A22" t="s" s="42">
         <v>77</v>
       </c>
-      <c r="B22" t="s" s="47">
+      <c r="B22" t="s" s="42">
         <v>86</v>
       </c>
-      <c r="C22" t="s" s="52">
+      <c r="C22" t="s" s="42">
         <v>41</v>
       </c>
-      <c r="D22" t="s" s="51">
+      <c r="D22" t="s" s="46">
         <v>83</v>
       </c>
-      <c r="E22" t="s" s="42">
+      <c r="E22" t="s" s="38">
         <v>84</v>
       </c>
-      <c r="F22" s="50"/>
+      <c r="F22" s="45"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="53"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="50"/>
+      <c r="A23" t="s" s="42">
+        <v>77</v>
+      </c>
+      <c r="B23" t="s" s="42">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s" s="42">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s" s="46">
+        <v>88</v>
+      </c>
+      <c r="E23" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="F23" s="45"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="53"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="50"/>
+      <c r="A24" t="s" s="42">
+        <v>77</v>
+      </c>
+      <c r="B24" t="s" s="42">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s" s="47">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s" s="42">
+        <v>90</v>
+      </c>
+      <c r="E24" s="44"/>
+      <c r="F24" s="45"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="53"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="50"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="45"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="53"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="55"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Added scripts for Home Page Test Suite
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="96">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -130,6 +130,12 @@
     <t>nickname=Pillows</t>
   </si>
   <si>
+    <t>verifyHomePage</t>
+  </si>
+  <si>
+    <t>nickname=Libertea</t>
+  </si>
+  <si>
     <t>Page</t>
   </si>
   <si>
@@ -302,6 +308,15 @@
   </si>
   <si>
     <t>ph.com.globe.mybusiness:id/sptxt_skip</t>
+  </si>
+  <si>
+    <t>HomePage</t>
+  </si>
+  <si>
+    <t>btnProceed</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/btn_positive</t>
   </si>
 </sst>
 </file>
@@ -387,7 +402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -549,10 +564,23 @@
       <right style="thin">
         <color indexed="13"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
       <top style="thin">
         <color indexed="13"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -569,6 +597,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -591,27 +632,40 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="13"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="8"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -689,13 +743,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -798,24 +916,33 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -828,26 +955,47 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2296,11 +2444,21 @@
       <c r="G10" s="28"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
+      <c r="A11" t="s" s="31">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s" s="31">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s" s="31">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s" s="31">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s" s="31">
+        <v>34</v>
+      </c>
       <c r="F11" s="32"/>
       <c r="G11" s="28"/>
     </row>
@@ -2399,7 +2557,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2415,484 +2573,564 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" t="s" s="26">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s" s="26">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s" s="26">
+      <c r="A1" t="s" s="34">
         <v>35</v>
       </c>
-      <c r="D1" t="s" s="26">
+      <c r="B1" t="s" s="35">
         <v>36</v>
       </c>
-      <c r="E1" t="s" s="26">
+      <c r="C1" t="s" s="35">
         <v>37</v>
       </c>
-      <c r="F1" t="s" s="26">
+      <c r="D1" t="s" s="35">
         <v>38</v>
       </c>
+      <c r="E1" t="s" s="35">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s" s="36">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s" s="26">
-        <v>39</v>
+      <c r="A2" t="s" s="37">
+        <v>41</v>
       </c>
       <c r="B2" t="s" s="26">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s" s="26">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s" s="26">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s" s="26">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s" s="38">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1">
+      <c r="A3" t="s" s="37">
         <v>41</v>
       </c>
-      <c r="D2" t="s" s="26">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s" s="26">
+      <c r="B3" t="s" s="26">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s" s="26">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s" s="26">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s" s="26">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s" s="38">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1">
+      <c r="A4" t="s" s="37">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s" s="26">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="F2" t="s" s="26">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" t="s" s="26">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s" s="26">
+      <c r="D4" t="s" s="26">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s" s="26">
         <v>45</v>
       </c>
-      <c r="C3" t="s" s="26">
+      <c r="F4" t="s" s="38">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1">
+      <c r="A5" t="s" s="37">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s" s="26">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="D3" t="s" s="26">
+      <c r="D5" t="s" s="26">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s" s="26">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s" s="39">
         <v>46</v>
       </c>
-      <c r="E3" t="s" s="26">
+    </row>
+    <row r="6" ht="12.75" customHeight="1">
+      <c r="A6" t="s" s="37">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s" s="26">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s" s="26">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s" s="26">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s" s="38">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1">
+      <c r="A7" t="s" s="37">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s" s="26">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="F3" t="s" s="26">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" t="s" s="26">
-        <v>47</v>
-      </c>
-      <c r="B4" t="s" s="26">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s" s="26">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s" s="26">
+      <c r="D7" t="s" s="41">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s" s="38">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="1">
+      <c r="A8" t="s" s="37">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s" s="41">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s" s="38">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s" s="42">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s" s="43">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="1">
+      <c r="A9" t="s" s="43">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s" s="42">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s" s="43">
         <v>43</v>
       </c>
-      <c r="F4" t="s" s="26">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" t="s" s="26">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s" s="26">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s" s="26">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s" s="26">
+      <c r="D9" t="s" s="42">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s" s="43">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" ht="12.75" customHeight="1">
+      <c r="A10" t="s" s="37">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s" s="44">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="F5" t="s" s="34">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" t="s" s="26">
-        <v>47</v>
-      </c>
-      <c r="B6" t="s" s="26">
-        <v>52</v>
-      </c>
-      <c r="C6" t="s" s="26">
+      <c r="D10" t="s" s="44">
+        <v>64</v>
+      </c>
+      <c r="E10" t="s" s="38">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" ht="12.75" customHeight="1">
+      <c r="A11" t="s" s="43">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s" s="42">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s" s="43">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s" s="42">
+        <v>66</v>
+      </c>
+      <c r="E11" t="s" s="43">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" ht="12.75" customHeight="1">
+      <c r="A12" t="s" s="37">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s" s="35">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s" s="26">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s" s="35">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s" s="38">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" ht="12.75" customHeight="1">
+      <c r="A13" t="s" s="37">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s" s="26">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s" s="26">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s" s="26">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s" s="38">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" ht="12.75" customHeight="1">
+      <c r="A14" t="s" s="37">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s" s="26">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s" s="26">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s" s="26">
+        <v>72</v>
+      </c>
+      <c r="E14" t="s" s="38">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" ht="12.75" customHeight="1">
+      <c r="A15" t="s" s="37">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s" s="26">
+        <v>73</v>
+      </c>
+      <c r="C15" t="s" s="26">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s" s="26">
+        <v>74</v>
+      </c>
+      <c r="E15" t="s" s="38">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" ht="12.75" customHeight="1">
+      <c r="A16" t="s" s="37">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s" s="26">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s" s="26">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="E16" t="s" s="38">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" t="s" s="45">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s" s="46">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s" s="46">
         <v>43</v>
       </c>
-      <c r="D6" t="s" s="26">
-        <v>53</v>
-      </c>
-      <c r="E6" t="s" s="35">
+      <c r="D17" t="s" s="46">
+        <v>78</v>
+      </c>
+      <c r="E17" t="s" s="38">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" ht="12.75" customHeight="1">
+      <c r="A18" t="s" s="47">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s" s="48">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s" s="48">
         <v>43</v>
       </c>
-      <c r="F6" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" t="s" s="26">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s" s="26">
-        <v>54</v>
-      </c>
-      <c r="C7" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s" s="34">
-        <v>55</v>
-      </c>
-      <c r="E7" t="s" s="35">
+      <c r="D18" t="s" s="48">
+        <v>81</v>
+      </c>
+      <c r="E18" t="s" s="49">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s" s="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" ht="12.75" customHeight="1">
+      <c r="A19" t="s" s="47">
+        <v>79</v>
+      </c>
+      <c r="B19" t="s" s="48">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s" s="48">
         <v>43</v>
       </c>
-      <c r="F7" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" t="s" s="26">
-        <v>56</v>
-      </c>
-      <c r="B8" t="s" s="34">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s" s="35">
+      <c r="D19" t="s" s="48">
+        <v>83</v>
+      </c>
+      <c r="E19" s="50"/>
+      <c r="F19" s="51"/>
+    </row>
+    <row r="20" ht="12.75" customHeight="1">
+      <c r="A20" t="s" s="47">
+        <v>79</v>
+      </c>
+      <c r="B20" t="s" s="48">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s" s="48">
         <v>43</v>
       </c>
-      <c r="D8" t="s" s="37">
-        <v>58</v>
-      </c>
-      <c r="E8" t="s" s="38">
+      <c r="D20" t="s" s="52">
+        <v>85</v>
+      </c>
+      <c r="E20" t="s" s="43">
+        <v>86</v>
+      </c>
+      <c r="F20" s="51"/>
+    </row>
+    <row r="21" ht="12.75" customHeight="1">
+      <c r="A21" t="s" s="47">
+        <v>79</v>
+      </c>
+      <c r="B21" t="s" s="48">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s" s="48">
         <v>43</v>
       </c>
-      <c r="F8" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" t="s" s="35">
-        <v>56</v>
-      </c>
-      <c r="B9" t="s" s="37">
-        <v>59</v>
-      </c>
-      <c r="C9" t="s" s="38">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s" s="37">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s" s="38">
+      <c r="D21" t="s" s="52">
+        <v>85</v>
+      </c>
+      <c r="E21" t="s" s="43">
+        <v>86</v>
+      </c>
+      <c r="F21" s="51"/>
+    </row>
+    <row r="22" ht="12.75" customHeight="1">
+      <c r="A22" t="s" s="47">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s" s="48">
+        <v>88</v>
+      </c>
+      <c r="C22" t="s" s="48">
         <v>43</v>
       </c>
-      <c r="F9" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" t="s" s="26">
-        <v>56</v>
-      </c>
-      <c r="B10" t="s" s="39">
-        <v>61</v>
-      </c>
-      <c r="C10" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s" s="39">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s" s="35">
+      <c r="D22" t="s" s="52">
+        <v>85</v>
+      </c>
+      <c r="E22" t="s" s="43">
+        <v>86</v>
+      </c>
+      <c r="F22" s="51"/>
+    </row>
+    <row r="23" ht="12.75" customHeight="1">
+      <c r="A23" t="s" s="47">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s" s="48">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s" s="48">
         <v>43</v>
       </c>
-      <c r="F10" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" t="s" s="35">
-        <v>56</v>
-      </c>
-      <c r="B11" t="s" s="37">
-        <v>63</v>
-      </c>
-      <c r="C11" t="s" s="38">
+      <c r="D23" t="s" s="52">
+        <v>90</v>
+      </c>
+      <c r="E23" t="s" s="43">
+        <v>86</v>
+      </c>
+      <c r="F23" s="51"/>
+    </row>
+    <row r="24" ht="12.75" customHeight="1">
+      <c r="A24" t="s" s="47">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s" s="48">
+        <v>91</v>
+      </c>
+      <c r="C24" t="s" s="53">
         <v>43</v>
       </c>
-      <c r="D11" t="s" s="37">
-        <v>64</v>
-      </c>
-      <c r="E11" t="s" s="38">
+      <c r="D24" t="s" s="48">
+        <v>92</v>
+      </c>
+      <c r="E24" s="50"/>
+      <c r="F24" s="51"/>
+    </row>
+    <row r="25" ht="12.75" customHeight="1">
+      <c r="A25" t="s" s="47">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s" s="48">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s" s="54">
         <v>43</v>
       </c>
-      <c r="F11" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" t="s" s="26">
-        <v>56</v>
-      </c>
-      <c r="B12" t="s" s="40">
-        <v>65</v>
-      </c>
-      <c r="C12" t="s" s="26">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s" s="40">
-        <v>66</v>
-      </c>
-      <c r="E12" t="s" s="35">
-        <v>43</v>
-      </c>
-      <c r="F12" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" t="s" s="26">
-        <v>56</v>
-      </c>
-      <c r="B13" t="s" s="26">
-        <v>67</v>
-      </c>
-      <c r="C13" t="s" s="26">
-        <v>43</v>
-      </c>
-      <c r="D13" t="s" s="26">
-        <v>68</v>
-      </c>
-      <c r="E13" t="s" s="35">
-        <v>43</v>
-      </c>
-      <c r="F13" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" t="s" s="26">
-        <v>56</v>
-      </c>
-      <c r="B14" t="s" s="26">
-        <v>69</v>
-      </c>
-      <c r="C14" t="s" s="26">
-        <v>43</v>
-      </c>
-      <c r="D14" t="s" s="26">
-        <v>70</v>
-      </c>
-      <c r="E14" t="s" s="35">
-        <v>43</v>
-      </c>
-      <c r="F14" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" t="s" s="26">
-        <v>56</v>
-      </c>
-      <c r="B15" t="s" s="26">
-        <v>71</v>
-      </c>
-      <c r="C15" t="s" s="26">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s" s="26">
-        <v>72</v>
-      </c>
-      <c r="E15" t="s" s="35">
-        <v>43</v>
-      </c>
-      <c r="F15" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" t="s" s="26">
-        <v>56</v>
-      </c>
-      <c r="B16" t="s" s="26">
-        <v>73</v>
-      </c>
-      <c r="C16" t="s" s="26">
-        <v>43</v>
-      </c>
-      <c r="D16" t="s" s="26">
-        <v>74</v>
-      </c>
-      <c r="E16" t="s" s="35">
-        <v>43</v>
-      </c>
-      <c r="F16" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" t="s" s="41">
-        <v>56</v>
-      </c>
-      <c r="B17" t="s" s="41">
-        <v>75</v>
-      </c>
-      <c r="C17" t="s" s="41">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s" s="41">
-        <v>76</v>
-      </c>
-      <c r="E17" t="s" s="35">
-        <v>43</v>
-      </c>
-      <c r="F17" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" t="s" s="42">
-        <v>77</v>
-      </c>
-      <c r="B18" t="s" s="42">
-        <v>78</v>
-      </c>
-      <c r="C18" t="s" s="42">
-        <v>41</v>
-      </c>
-      <c r="D18" t="s" s="42">
-        <v>79</v>
-      </c>
-      <c r="E18" t="s" s="43">
-        <v>43</v>
-      </c>
-      <c r="F18" t="s" s="36">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" t="s" s="42">
-        <v>77</v>
-      </c>
-      <c r="B19" t="s" s="42">
-        <v>80</v>
-      </c>
-      <c r="C19" t="s" s="42">
-        <v>41</v>
-      </c>
-      <c r="D19" t="s" s="42">
-        <v>81</v>
-      </c>
-      <c r="E19" s="44"/>
-      <c r="F19" s="45"/>
-    </row>
-    <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" t="s" s="42">
-        <v>77</v>
-      </c>
-      <c r="B20" t="s" s="42">
-        <v>82</v>
-      </c>
-      <c r="C20" t="s" s="42">
-        <v>41</v>
-      </c>
-      <c r="D20" t="s" s="46">
-        <v>83</v>
-      </c>
-      <c r="E20" t="s" s="38">
-        <v>84</v>
-      </c>
-      <c r="F20" s="45"/>
-    </row>
-    <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" t="s" s="42">
-        <v>77</v>
-      </c>
-      <c r="B21" t="s" s="42">
-        <v>85</v>
-      </c>
-      <c r="C21" t="s" s="42">
-        <v>41</v>
-      </c>
-      <c r="D21" t="s" s="46">
-        <v>83</v>
-      </c>
-      <c r="E21" t="s" s="38">
-        <v>84</v>
-      </c>
-      <c r="F21" s="45"/>
-    </row>
-    <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" t="s" s="42">
-        <v>77</v>
-      </c>
-      <c r="B22" t="s" s="42">
-        <v>86</v>
-      </c>
-      <c r="C22" t="s" s="42">
-        <v>41</v>
-      </c>
-      <c r="D22" t="s" s="46">
-        <v>83</v>
-      </c>
-      <c r="E22" t="s" s="38">
-        <v>84</v>
-      </c>
-      <c r="F22" s="45"/>
-    </row>
-    <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" t="s" s="42">
-        <v>77</v>
-      </c>
-      <c r="B23" t="s" s="42">
-        <v>87</v>
-      </c>
-      <c r="C23" t="s" s="42">
-        <v>41</v>
-      </c>
-      <c r="D23" t="s" s="46">
-        <v>88</v>
-      </c>
-      <c r="E23" t="s" s="38">
-        <v>84</v>
-      </c>
-      <c r="F23" s="45"/>
-    </row>
-    <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" t="s" s="42">
-        <v>77</v>
-      </c>
-      <c r="B24" t="s" s="42">
-        <v>89</v>
-      </c>
-      <c r="C24" t="s" s="47">
-        <v>41</v>
-      </c>
-      <c r="D24" t="s" s="42">
-        <v>90</v>
-      </c>
-      <c r="E24" s="44"/>
-      <c r="F24" s="45"/>
-    </row>
-    <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="48"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="45"/>
+      <c r="D25" t="s" s="48">
+        <v>95</v>
+      </c>
+      <c r="E25" s="50"/>
+      <c r="F25" s="51"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="48"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="50"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="51"/>
+    </row>
+    <row r="27" ht="12.75" customHeight="1">
+      <c r="A27" s="58"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="51"/>
+    </row>
+    <row r="28" ht="12.75" customHeight="1">
+      <c r="A28" s="58"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="51"/>
+    </row>
+    <row r="29" ht="12.75" customHeight="1">
+      <c r="A29" s="58"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="51"/>
+    </row>
+    <row r="30" ht="12.75" customHeight="1">
+      <c r="A30" s="58"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="51"/>
+    </row>
+    <row r="31" ht="12.75" customHeight="1">
+      <c r="A31" s="58"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="51"/>
+    </row>
+    <row r="32" ht="12.75" customHeight="1">
+      <c r="A32" s="58"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="51"/>
+    </row>
+    <row r="33" ht="12.75" customHeight="1">
+      <c r="A33" s="58"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="51"/>
+    </row>
+    <row r="34" ht="12.75" customHeight="1">
+      <c r="A34" s="58"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="51"/>
+    </row>
+    <row r="35" ht="12.75" customHeight="1">
+      <c r="A35" s="58"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Refactored Secure App Page
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="120">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -27,20 +27,17 @@
     <t>Excel Worksheet Name</t>
   </si>
   <si>
-    <t>Export Summary</t>
+    <t>Testdata</t>
   </si>
   <si>
     <t>Table 1</t>
-  </si>
-  <si>
-    <t>Testdata</t>
   </si>
   <si>
     <r>
       <rPr>
         <u val="single"/>
         <sz val="12"/>
-        <color indexed="11"/>
+        <color indexed="13"/>
         <rFont val="Arial"/>
       </rPr>
       <t>Testdata</t>
@@ -54,7 +51,7 @@
       <rPr>
         <u val="single"/>
         <sz val="12"/>
-        <color indexed="11"/>
+        <color indexed="13"/>
         <rFont val="Arial"/>
       </rPr>
       <t>Locators</t>
@@ -79,15 +76,27 @@
     <t>text4=Get more data</t>
   </si>
   <si>
+    <t>verifySecureAppMatchingPin</t>
+  </si>
+  <si>
+    <t>mobileNumber=09271080510</t>
+  </si>
+  <si>
+    <t>pin=1111</t>
+  </si>
+  <si>
+    <t>verifySecureAppMismatchPin</t>
+  </si>
+  <si>
+    <t>pin2=1234</t>
+  </si>
+  <si>
+    <t>text1=App PIN did not match. Try again.</t>
+  </si>
+  <si>
     <t>customerProfileEnterNickname</t>
   </si>
   <si>
-    <t>mobileNumber=09271080510</t>
-  </si>
-  <si>
-    <t>pin=1111</t>
-  </si>
-  <si>
     <t>nickname=Lexter</t>
   </si>
   <si>
@@ -178,6 +187,75 @@
     <t>//*[@resource-id='ph.com.globe.mybusiness:id/btn_walkthrough_start']</t>
   </si>
   <si>
+    <t>SecureAppPage</t>
+  </si>
+  <si>
+    <t>txtSecureApp</t>
+  </si>
+  <si>
+    <t>//*[@text='Secure the app']</t>
+  </si>
+  <si>
+    <t>txtSecureAppConfirm</t>
+  </si>
+  <si>
+    <t>//*[@text='Re-enter 4-digit app PIN']</t>
+  </si>
+  <si>
+    <t>txtSecurePin</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/pet_pin</t>
+  </si>
+  <si>
+    <t>unmatchedSecurePin</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/sptxt_pin_error_spiel</t>
+  </si>
+  <si>
+    <t>btnNextSecurePage</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/pbtn_pin_submit</t>
+  </si>
+  <si>
+    <t>btnDelete</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/spbtn_pin_key_clear</t>
+  </si>
+  <si>
+    <t>btn1</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/spbtn_pin_key_1</t>
+  </si>
+  <si>
+    <t>btn2</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/spbtn_pin_key_2</t>
+  </si>
+  <si>
+    <t>btn3</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/spbtn_pin_key_3</t>
+  </si>
+  <si>
+    <t>btn4</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/spbtn_pin_key_4</t>
+  </si>
+  <si>
+    <t>txtCustomerProfile</t>
+  </si>
+  <si>
+    <t>//*[@text='Customize your profile']</t>
+  </si>
+  <si>
     <t>CustomerProfilePage</t>
   </si>
   <si>
@@ -191,12 +269,6 @@
   </si>
   <si>
     <t>ph.com.globe.mybusiness:id/pbtn_customize_profile_submit</t>
-  </si>
-  <si>
-    <t>txtCustomerProfile</t>
-  </si>
-  <si>
-    <t>//*[@text='Customize your profile']</t>
   </si>
   <si>
     <t>btnSkip</t>
@@ -335,6 +407,16 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -343,19 +425,9 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
+      <color indexed="13"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -364,7 +436,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,7 +451,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -389,20 +461,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="14"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="15"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="34">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -412,11 +472,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -425,7 +485,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -433,17 +493,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
@@ -460,7 +520,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -468,23 +528,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,182 +553,67 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="16"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="16"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="16"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -689,62 +634,8 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="8"/>
       </right>
@@ -773,13 +664,26 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="8"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
@@ -807,195 +711,187 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1014,13 +910,11 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="015e88b1"/>
-      <rgbColor rgb="01eef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ff9a9a9a"/>
     </indexedColors>
   </colors>
@@ -2092,150 +1986,142 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="1" max="1" width="2" style="6" customWidth="1"/>
-    <col min="2" max="4" width="33.6016" customWidth="1"/>
-    <col min="2" max="2" width="33.6719" style="6" customWidth="1"/>
-    <col min="3" max="3" width="33.6719" style="6" customWidth="1"/>
-    <col min="4" max="4" width="33.6719" style="6" customWidth="1"/>
-    <col min="5" max="5" width="10" style="6" customWidth="1"/>
-    <col min="6" max="256" width="10" style="6" customWidth="1"/>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="4" width="33.6719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" t="s" s="13">
+      <c r="A3" s="5"/>
+      <c r="B3" t="s" s="8">
         <v>0</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="10"/>
-      <c r="B7" t="s" s="14">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" ht="18.5" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" t="s" s="9">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="14">
+      <c r="C7" t="s" s="9">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="14">
+      <c r="D7" t="s" s="9">
         <v>3</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="10"/>
-      <c r="B9" t="s" s="15">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" ht="16.6" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" ht="16.6" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="12"/>
+      <c r="C10" t="s" s="13">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s" s="14">
         <v>6</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="10"/>
-      <c r="B10" s="17"/>
-      <c r="C10" t="s" s="18">
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" ht="13" customHeight="1">
+      <c r="A12" s="15"/>
+      <c r="B12" s="12"/>
+      <c r="C12" t="s" s="13">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="19">
+      <c r="D12" t="s" s="14">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" ht="13" customHeight="1">
+      <c r="A13" s="2"/>
+      <c r="B13" t="s" s="10">
         <v>7</v>
       </c>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" ht="13" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" ht="13" customHeight="1">
-      <c r="A12" s="20"/>
-      <c r="B12" s="4"/>
-      <c r="C12" t="s" s="4">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" ht="13" customHeight="1">
+      <c r="A14" s="15"/>
+      <c r="B14" s="17"/>
+      <c r="C14" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="D12" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="E12" s="21"/>
-    </row>
-    <row r="13" ht="13" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" t="s" s="3">
+      <c r="D14" t="s" s="19">
         <v>8</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" ht="13" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="4"/>
-      <c r="C14" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s" s="5">
-        <v>8</v>
-      </c>
-      <c r="E14" s="21"/>
+      <c r="E14" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:D3"/>
+  <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
-    <hyperlink ref="D12" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
-    <hyperlink ref="D14" location="'Locators'!R1C1" tooltip="" display="Locators"/>
     <hyperlink ref="D12" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
     <hyperlink ref="D14" location="'Locators'!R1C1" tooltip="" display="Locators"/>
   </hyperlinks>
@@ -2249,299 +2135,333 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="25.3516" style="25" customWidth="1"/>
-    <col min="2" max="2" width="32.8516" style="25" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="25" customWidth="1"/>
-    <col min="4" max="4" width="23.6719" style="25" customWidth="1"/>
-    <col min="5" max="5" width="24.3516" style="25" customWidth="1"/>
-    <col min="6" max="6" width="15" style="25" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="25" customWidth="1"/>
-    <col min="8" max="256" width="14.5" style="25" customWidth="1"/>
+    <col min="1" max="1" width="25.3516" style="20" customWidth="1"/>
+    <col min="2" max="2" width="32.8516" style="20" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="20" customWidth="1"/>
+    <col min="4" max="4" width="23.6719" style="20" customWidth="1"/>
+    <col min="5" max="5" width="24.3516" style="20" customWidth="1"/>
+    <col min="6" max="6" width="15" style="20" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="20" customWidth="1"/>
+    <col min="8" max="16384" width="14.5" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" t="s" s="26">
+      <c r="A1" t="s" s="21">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s" s="22">
+        <v>4</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" t="s" s="21">
         <v>10</v>
       </c>
-      <c r="B1" t="s" s="27">
-        <v>6</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" t="s" s="26">
+      <c r="B2" t="s" s="21">
         <v>11</v>
       </c>
-      <c r="B2" t="s" s="26">
+      <c r="C2" t="s" s="21">
         <v>12</v>
       </c>
-      <c r="C2" t="s" s="26">
+      <c r="D2" t="s" s="21">
         <v>13</v>
       </c>
-      <c r="D2" t="s" s="26">
+      <c r="E2" t="s" s="21">
         <v>14</v>
       </c>
-      <c r="E2" t="s" s="26">
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" t="s" s="21">
         <v>15</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" t="s" s="26">
+      <c r="B3" t="s" s="21">
         <v>16</v>
       </c>
-      <c r="B3" t="s" s="26">
+      <c r="C3" t="s" s="21">
         <v>17</v>
       </c>
-      <c r="C3" t="s" s="26">
+      <c r="D3" s="21"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" t="s" s="21">
         <v>18</v>
       </c>
-      <c r="D3" t="s" s="26">
+      <c r="B4" t="s" s="21">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s" s="21">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s" s="21">
         <v>19</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" t="s" s="26">
+      <c r="E4" t="s" s="21">
         <v>20</v>
       </c>
-      <c r="B4" t="s" s="26">
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" t="s" s="21">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="21">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s" s="21">
         <v>17</v>
       </c>
-      <c r="C4" t="s" s="26">
-        <v>18</v>
-      </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" t="s" s="29">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s" s="29">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s" s="29">
+      <c r="D5" t="s" s="21">
+        <v>22</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" t="s" s="21">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s" s="21">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s" s="21">
         <v>17</v>
       </c>
-      <c r="D5" t="s" s="29">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s" s="29">
-        <v>22</v>
-      </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" t="s" s="29">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s" s="29">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s" s="29">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" t="s" s="24">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s" s="24">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s" s="24">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s" s="24">
         <v>17</v>
       </c>
-      <c r="D6" t="s" s="29">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s" s="29">
-        <v>24</v>
-      </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" t="s" s="29">
+      <c r="E7" t="s" s="24">
         <v>25</v>
       </c>
-      <c r="B7" t="s" s="29">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s" s="29">
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" t="s" s="24">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s" s="24">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s" s="24">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s" s="24">
         <v>17</v>
       </c>
-      <c r="D7" t="s" s="29">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s" s="29">
-        <v>26</v>
-      </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" t="s" s="30">
+      <c r="E8" t="s" s="24">
         <v>27</v>
       </c>
-      <c r="B8" t="s" s="30">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s" s="30">
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" t="s" s="24">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s" s="24">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s" s="24">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s" s="24">
         <v>17</v>
       </c>
-      <c r="D8" t="s" s="30">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s" s="30">
-        <v>28</v>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" t="s" s="31">
+      <c r="E9" t="s" s="24">
         <v>29</v>
       </c>
-      <c r="B9" t="s" s="31">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s" s="31">
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" t="s" s="25">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s" s="25">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s" s="25">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s" s="25">
         <v>17</v>
       </c>
-      <c r="D9" t="s" s="31">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s" s="31">
-        <v>30</v>
-      </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="28"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" t="s" s="31">
+      <c r="E10" t="s" s="25">
         <v>31</v>
       </c>
-      <c r="B10" t="s" s="31">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s" s="31">
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" t="s" s="26">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s" s="26">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s" s="26">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="D10" t="s" s="31">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s" s="31">
-        <v>32</v>
-      </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="28"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" t="s" s="31">
+      <c r="E11" t="s" s="26">
         <v>33</v>
       </c>
-      <c r="B11" t="s" s="31">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s" s="31">
+      <c r="F11" s="27"/>
+      <c r="G11" s="23"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" t="s" s="26">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s" s="26">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s" s="26">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="D11" t="s" s="31">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s" s="31">
-        <v>34</v>
-      </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="28"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="28"/>
+      <c r="E12" t="s" s="26">
+        <v>35</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="28"/>
+      <c r="A13" t="s" s="26">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s" s="26">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s" s="26">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s" s="26">
+        <v>37</v>
+      </c>
+      <c r="F13" s="27"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="28"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="28"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="28"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="28"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="28"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="23"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="28"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="23"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="28"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="23"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="23"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2557,580 +2477,800 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.3516" style="33" customWidth="1"/>
-    <col min="2" max="2" width="19" style="33" customWidth="1"/>
-    <col min="3" max="3" width="19.3516" style="33" customWidth="1"/>
-    <col min="4" max="4" width="83.8516" style="33" customWidth="1"/>
-    <col min="5" max="5" width="21.3516" style="33" customWidth="1"/>
-    <col min="6" max="6" width="11.3516" style="33" customWidth="1"/>
-    <col min="7" max="256" width="14.5" style="33" customWidth="1"/>
+    <col min="1" max="1" width="19.3516" style="28" customWidth="1"/>
+    <col min="2" max="2" width="19" style="28" customWidth="1"/>
+    <col min="3" max="3" width="19.3516" style="28" customWidth="1"/>
+    <col min="4" max="4" width="83.8516" style="28" customWidth="1"/>
+    <col min="5" max="5" width="21.3516" style="28" customWidth="1"/>
+    <col min="6" max="6" width="11.3516" style="28" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" t="s" s="34">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s" s="35">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s" s="35">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s" s="35">
+      <c r="A1" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="E1" t="s" s="35">
+      <c r="B1" t="s" s="29">
         <v>39</v>
       </c>
-      <c r="F1" t="s" s="36">
+      <c r="C1" t="s" s="29">
         <v>40</v>
       </c>
+      <c r="D1" t="s" s="29">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s" s="29">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s" s="29">
+        <v>43</v>
+      </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s" s="37">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s" s="26">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s" s="26">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s" s="26">
+      <c r="A2" t="s" s="29">
         <v>44</v>
       </c>
-      <c r="E2" t="s" s="26">
+      <c r="B2" t="s" s="29">
         <v>45</v>
       </c>
-      <c r="F2" t="s" s="38">
+      <c r="C2" t="s" s="29">
         <v>46</v>
       </c>
+      <c r="D2" t="s" s="29">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s" s="29">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" t="s" s="37">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s" s="26">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="D3" t="s" s="26">
-        <v>48</v>
-      </c>
-      <c r="E3" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s" s="38">
+      <c r="A3" t="s" s="29">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s" s="29">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s" s="29">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1">
+      <c r="A4" t="s" s="29">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s" s="29">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s" s="29">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1">
+      <c r="A5" t="s" s="29">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s" s="29">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s" s="29">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1">
+      <c r="A6" t="s" s="29">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s" s="29">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" t="s" s="37">
+      <c r="D6" t="s" s="30">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s" s="29">
         <v>49</v>
       </c>
-      <c r="B4" t="s" s="26">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s" s="26">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s" s="26">
-        <v>51</v>
-      </c>
-      <c r="E4" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="F4" t="s" s="38">
+    </row>
+    <row r="7" ht="12.75" customHeight="1">
+      <c r="A7" t="s" s="29">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s" s="29">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" t="s" s="37">
+      <c r="D7" t="s" s="29">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s" s="29">
         <v>49</v>
       </c>
-      <c r="B5" t="s" s="26">
+    </row>
+    <row r="8" ht="12.75" customHeight="1">
+      <c r="A8" t="s" s="29">
         <v>52</v>
       </c>
-      <c r="C5" t="s" s="26">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s" s="26">
-        <v>53</v>
-      </c>
-      <c r="E5" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s" s="39">
+      <c r="B8" t="s" s="29">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" t="s" s="37">
+      <c r="D8" t="s" s="29">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s" s="29">
         <v>49</v>
       </c>
-      <c r="B6" t="s" s="26">
-        <v>54</v>
-      </c>
-      <c r="C6" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="D6" t="s" s="26">
-        <v>55</v>
-      </c>
-      <c r="E6" t="s" s="38">
-        <v>45</v>
-      </c>
-      <c r="F6" t="s" s="40">
+    </row>
+    <row r="9" ht="12.75" customHeight="1">
+      <c r="A9" t="s" s="29">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s" s="29">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" t="s" s="37">
+      <c r="D9" t="s" s="30">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s" s="29">
         <v>49</v>
       </c>
-      <c r="B7" t="s" s="26">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s" s="26">
-        <v>43</v>
-      </c>
-      <c r="D7" t="s" s="41">
-        <v>57</v>
-      </c>
-      <c r="E7" t="s" s="38">
-        <v>45</v>
-      </c>
-      <c r="F7" t="s" s="40">
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" t="s" s="29">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s" s="29">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" t="s" s="37">
-        <v>58</v>
-      </c>
-      <c r="B8" t="s" s="41">
-        <v>59</v>
-      </c>
-      <c r="C8" t="s" s="38">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s" s="42">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s" s="43">
-        <v>45</v>
-      </c>
-      <c r="F8" t="s" s="40">
+      <c r="D10" t="s" s="29">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" ht="12.75" customHeight="1">
+      <c r="A11" t="s" s="29">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s" s="29">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" t="s" s="43">
-        <v>58</v>
-      </c>
-      <c r="B9" t="s" s="42">
-        <v>61</v>
-      </c>
-      <c r="C9" t="s" s="43">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s" s="42">
-        <v>62</v>
-      </c>
-      <c r="E9" t="s" s="43">
-        <v>45</v>
-      </c>
-      <c r="F9" t="s" s="40">
+      <c r="D11" t="s" s="29">
+        <v>68</v>
+      </c>
+      <c r="E11" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" ht="12.75" customHeight="1">
+      <c r="A12" t="s" s="29">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s" s="29">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" t="s" s="37">
-        <v>58</v>
-      </c>
-      <c r="B10" t="s" s="44">
-        <v>63</v>
-      </c>
-      <c r="C10" t="s" s="26">
-        <v>43</v>
-      </c>
-      <c r="D10" t="s" s="44">
-        <v>64</v>
-      </c>
-      <c r="E10" t="s" s="38">
-        <v>45</v>
-      </c>
-      <c r="F10" t="s" s="40">
+      <c r="D12" t="s" s="29">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" ht="12.75" customHeight="1">
+      <c r="A13" t="s" s="29">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s" s="29">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" t="s" s="43">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s" s="42">
-        <v>65</v>
-      </c>
-      <c r="C11" t="s" s="43">
-        <v>45</v>
-      </c>
-      <c r="D11" t="s" s="42">
-        <v>66</v>
-      </c>
-      <c r="E11" t="s" s="43">
-        <v>45</v>
-      </c>
-      <c r="F11" t="s" s="40">
+      <c r="D13" t="s" s="29">
+        <v>72</v>
+      </c>
+      <c r="E13" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" ht="12.75" customHeight="1">
+      <c r="A14" t="s" s="29">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s" s="29">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s" s="29">
+        <v>74</v>
+      </c>
+      <c r="E14" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F14" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" ht="12.75" customHeight="1">
+      <c r="A15" t="s" s="29">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s" s="29">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" t="s" s="37">
-        <v>58</v>
-      </c>
-      <c r="B12" t="s" s="35">
-        <v>67</v>
-      </c>
-      <c r="C12" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="D12" t="s" s="35">
-        <v>68</v>
-      </c>
-      <c r="E12" t="s" s="38">
-        <v>45</v>
-      </c>
-      <c r="F12" t="s" s="40">
+      <c r="D15" t="s" s="29">
+        <v>77</v>
+      </c>
+      <c r="E15" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" ht="12.75" customHeight="1">
+      <c r="A16" t="s" s="29">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" t="s" s="37">
-        <v>58</v>
-      </c>
-      <c r="B13" t="s" s="26">
-        <v>69</v>
-      </c>
-      <c r="C13" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="D13" t="s" s="26">
-        <v>70</v>
-      </c>
-      <c r="E13" t="s" s="38">
-        <v>45</v>
-      </c>
-      <c r="F13" t="s" s="40">
+      <c r="D16" t="s" s="29">
+        <v>79</v>
+      </c>
+      <c r="E16" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" t="s" s="29">
+        <v>75</v>
+      </c>
+      <c r="B17" t="s" s="29">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s" s="29">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F17" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" ht="12.75" customHeight="1">
+      <c r="A18" t="s" s="29">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s" s="29">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" t="s" s="37">
-        <v>58</v>
-      </c>
-      <c r="B14" t="s" s="26">
-        <v>71</v>
-      </c>
-      <c r="C14" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="D14" t="s" s="26">
-        <v>72</v>
-      </c>
-      <c r="E14" t="s" s="38">
-        <v>45</v>
-      </c>
-      <c r="F14" t="s" s="40">
+      <c r="D18" t="s" s="29">
+        <v>81</v>
+      </c>
+      <c r="E18" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" ht="12.75" customHeight="1">
+      <c r="A19" t="s" s="29">
+        <v>82</v>
+      </c>
+      <c r="B19" t="s" s="29">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s" s="29">
+        <v>84</v>
+      </c>
+      <c r="E19" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F19" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" ht="12.75" customHeight="1">
+      <c r="A20" t="s" s="29">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s" s="29">
+        <v>85</v>
+      </c>
+      <c r="C20" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" t="s" s="37">
-        <v>58</v>
-      </c>
-      <c r="B15" t="s" s="26">
-        <v>73</v>
-      </c>
-      <c r="C15" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="D15" t="s" s="26">
-        <v>74</v>
-      </c>
-      <c r="E15" t="s" s="38">
-        <v>45</v>
-      </c>
-      <c r="F15" t="s" s="40">
+      <c r="D20" t="s" s="29">
+        <v>86</v>
+      </c>
+      <c r="E20" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" ht="12.75" customHeight="1">
+      <c r="A21" t="s" s="29">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s" s="29">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" t="s" s="37">
-        <v>58</v>
-      </c>
-      <c r="B16" t="s" s="26">
-        <v>75</v>
-      </c>
-      <c r="C16" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="E16" t="s" s="38">
-        <v>45</v>
-      </c>
-      <c r="F16" t="s" s="40">
+      <c r="D21" t="s" s="29">
+        <v>88</v>
+      </c>
+      <c r="E21" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" ht="12.75" customHeight="1">
+      <c r="A22" t="s" s="29">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s" s="29">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s" s="29">
+        <v>90</v>
+      </c>
+      <c r="E22" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F22" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" ht="12.75" customHeight="1">
+      <c r="A23" t="s" s="29">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s" s="29">
+        <v>91</v>
+      </c>
+      <c r="C23" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s" s="29">
+        <v>92</v>
+      </c>
+      <c r="E23" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" ht="12.75" customHeight="1">
+      <c r="A24" t="s" s="29">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s" s="29">
+        <v>93</v>
+      </c>
+      <c r="C24" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s" s="29">
+        <v>94</v>
+      </c>
+      <c r="E24" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F24" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" ht="12.75" customHeight="1">
+      <c r="A25" t="s" s="29">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s" s="29">
+        <v>95</v>
+      </c>
+      <c r="C25" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D25" t="s" s="29">
+        <v>96</v>
+      </c>
+      <c r="E25" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F25" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" ht="12.75" customHeight="1">
+      <c r="A26" t="s" s="29">
+        <v>82</v>
+      </c>
+      <c r="B26" t="s" s="29">
+        <v>97</v>
+      </c>
+      <c r="C26" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s" s="29">
+        <v>98</v>
+      </c>
+      <c r="E26" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F26" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" ht="12.75" customHeight="1">
+      <c r="A27" t="s" s="29">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s" s="29">
+        <v>99</v>
+      </c>
+      <c r="C27" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D27" t="s" s="29">
+        <v>100</v>
+      </c>
+      <c r="E27" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F27" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" ht="12.75" customHeight="1">
+      <c r="A28" t="s" s="29">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s" s="29">
+        <v>101</v>
+      </c>
+      <c r="C28" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" t="s" s="45">
-        <v>58</v>
-      </c>
-      <c r="B17" t="s" s="46">
-        <v>77</v>
-      </c>
-      <c r="C17" t="s" s="46">
-        <v>43</v>
-      </c>
-      <c r="D17" t="s" s="46">
-        <v>78</v>
-      </c>
-      <c r="E17" t="s" s="38">
-        <v>45</v>
-      </c>
-      <c r="F17" t="s" s="40">
+      <c r="D28" t="s" s="29">
+        <v>102</v>
+      </c>
+      <c r="E28" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F28" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" ht="12.75" customHeight="1">
+      <c r="A29" t="s" s="29">
+        <v>103</v>
+      </c>
+      <c r="B29" t="s" s="29">
+        <v>104</v>
+      </c>
+      <c r="C29" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" t="s" s="47">
-        <v>79</v>
-      </c>
-      <c r="B18" t="s" s="48">
-        <v>80</v>
-      </c>
-      <c r="C18" t="s" s="48">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s" s="48">
-        <v>81</v>
-      </c>
-      <c r="E18" t="s" s="49">
-        <v>45</v>
-      </c>
-      <c r="F18" t="s" s="40">
+      <c r="D29" t="s" s="29">
+        <v>105</v>
+      </c>
+      <c r="E29" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="F29" t="s" s="31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" ht="12.75" customHeight="1">
+      <c r="A30" t="s" s="29">
+        <v>103</v>
+      </c>
+      <c r="B30" t="s" s="29">
+        <v>106</v>
+      </c>
+      <c r="C30" t="s" s="29">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" t="s" s="47">
-        <v>79</v>
-      </c>
-      <c r="B19" t="s" s="48">
-        <v>82</v>
-      </c>
-      <c r="C19" t="s" s="48">
-        <v>43</v>
-      </c>
-      <c r="D19" t="s" s="48">
-        <v>83</v>
-      </c>
-      <c r="E19" s="50"/>
-      <c r="F19" s="51"/>
-    </row>
-    <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" t="s" s="47">
-        <v>79</v>
-      </c>
-      <c r="B20" t="s" s="48">
-        <v>84</v>
-      </c>
-      <c r="C20" t="s" s="48">
-        <v>43</v>
-      </c>
-      <c r="D20" t="s" s="52">
-        <v>85</v>
-      </c>
-      <c r="E20" t="s" s="43">
-        <v>86</v>
-      </c>
-      <c r="F20" s="51"/>
-    </row>
-    <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" t="s" s="47">
-        <v>79</v>
-      </c>
-      <c r="B21" t="s" s="48">
-        <v>87</v>
-      </c>
-      <c r="C21" t="s" s="48">
-        <v>43</v>
-      </c>
-      <c r="D21" t="s" s="52">
-        <v>85</v>
-      </c>
-      <c r="E21" t="s" s="43">
-        <v>86</v>
-      </c>
-      <c r="F21" s="51"/>
-    </row>
-    <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" t="s" s="47">
-        <v>79</v>
-      </c>
-      <c r="B22" t="s" s="48">
-        <v>88</v>
-      </c>
-      <c r="C22" t="s" s="48">
-        <v>43</v>
-      </c>
-      <c r="D22" t="s" s="52">
-        <v>85</v>
-      </c>
-      <c r="E22" t="s" s="43">
-        <v>86</v>
-      </c>
-      <c r="F22" s="51"/>
-    </row>
-    <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" t="s" s="47">
-        <v>79</v>
-      </c>
-      <c r="B23" t="s" s="48">
-        <v>89</v>
-      </c>
-      <c r="C23" t="s" s="48">
-        <v>43</v>
-      </c>
-      <c r="D23" t="s" s="52">
-        <v>90</v>
-      </c>
-      <c r="E23" t="s" s="43">
-        <v>86</v>
-      </c>
-      <c r="F23" s="51"/>
-    </row>
-    <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" t="s" s="47">
-        <v>79</v>
-      </c>
-      <c r="B24" t="s" s="48">
-        <v>91</v>
-      </c>
-      <c r="C24" t="s" s="53">
-        <v>43</v>
-      </c>
-      <c r="D24" t="s" s="48">
-        <v>92</v>
-      </c>
-      <c r="E24" s="50"/>
-      <c r="F24" s="51"/>
-    </row>
-    <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" t="s" s="47">
-        <v>93</v>
-      </c>
-      <c r="B25" t="s" s="48">
-        <v>94</v>
-      </c>
-      <c r="C25" t="s" s="54">
-        <v>43</v>
-      </c>
-      <c r="D25" t="s" s="48">
-        <v>95</v>
-      </c>
-      <c r="E25" s="50"/>
-      <c r="F25" s="51"/>
-    </row>
-    <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="55"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="51"/>
-    </row>
-    <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="58"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="51"/>
-    </row>
-    <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="58"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="51"/>
-    </row>
-    <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="58"/>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="51"/>
-    </row>
-    <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="58"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="51"/>
+      <c r="D30" t="s" s="29">
+        <v>107</v>
+      </c>
+      <c r="E30" s="32"/>
+      <c r="F30" s="33"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="58"/>
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="51"/>
+      <c r="A31" t="s" s="29">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s" s="29">
+        <v>108</v>
+      </c>
+      <c r="C31" t="s" s="29">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s" s="29">
+        <v>109</v>
+      </c>
+      <c r="E31" t="s" s="29">
+        <v>110</v>
+      </c>
+      <c r="F31" s="33"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="58"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="51"/>
+      <c r="A32" t="s" s="29">
+        <v>103</v>
+      </c>
+      <c r="B32" t="s" s="29">
+        <v>111</v>
+      </c>
+      <c r="C32" t="s" s="29">
+        <v>46</v>
+      </c>
+      <c r="D32" t="s" s="29">
+        <v>109</v>
+      </c>
+      <c r="E32" t="s" s="29">
+        <v>110</v>
+      </c>
+      <c r="F32" s="33"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="58"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="51"/>
+      <c r="A33" t="s" s="29">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s" s="29">
+        <v>112</v>
+      </c>
+      <c r="C33" t="s" s="29">
+        <v>46</v>
+      </c>
+      <c r="D33" t="s" s="29">
+        <v>109</v>
+      </c>
+      <c r="E33" t="s" s="29">
+        <v>110</v>
+      </c>
+      <c r="F33" s="33"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="58"/>
-      <c r="B34" s="59"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="51"/>
+      <c r="A34" t="s" s="29">
+        <v>103</v>
+      </c>
+      <c r="B34" t="s" s="29">
+        <v>113</v>
+      </c>
+      <c r="C34" t="s" s="29">
+        <v>46</v>
+      </c>
+      <c r="D34" t="s" s="29">
+        <v>114</v>
+      </c>
+      <c r="E34" t="s" s="29">
+        <v>110</v>
+      </c>
+      <c r="F34" s="33"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="58"/>
-      <c r="B35" s="59"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="51"/>
+      <c r="A35" t="s" s="29">
+        <v>103</v>
+      </c>
+      <c r="B35" t="s" s="29">
+        <v>115</v>
+      </c>
+      <c r="C35" t="s" s="29">
+        <v>46</v>
+      </c>
+      <c r="D35" t="s" s="29">
+        <v>116</v>
+      </c>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
+    </row>
+    <row r="36" ht="13.65" customHeight="1">
+      <c r="A36" t="s" s="29">
+        <v>117</v>
+      </c>
+      <c r="B36" t="s" s="29">
+        <v>118</v>
+      </c>
+      <c r="C36" t="s" s="29">
+        <v>46</v>
+      </c>
+      <c r="D36" t="s" s="29">
+        <v>119</v>
+      </c>
+      <c r="E36" s="32"/>
+      <c r="F36" s="33"/>
+    </row>
+    <row r="37" ht="12.75" customHeight="1">
+      <c r="A37" s="34"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="37"/>
+    </row>
+    <row r="38" ht="12.75" customHeight="1">
+      <c r="A38" s="38"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="41"/>
+    </row>
+    <row r="39" ht="12.75" customHeight="1">
+      <c r="A39" s="38"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="41"/>
+    </row>
+    <row r="40" ht="12.75" customHeight="1">
+      <c r="A40" s="38"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="41"/>
+    </row>
+    <row r="41" ht="12.75" customHeight="1">
+      <c r="A41" s="38"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="41"/>
+    </row>
+    <row r="42" ht="12.75" customHeight="1">
+      <c r="A42" s="38"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="41"/>
+    </row>
+    <row r="43" ht="12.75" customHeight="1">
+      <c r="A43" s="38"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="41"/>
+    </row>
+    <row r="44" ht="12.75" customHeight="1">
+      <c r="A44" s="38"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="41"/>
+    </row>
+    <row r="45" ht="12.75" customHeight="1">
+      <c r="A45" s="38"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="41"/>
+    </row>
+    <row r="46" ht="12.75" customHeight="1">
+      <c r="A46" s="42"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Added test scripts for HomaPage and VerifyHomePage.java
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="130">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -27,17 +27,20 @@
     <t>Excel Worksheet Name</t>
   </si>
   <si>
+    <t>Export Summary</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
     <t>Testdata</t>
-  </si>
-  <si>
-    <t>Table 1</t>
   </si>
   <si>
     <r>
       <rPr>
         <u val="single"/>
         <sz val="12"/>
-        <color indexed="13"/>
+        <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
       <t>Testdata</t>
@@ -51,7 +54,7 @@
       <rPr>
         <u val="single"/>
         <sz val="12"/>
-        <color indexed="13"/>
+        <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
       <t>Locators</t>
@@ -145,6 +148,18 @@
     <t>nickname=Libertea</t>
   </si>
   <si>
+    <t>verifyNickname</t>
+  </si>
+  <si>
+    <t>nickname=Valir</t>
+  </si>
+  <si>
+    <t>verifyNotificationBell</t>
+  </si>
+  <si>
+    <t>nickname=Gloo</t>
+  </si>
+  <si>
     <t>Page</t>
   </si>
   <si>
@@ -389,6 +404,21 @@
   </si>
   <si>
     <t>ph.com.globe.mybusiness:id/btn_positive</t>
+  </si>
+  <si>
+    <t>txtNickname</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/title_small</t>
+  </si>
+  <si>
+    <t>btnNotificationBell</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/notif_inbox</t>
   </si>
 </sst>
 </file>
@@ -407,16 +437,6 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -425,9 +445,19 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="13"/>
+      <color indexed="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -436,7 +466,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,7 +481,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -461,8 +491,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -472,11 +514,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -485,7 +527,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -493,17 +535,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
@@ -520,7 +562,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom/>
@@ -528,23 +570,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,67 +595,67 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -634,7 +676,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -642,7 +684,9 @@
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -671,8 +715,17 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -682,12 +735,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -713,14 +768,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,7 +799,7 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -744,7 +810,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -754,143 +820,173 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -910,11 +1006,13 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="015e88b1"/>
+      <rgbColor rgb="01eef3f4"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ff9a9a9a"/>
     </indexedColors>
   </colors>
@@ -1986,142 +2084,150 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="4" width="33.6719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" style="6" customWidth="1"/>
+    <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="2" max="2" width="33.6719" style="6" customWidth="1"/>
+    <col min="3" max="3" width="33.6719" style="6" customWidth="1"/>
+    <col min="4" max="4" width="33.6719" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="256" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" t="s" s="8">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s" s="13">
         <v>0</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" ht="18.5" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" t="s" s="9">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="14">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="9">
+      <c r="C7" t="s" s="14">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="9">
+      <c r="D7" t="s" s="14">
         <v>3</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" ht="16.6" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" t="s" s="10">
-        <v>4</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" ht="16.6" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="12"/>
-      <c r="C10" t="s" s="13">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="10"/>
+      <c r="B9" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="10"/>
+      <c r="B10" s="17"/>
+      <c r="C10" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="14">
+      <c r="D10" t="s" s="19">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="10"/>
+      <c r="B11" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" ht="13" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" t="s" s="10">
-        <v>4</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="7"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="12"/>
     </row>
     <row r="12" ht="13" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="12"/>
-      <c r="C12" t="s" s="13">
+      <c r="A12" s="20"/>
+      <c r="B12" s="4"/>
+      <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="D12" t="s" s="14">
+      <c r="D12" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="21"/>
     </row>
     <row r="13" ht="13" customHeight="1">
-      <c r="A13" s="2"/>
-      <c r="B13" t="s" s="10">
-        <v>7</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="4"/>
+      <c r="A13" s="7"/>
+      <c r="B13" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" ht="13" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="17"/>
-      <c r="C14" t="s" s="18">
+      <c r="A14" s="20"/>
+      <c r="B14" s="4"/>
+      <c r="C14" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="D14" t="s" s="19">
+      <c r="D14" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="E14" s="16"/>
+      <c r="E14" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
+    <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
+    <hyperlink ref="D12" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
+    <hyperlink ref="D14" location="'Locators'!R1C1" tooltip="" display="Locators"/>
     <hyperlink ref="D12" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
     <hyperlink ref="D14" location="'Locators'!R1C1" tooltip="" display="Locators"/>
   </hyperlinks>
@@ -2141,327 +2247,347 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="25.3516" style="20" customWidth="1"/>
-    <col min="2" max="2" width="32.8516" style="20" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="20" customWidth="1"/>
-    <col min="4" max="4" width="23.6719" style="20" customWidth="1"/>
-    <col min="5" max="5" width="24.3516" style="20" customWidth="1"/>
-    <col min="6" max="6" width="15" style="20" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="20" customWidth="1"/>
-    <col min="8" max="16384" width="14.5" style="20" customWidth="1"/>
+    <col min="1" max="1" width="25.3516" style="25" customWidth="1"/>
+    <col min="2" max="2" width="32.8516" style="25" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="25" customWidth="1"/>
+    <col min="4" max="4" width="23.6719" style="25" customWidth="1"/>
+    <col min="5" max="5" width="24.3516" style="25" customWidth="1"/>
+    <col min="6" max="6" width="15" style="25" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="25" customWidth="1"/>
+    <col min="8" max="256" width="14.5" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" t="s" s="21">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s" s="22">
-        <v>4</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="A1" t="s" s="26">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s" s="27">
+        <v>6</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" t="s" s="21">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s" s="21">
+      <c r="A2" t="s" s="26">
         <v>11</v>
       </c>
-      <c r="C2" t="s" s="21">
+      <c r="B2" t="s" s="26">
         <v>12</v>
       </c>
-      <c r="D2" t="s" s="21">
+      <c r="C2" t="s" s="26">
         <v>13</v>
       </c>
-      <c r="E2" t="s" s="21">
+      <c r="D2" t="s" s="26">
         <v>14</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="E2" t="s" s="26">
+        <v>15</v>
+      </c>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" t="s" s="21">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s" s="21">
+      <c r="A3" t="s" s="26">
         <v>16</v>
       </c>
-      <c r="C3" t="s" s="21">
+      <c r="B3" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
+      <c r="C3" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" t="s" s="21">
+      <c r="A4" t="s" s="26">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s" s="26">
         <v>18</v>
       </c>
-      <c r="B4" t="s" s="21">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s" s="21">
+      <c r="D4" t="s" s="26">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" t="s" s="26">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="D4" t="s" s="21">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s" s="21">
-        <v>20</v>
-      </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" t="s" s="21">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s" s="21">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s" s="21">
+      <c r="C5" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s" s="26">
+        <v>23</v>
+      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" t="s" s="26">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="D5" t="s" s="21">
-        <v>22</v>
-      </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" t="s" s="21">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s" s="21">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s" s="21">
+      <c r="C6" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" t="s" s="29">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s" s="29">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s" s="29">
         <v>17</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" t="s" s="24">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s" s="24">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s" s="24">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s" s="24">
+      <c r="D7" t="s" s="29">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s" s="29">
+        <v>26</v>
+      </c>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" t="s" s="29">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s" s="29">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s" s="29">
         <v>17</v>
       </c>
-      <c r="E7" t="s" s="24">
-        <v>25</v>
-      </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" t="s" s="24">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s" s="24">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s" s="24">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s" s="24">
+      <c r="D8" t="s" s="29">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s" s="29">
+        <v>28</v>
+      </c>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" t="s" s="29">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s" s="29">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s" s="29">
         <v>17</v>
       </c>
-      <c r="E8" t="s" s="24">
-        <v>27</v>
-      </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" t="s" s="24">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s" s="24">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s" s="24">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s" s="24">
+      <c r="D9" t="s" s="29">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s" s="29">
+        <v>30</v>
+      </c>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" t="s" s="30">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s" s="30">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s" s="30">
         <v>17</v>
       </c>
-      <c r="E9" t="s" s="24">
-        <v>29</v>
-      </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" t="s" s="25">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s" s="25">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s" s="25">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s" s="25">
+      <c r="D10" t="s" s="30">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s" s="30">
+        <v>32</v>
+      </c>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" t="s" s="31">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s" s="31">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s" s="31">
         <v>17</v>
       </c>
-      <c r="E10" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" t="s" s="26">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s" s="26">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s" s="26">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s" s="26">
+      <c r="D11" t="s" s="31">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s" s="31">
+        <v>34</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="28"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" t="s" s="31">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s" s="31">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s" s="31">
         <v>17</v>
       </c>
-      <c r="E11" t="s" s="26">
-        <v>33</v>
-      </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="23"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" t="s" s="26">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s" s="26">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s" s="26">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s" s="26">
+      <c r="D12" t="s" s="31">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s" s="31">
+        <v>36</v>
+      </c>
+      <c r="F12" s="32"/>
+      <c r="G12" s="28"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" t="s" s="31">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s" s="31">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s" s="31">
         <v>17</v>
       </c>
-      <c r="E12" t="s" s="26">
-        <v>35</v>
-      </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="23"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" t="s" s="26">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s" s="26">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s" s="26">
-        <v>16</v>
-      </c>
-      <c r="D13" t="s" s="26">
+      <c r="D13" t="s" s="31">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s" s="31">
+        <v>38</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="28"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" t="s" s="31">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s" s="31">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s" s="31">
         <v>17</v>
       </c>
-      <c r="E13" t="s" s="26">
-        <v>37</v>
-      </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="23"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="23"/>
+      <c r="D14" t="s" s="31">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s" s="31">
+        <v>40</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="23"/>
+      <c r="A15" t="s" s="31">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s" s="31">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s" s="31">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s" s="31">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s" s="31">
+        <v>42</v>
+      </c>
+      <c r="F15" s="32"/>
+      <c r="G15" s="28"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="23"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="28"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="23"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="28"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="23"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="28"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="23"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="28"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="23"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="23"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="28"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="23"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2483,794 +2609,812 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.3516" style="28" customWidth="1"/>
-    <col min="2" max="2" width="19" style="28" customWidth="1"/>
-    <col min="3" max="3" width="19.3516" style="28" customWidth="1"/>
-    <col min="4" max="4" width="83.8516" style="28" customWidth="1"/>
-    <col min="5" max="5" width="21.3516" style="28" customWidth="1"/>
-    <col min="6" max="6" width="11.3516" style="28" customWidth="1"/>
-    <col min="7" max="16384" width="14.5" style="28" customWidth="1"/>
+    <col min="1" max="1" width="19.3516" style="33" customWidth="1"/>
+    <col min="2" max="2" width="19" style="33" customWidth="1"/>
+    <col min="3" max="3" width="19.3516" style="33" customWidth="1"/>
+    <col min="4" max="4" width="83.8516" style="33" customWidth="1"/>
+    <col min="5" max="5" width="21.3516" style="33" customWidth="1"/>
+    <col min="6" max="6" width="11.3516" style="33" customWidth="1"/>
+    <col min="7" max="256" width="14.5" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" t="s" s="29">
-        <v>38</v>
-      </c>
-      <c r="B1" t="s" s="29">
-        <v>39</v>
-      </c>
-      <c r="C1" t="s" s="29">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s" s="29">
-        <v>41</v>
-      </c>
-      <c r="E1" t="s" s="29">
-        <v>42</v>
-      </c>
-      <c r="F1" t="s" s="29">
+      <c r="A1" t="s" s="34">
         <v>43</v>
       </c>
+      <c r="B1" t="s" s="34">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s" s="34">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s" s="34">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s" s="34">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s" s="34">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s" s="29">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s" s="29">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s" s="29">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s" s="29">
+      <c r="A2" t="s" s="34">
         <v>49</v>
       </c>
+      <c r="B2" t="s" s="34">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s" s="34">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s" s="34">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" t="s" s="29">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s" s="29">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="D3" t="s" s="29">
+      <c r="A3" t="s" s="34">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s" s="34">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s" s="34">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s" s="34">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1">
+      <c r="A4" t="s" s="34">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s" s="34">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s" s="34">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s" s="34">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1">
+      <c r="A5" t="s" s="34">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s" s="34">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s" s="34">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s" s="34">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1">
+      <c r="A6" t="s" s="34">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s" s="34">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s" s="34">
         <v>51</v>
       </c>
-      <c r="E3" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F3" t="s" s="29">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" t="s" s="29">
-        <v>52</v>
-      </c>
-      <c r="B4" t="s" s="29">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s" s="29">
+      <c r="D6" t="s" s="35">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s" s="34">
         <v>54</v>
       </c>
-      <c r="E4" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F4" t="s" s="29">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" t="s" s="29">
-        <v>52</v>
-      </c>
-      <c r="B5" t="s" s="29">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="D5" t="s" s="29">
-        <v>56</v>
-      </c>
-      <c r="E5" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s" s="29">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" t="s" s="29">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s" s="29">
+    </row>
+    <row r="7" ht="12.75" customHeight="1">
+      <c r="A7" t="s" s="34">
         <v>57</v>
       </c>
-      <c r="C6" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s" s="30">
-        <v>58</v>
-      </c>
-      <c r="E6" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s" s="29">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" t="s" s="29">
-        <v>52</v>
-      </c>
-      <c r="B7" t="s" s="29">
-        <v>59</v>
-      </c>
-      <c r="C7" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s" s="29">
-        <v>60</v>
-      </c>
-      <c r="E7" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F7" t="s" s="29">
-        <v>49</v>
+      <c r="B7" t="s" s="34">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s" s="34">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F7" t="s" s="34">
+        <v>54</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" t="s" s="29">
-        <v>52</v>
-      </c>
-      <c r="B8" t="s" s="29">
-        <v>61</v>
-      </c>
-      <c r="C8" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s" s="29">
-        <v>62</v>
-      </c>
-      <c r="E8" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F8" t="s" s="29">
-        <v>49</v>
+      <c r="A8" t="s" s="34">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s" s="34">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s" s="34">
+        <v>67</v>
+      </c>
+      <c r="E8" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s" s="34">
+        <v>54</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" t="s" s="29">
-        <v>52</v>
-      </c>
-      <c r="B9" t="s" s="29">
-        <v>63</v>
-      </c>
-      <c r="C9" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s" s="30">
-        <v>64</v>
-      </c>
-      <c r="E9" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F9" t="s" s="29">
-        <v>49</v>
+      <c r="A9" t="s" s="34">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s" s="34">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s" s="35">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s" s="34">
+        <v>54</v>
       </c>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" t="s" s="29">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s" s="29">
-        <v>65</v>
-      </c>
-      <c r="C10" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s" s="29">
-        <v>66</v>
-      </c>
-      <c r="E10" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F10" t="s" s="29">
-        <v>49</v>
+      <c r="A10" t="s" s="34">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s" s="34">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s" s="34">
+        <v>71</v>
+      </c>
+      <c r="E10" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F10" t="s" s="34">
+        <v>54</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" t="s" s="29">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s" s="29">
-        <v>67</v>
-      </c>
-      <c r="C11" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s" s="29">
-        <v>68</v>
-      </c>
-      <c r="E11" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F11" t="s" s="29">
-        <v>49</v>
+      <c r="A11" t="s" s="34">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s" s="34">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s" s="34">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s" s="34">
+        <v>54</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" t="s" s="29">
-        <v>52</v>
-      </c>
-      <c r="B12" t="s" s="29">
-        <v>69</v>
-      </c>
-      <c r="C12" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D12" t="s" s="29">
-        <v>70</v>
-      </c>
-      <c r="E12" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F12" t="s" s="29">
-        <v>49</v>
+      <c r="A12" t="s" s="34">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s" s="34">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s" s="34">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s" s="34">
+        <v>54</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" t="s" s="29">
-        <v>52</v>
-      </c>
-      <c r="B13" t="s" s="29">
-        <v>71</v>
-      </c>
-      <c r="C13" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D13" t="s" s="29">
-        <v>72</v>
-      </c>
-      <c r="E13" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F13" t="s" s="29">
-        <v>49</v>
+      <c r="A13" t="s" s="34">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s" s="34">
+        <v>76</v>
+      </c>
+      <c r="C13" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s" s="34">
+        <v>77</v>
+      </c>
+      <c r="E13" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s" s="34">
+        <v>54</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" t="s" s="29">
-        <v>52</v>
-      </c>
-      <c r="B14" t="s" s="29">
-        <v>73</v>
-      </c>
-      <c r="C14" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="D14" t="s" s="29">
-        <v>74</v>
-      </c>
-      <c r="E14" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F14" t="s" s="31">
-        <v>49</v>
+      <c r="A14" t="s" s="34">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s" s="34">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s" s="34">
+        <v>79</v>
+      </c>
+      <c r="E14" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" t="s" s="29">
-        <v>75</v>
-      </c>
-      <c r="B15" t="s" s="29">
-        <v>76</v>
-      </c>
-      <c r="C15" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D15" t="s" s="29">
-        <v>77</v>
-      </c>
-      <c r="E15" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F15" t="s" s="29">
-        <v>49</v>
+      <c r="A15" t="s" s="34">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s" s="34">
+        <v>81</v>
+      </c>
+      <c r="C15" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s" s="34">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s" s="34">
+        <v>54</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" t="s" s="29">
-        <v>75</v>
-      </c>
-      <c r="B16" t="s" s="29">
+      <c r="A16" t="s" s="34">
+        <v>80</v>
+      </c>
+      <c r="B16" t="s" s="34">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s" s="34">
+        <v>84</v>
+      </c>
+      <c r="E16" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F16" t="s" s="34">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" t="s" s="34">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s" s="34">
         <v>78</v>
       </c>
-      <c r="C16" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D16" t="s" s="29">
+      <c r="C17" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s" s="34">
         <v>79</v>
       </c>
-      <c r="E16" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F16" t="s" s="29">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" t="s" s="29">
-        <v>75</v>
-      </c>
-      <c r="B17" t="s" s="29">
-        <v>73</v>
-      </c>
-      <c r="C17" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="D17" t="s" s="29">
-        <v>74</v>
-      </c>
-      <c r="E17" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F17" t="s" s="31">
-        <v>49</v>
+      <c r="E17" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" t="s" s="29">
-        <v>75</v>
-      </c>
-      <c r="B18" t="s" s="29">
+      <c r="A18" t="s" s="34">
         <v>80</v>
       </c>
-      <c r="C18" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s" s="29">
-        <v>81</v>
-      </c>
-      <c r="E18" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F18" t="s" s="31">
-        <v>49</v>
+      <c r="B18" t="s" s="34">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s" s="34">
+        <v>86</v>
+      </c>
+      <c r="E18" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F18" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" t="s" s="29">
-        <v>82</v>
-      </c>
-      <c r="B19" t="s" s="29">
-        <v>83</v>
-      </c>
-      <c r="C19" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="D19" t="s" s="29">
-        <v>84</v>
-      </c>
-      <c r="E19" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F19" t="s" s="31">
-        <v>49</v>
+      <c r="A19" t="s" s="34">
+        <v>87</v>
+      </c>
+      <c r="B19" t="s" s="34">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s" s="34">
+        <v>89</v>
+      </c>
+      <c r="E19" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F19" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" t="s" s="29">
-        <v>82</v>
-      </c>
-      <c r="B20" t="s" s="29">
-        <v>85</v>
-      </c>
-      <c r="C20" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D20" t="s" s="29">
-        <v>86</v>
-      </c>
-      <c r="E20" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F20" t="s" s="31">
-        <v>49</v>
+      <c r="A20" t="s" s="34">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s" s="34">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s" s="34">
+        <v>91</v>
+      </c>
+      <c r="E20" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F20" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" t="s" s="29">
-        <v>82</v>
-      </c>
-      <c r="B21" t="s" s="29">
+      <c r="A21" t="s" s="34">
         <v>87</v>
       </c>
-      <c r="C21" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D21" t="s" s="29">
-        <v>88</v>
-      </c>
-      <c r="E21" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F21" t="s" s="31">
-        <v>49</v>
+      <c r="B21" t="s" s="34">
+        <v>92</v>
+      </c>
+      <c r="C21" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s" s="34">
+        <v>93</v>
+      </c>
+      <c r="E21" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F21" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" t="s" s="29">
-        <v>82</v>
-      </c>
-      <c r="B22" t="s" s="29">
-        <v>89</v>
-      </c>
-      <c r="C22" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="D22" t="s" s="29">
-        <v>90</v>
-      </c>
-      <c r="E22" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F22" t="s" s="31">
-        <v>49</v>
+      <c r="A22" t="s" s="34">
+        <v>87</v>
+      </c>
+      <c r="B22" t="s" s="34">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s" s="34">
+        <v>95</v>
+      </c>
+      <c r="E22" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F22" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" t="s" s="29">
-        <v>82</v>
-      </c>
-      <c r="B23" t="s" s="29">
-        <v>91</v>
-      </c>
-      <c r="C23" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="D23" t="s" s="29">
-        <v>92</v>
-      </c>
-      <c r="E23" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F23" t="s" s="31">
-        <v>49</v>
+      <c r="A23" t="s" s="34">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s" s="34">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s" s="34">
+        <v>97</v>
+      </c>
+      <c r="E23" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F23" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" t="s" s="29">
-        <v>82</v>
-      </c>
-      <c r="B24" t="s" s="29">
-        <v>93</v>
-      </c>
-      <c r="C24" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="D24" t="s" s="29">
-        <v>94</v>
-      </c>
-      <c r="E24" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F24" t="s" s="31">
-        <v>49</v>
+      <c r="A24" t="s" s="34">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s" s="34">
+        <v>98</v>
+      </c>
+      <c r="C24" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="D24" t="s" s="34">
+        <v>99</v>
+      </c>
+      <c r="E24" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F24" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" t="s" s="29">
-        <v>82</v>
-      </c>
-      <c r="B25" t="s" s="29">
-        <v>95</v>
-      </c>
-      <c r="C25" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="D25" t="s" s="29">
-        <v>96</v>
-      </c>
-      <c r="E25" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F25" t="s" s="31">
-        <v>49</v>
+      <c r="A25" t="s" s="34">
+        <v>87</v>
+      </c>
+      <c r="B25" t="s" s="34">
+        <v>100</v>
+      </c>
+      <c r="C25" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="D25" t="s" s="34">
+        <v>101</v>
+      </c>
+      <c r="E25" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F25" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" t="s" s="29">
-        <v>82</v>
-      </c>
-      <c r="B26" t="s" s="29">
-        <v>97</v>
-      </c>
-      <c r="C26" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="D26" t="s" s="29">
-        <v>98</v>
-      </c>
-      <c r="E26" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F26" t="s" s="31">
-        <v>49</v>
+      <c r="A26" t="s" s="34">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s" s="34">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="D26" t="s" s="34">
+        <v>103</v>
+      </c>
+      <c r="E26" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F26" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" t="s" s="29">
-        <v>82</v>
-      </c>
-      <c r="B27" t="s" s="29">
-        <v>99</v>
-      </c>
-      <c r="C27" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="D27" t="s" s="29">
-        <v>100</v>
-      </c>
-      <c r="E27" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F27" t="s" s="31">
-        <v>49</v>
+      <c r="A27" t="s" s="34">
+        <v>87</v>
+      </c>
+      <c r="B27" t="s" s="34">
+        <v>104</v>
+      </c>
+      <c r="C27" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s" s="34">
+        <v>105</v>
+      </c>
+      <c r="E27" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F27" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" t="s" s="29">
-        <v>82</v>
-      </c>
-      <c r="B28" t="s" s="29">
-        <v>101</v>
-      </c>
-      <c r="C28" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D28" t="s" s="29">
-        <v>102</v>
-      </c>
-      <c r="E28" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F28" t="s" s="31">
-        <v>49</v>
+      <c r="A28" t="s" s="34">
+        <v>87</v>
+      </c>
+      <c r="B28" t="s" s="34">
+        <v>106</v>
+      </c>
+      <c r="C28" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s" s="34">
+        <v>107</v>
+      </c>
+      <c r="E28" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F28" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" t="s" s="29">
-        <v>103</v>
-      </c>
-      <c r="B29" t="s" s="29">
-        <v>104</v>
-      </c>
-      <c r="C29" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D29" t="s" s="29">
-        <v>105</v>
-      </c>
-      <c r="E29" t="s" s="29">
-        <v>48</v>
-      </c>
-      <c r="F29" t="s" s="31">
-        <v>49</v>
+      <c r="A29" t="s" s="34">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s" s="34">
+        <v>109</v>
+      </c>
+      <c r="C29" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D29" t="s" s="34">
+        <v>110</v>
+      </c>
+      <c r="E29" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="F29" t="s" s="36">
+        <v>54</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" t="s" s="29">
-        <v>103</v>
-      </c>
-      <c r="B30" t="s" s="29">
-        <v>106</v>
-      </c>
-      <c r="C30" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D30" t="s" s="29">
-        <v>107</v>
-      </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="33"/>
+      <c r="A30" t="s" s="34">
+        <v>108</v>
+      </c>
+      <c r="B30" t="s" s="34">
+        <v>111</v>
+      </c>
+      <c r="C30" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D30" t="s" s="34">
+        <v>112</v>
+      </c>
+      <c r="E30" s="37"/>
+      <c r="F30" s="38"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" t="s" s="29">
-        <v>103</v>
-      </c>
-      <c r="B31" t="s" s="29">
+      <c r="A31" t="s" s="34">
         <v>108</v>
       </c>
-      <c r="C31" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D31" t="s" s="29">
-        <v>109</v>
-      </c>
-      <c r="E31" t="s" s="29">
-        <v>110</v>
-      </c>
-      <c r="F31" s="33"/>
+      <c r="B31" t="s" s="34">
+        <v>113</v>
+      </c>
+      <c r="C31" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D31" t="s" s="34">
+        <v>114</v>
+      </c>
+      <c r="E31" t="s" s="34">
+        <v>115</v>
+      </c>
+      <c r="F31" s="38"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" t="s" s="29">
-        <v>103</v>
-      </c>
-      <c r="B32" t="s" s="29">
-        <v>111</v>
-      </c>
-      <c r="C32" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D32" t="s" s="29">
-        <v>109</v>
-      </c>
-      <c r="E32" t="s" s="29">
-        <v>110</v>
-      </c>
-      <c r="F32" s="33"/>
+      <c r="A32" t="s" s="34">
+        <v>108</v>
+      </c>
+      <c r="B32" t="s" s="34">
+        <v>116</v>
+      </c>
+      <c r="C32" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D32" t="s" s="34">
+        <v>114</v>
+      </c>
+      <c r="E32" t="s" s="34">
+        <v>115</v>
+      </c>
+      <c r="F32" s="38"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" t="s" s="29">
-        <v>103</v>
-      </c>
-      <c r="B33" t="s" s="29">
-        <v>112</v>
-      </c>
-      <c r="C33" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D33" t="s" s="29">
-        <v>109</v>
-      </c>
-      <c r="E33" t="s" s="29">
-        <v>110</v>
-      </c>
-      <c r="F33" s="33"/>
+      <c r="A33" t="s" s="34">
+        <v>108</v>
+      </c>
+      <c r="B33" t="s" s="34">
+        <v>117</v>
+      </c>
+      <c r="C33" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D33" t="s" s="34">
+        <v>114</v>
+      </c>
+      <c r="E33" t="s" s="34">
+        <v>115</v>
+      </c>
+      <c r="F33" s="38"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" t="s" s="29">
-        <v>103</v>
-      </c>
-      <c r="B34" t="s" s="29">
-        <v>113</v>
-      </c>
-      <c r="C34" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D34" t="s" s="29">
-        <v>114</v>
-      </c>
-      <c r="E34" t="s" s="29">
-        <v>110</v>
-      </c>
-      <c r="F34" s="33"/>
+      <c r="A34" t="s" s="34">
+        <v>108</v>
+      </c>
+      <c r="B34" t="s" s="34">
+        <v>118</v>
+      </c>
+      <c r="C34" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D34" t="s" s="34">
+        <v>119</v>
+      </c>
+      <c r="E34" t="s" s="34">
+        <v>115</v>
+      </c>
+      <c r="F34" s="38"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" t="s" s="29">
-        <v>103</v>
-      </c>
-      <c r="B35" t="s" s="29">
+      <c r="A35" t="s" s="34">
+        <v>108</v>
+      </c>
+      <c r="B35" t="s" s="34">
+        <v>120</v>
+      </c>
+      <c r="C35" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D35" t="s" s="34">
+        <v>121</v>
+      </c>
+      <c r="E35" s="37"/>
+      <c r="F35" s="38"/>
+    </row>
+    <row r="36" ht="13.65" customHeight="1">
+      <c r="A36" t="s" s="34">
+        <v>122</v>
+      </c>
+      <c r="B36" t="s" s="34">
+        <v>123</v>
+      </c>
+      <c r="C36" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="D36" t="s" s="34">
+        <v>124</v>
+      </c>
+      <c r="E36" s="37"/>
+      <c r="F36" s="38"/>
+    </row>
+    <row r="37" ht="12.75" customHeight="1">
+      <c r="A37" t="s" s="39">
+        <v>122</v>
+      </c>
+      <c r="B37" t="s" s="40">
+        <v>125</v>
+      </c>
+      <c r="C37" t="s" s="40">
+        <v>126</v>
+      </c>
+      <c r="D37" t="s" s="41">
+        <v>127</v>
+      </c>
+      <c r="E37" s="42"/>
+      <c r="F37" s="43"/>
+    </row>
+    <row r="38" ht="12.75" customHeight="1">
+      <c r="A38" t="s" s="44">
+        <v>122</v>
+      </c>
+      <c r="B38" t="s" s="45">
+        <v>128</v>
+      </c>
+      <c r="C38" t="s" s="45">
+        <v>126</v>
+      </c>
+      <c r="D38" t="s" s="46">
+        <v>129</v>
+      </c>
+      <c r="E38" t="s" s="47">
         <v>115</v>
       </c>
-      <c r="C35" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D35" t="s" s="29">
-        <v>116</v>
-      </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
-    </row>
-    <row r="36" ht="13.65" customHeight="1">
-      <c r="A36" t="s" s="29">
-        <v>117</v>
-      </c>
-      <c r="B36" t="s" s="29">
-        <v>118</v>
-      </c>
-      <c r="C36" t="s" s="29">
-        <v>46</v>
-      </c>
-      <c r="D36" t="s" s="29">
-        <v>119</v>
-      </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="33"/>
-    </row>
-    <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="34"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="37"/>
-    </row>
-    <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="38"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="41"/>
+      <c r="F38" s="48"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="38"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="41"/>
+      <c r="A39" s="49"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="48"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="38"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="41"/>
+      <c r="A40" s="49"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="48"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="38"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="41"/>
+      <c r="A41" s="49"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="48"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="38"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="41"/>
+      <c r="A42" s="49"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="48"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="38"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="40"/>
-      <c r="F43" s="41"/>
+      <c r="A43" s="49"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="48"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="38"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="41"/>
+      <c r="A44" s="49"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="48"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
-      <c r="A45" s="38"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="40"/>
-      <c r="F45" s="41"/>
+      <c r="A45" s="49"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="48"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="42"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="45"/>
+      <c r="A46" s="52"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Modified NotificationPage and VerifyNotificationPage
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="138">
   <si>
     <t>TCName</t>
   </si>
@@ -127,7 +127,13 @@
     <t>nickname=Laine</t>
   </si>
   <si>
-    <t>verifyViewNotification</t>
+    <t>verifyViewNotificationContent</t>
+  </si>
+  <si>
+    <t>verifyNotifSearchResults</t>
+  </si>
+  <si>
+    <t>message=Sample Notification - SGBBAPP</t>
   </si>
   <si>
     <t>Page</t>
@@ -409,16 +415,22 @@
     <t>ph.com.globe.mybusiness:id/tv_customer_id</t>
   </si>
   <si>
-    <t>firstNotif</t>
+    <t>btnNotification</t>
   </si>
   <si>
     <t>//android.widget.LinearLayout[@resource-id='ph.com.globe.mybusiness:id/front_layout']</t>
   </si>
   <si>
-    <t>notifContent</t>
+    <t>txtNotifContent</t>
   </si>
   <si>
     <t>//android.widget.LinearLayout[@resource-id='ph.com.globe.mybusiness:id/clickable_area']</t>
+  </si>
+  <si>
+    <t>txtNotifSearchResult</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/tv_message</t>
   </si>
 </sst>
 </file>
@@ -529,9 +541,6 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -548,6 +557,9 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1054,7 +1066,7 @@
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -1067,7 +1079,23 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="19" ht="15.75" customHeight="1"/>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2085,833 +2113,852 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" ht="12.75" customHeight="1">
+      <c r="A15" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="6" t="s">
+      <c r="D15" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" ht="12.75" customHeight="1">
+      <c r="A16" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="17" t="s">
+      <c r="D16" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="C17" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="18" t="s">
+      <c r="E17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" ht="12.75" customHeight="1">
+      <c r="A18" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="B18" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>45</v>
-      </c>
       <c r="D18" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>83</v>
+        <v>49</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>85</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>86</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>85</v>
+        <v>47</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>87</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>90</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>89</v>
+        <v>49</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B33" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>108</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="13" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="13" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D40" s="22" t="s">
+      <c r="A40" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="B40" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F40" s="22" t="s">
-        <v>48</v>
+      <c r="D40" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="16" t="s">
-        <v>123</v>
+      <c r="A41" s="22" t="s">
+        <v>125</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E41" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" ht="12.75" customHeight="1">
+      <c r="A42" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>45</v>
-      </c>
       <c r="D42" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="E42" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" ht="12.75" customHeight="1">
+      <c r="A43" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" ht="12.75" customHeight="1">
+      <c r="A44" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" ht="12.75" customHeight="1">
+      <c r="A45" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F42" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F43" s="22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F44" s="22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" ht="12.75" customHeight="1"/>
+      <c r="D45" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="46" ht="12.75" customHeight="1"/>
     <row r="47" ht="12.75" customHeight="1"/>
     <row r="48" ht="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added Test Cases for HomePage
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="168">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -154,6 +154,12 @@
     <t>nickname=Valir</t>
   </si>
   <si>
+    <t>verifyClickRefresh</t>
+  </si>
+  <si>
+    <t>nickname=Strat</t>
+  </si>
+  <si>
     <t>verifyNotificationBell</t>
   </si>
   <si>
@@ -521,6 +527,12 @@
   </si>
   <si>
     <t>ph.com.globe.mybusiness:id/tv_message</t>
+  </si>
+  <si>
+    <t>txtNotifEmptyResult</t>
+  </si>
+  <si>
+    <t>//android.widget.TextView[@text='Your search is empty.’]</t>
   </si>
 </sst>
 </file>
@@ -2161,7 +2173,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2447,19 +2459,21 @@
       <c r="G15" s="28"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" t="s" s="32">
+      <c r="A16" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="B16" t="s" s="29">
+      <c r="B16" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="C16" t="s" s="29">
+      <c r="D16" t="s" s="26">
         <v>18</v>
       </c>
-      <c r="D16" t="s" s="32">
+      <c r="E16" t="s" s="26">
         <v>44</v>
       </c>
-      <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
     </row>
@@ -2474,7 +2488,7 @@
         <v>18</v>
       </c>
       <c r="D17" t="s" s="32">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
@@ -2482,7 +2496,7 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" t="s" s="32">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s" s="29">
         <v>17</v>
@@ -2490,14 +2504,121 @@
       <c r="C18" t="s" s="29">
         <v>18</v>
       </c>
-      <c r="D18" t="s" s="26">
-        <v>44</v>
-      </c>
-      <c r="E18" t="s" s="26">
-        <v>47</v>
-      </c>
+      <c r="D18" t="s" s="32">
+        <v>46</v>
+      </c>
+      <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" t="s" s="32">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s" s="29">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s" s="29">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s" s="26">
+        <v>49</v>
+      </c>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="32"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="32"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="32"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="32"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="32"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="32"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="32"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="32"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="32"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="32"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2530,1024 +2651,1032 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" t="s" s="26">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s" s="26">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s" s="26">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s" s="26">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s" s="26">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s" s="26">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" t="s" s="26">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s" s="26">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s" s="26">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s" s="26">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" t="s" s="26">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s" s="26">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s" s="26">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s" s="26">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s" s="26">
         <v>61</v>
-      </c>
-      <c r="E3" t="s" s="26">
-        <v>58</v>
-      </c>
-      <c r="F3" t="s" s="26">
-        <v>59</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" t="s" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s" s="29">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s" s="29">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s" s="29">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" t="s" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s" s="29">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s" s="29">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s" s="29">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" t="s" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s" s="29">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s" s="29">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s" s="29">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s" s="29">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" t="s" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s" s="29">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s" s="29">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s" s="29">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s" s="29">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" t="s" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s" s="29">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s" s="29">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s" s="29">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s" s="29">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" t="s" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s" s="29">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s" s="29">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s" s="29">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s" s="29">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" t="s" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s" s="29">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s" s="29">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s" s="29">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s" s="29">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" t="s" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s" s="29">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s" s="29">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s" s="29">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s" s="29">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" t="s" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s" s="29">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s" s="29">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s" s="29">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E12" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s" s="29">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" t="s" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s" s="29">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s" s="29">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s" s="29">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E13" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s" s="29">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" t="s" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s" s="29">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s" s="29">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E14" t="s" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s" s="29">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" t="s" s="32">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s" s="32">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s" s="32">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s" s="32">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s" s="32">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s" s="32">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" t="s" s="26">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s" s="26">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s" s="26">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s" s="34">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" t="s" s="26">
+        <v>87</v>
+      </c>
+      <c r="B17" t="s" s="26">
         <v>85</v>
       </c>
-      <c r="B17" t="s" s="26">
-        <v>83</v>
-      </c>
       <c r="C17" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s" s="26">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E17" t="s" s="35">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F17" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" t="s" s="26">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s" s="26">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s" s="34">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s" s="35">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" t="s" s="26">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s" s="34">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C19" t="s" s="35">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s" s="37">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s" s="38">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" t="s" s="35">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s" s="37">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C20" t="s" s="38">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s" s="37">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E20" t="s" s="38">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F20" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" t="s" s="26">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s" s="39">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C21" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s" s="39">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E21" t="s" s="35">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F21" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" t="s" s="35">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s" s="37">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s" s="38">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s" s="37">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E22" t="s" s="38">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F22" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" t="s" s="26">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s" s="40">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s" s="40">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E23" t="s" s="35">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F23" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" t="s" s="26">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s" s="26">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C24" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s" s="26">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E24" t="s" s="35">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" t="s" s="26">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B25" t="s" s="26">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C25" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s" s="26">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E25" t="s" s="35">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F25" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" t="s" s="26">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s" s="26">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s" s="26">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E26" t="s" s="35">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F26" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" t="s" s="26">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s" s="26">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D27" t="s" s="26">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E27" t="s" s="35">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F27" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" t="s" s="26">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s" s="26">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C28" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s" s="26">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E28" t="s" s="35">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F28" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" t="s" s="26">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s" s="26">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s" s="26">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E29" t="s" s="35">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F29" t="s" s="36">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" t="s" s="26">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s" s="26">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C30" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D30" t="s" s="26">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E30" s="31"/>
       <c r="F30" s="41"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" t="s" s="26">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s" s="26">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D31" t="s" s="26">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E31" s="31"/>
       <c r="F31" s="31"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" t="s" s="26">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B32" t="s" s="26">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C32" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D32" t="s" s="26">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E32" s="31"/>
       <c r="F32" s="31"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" t="s" s="26">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s" s="26">
+        <v>123</v>
+      </c>
+      <c r="C33" t="s" s="26">
+        <v>58</v>
+      </c>
+      <c r="D33" t="s" s="26">
         <v>121</v>
-      </c>
-      <c r="C33" t="s" s="26">
-        <v>56</v>
-      </c>
-      <c r="D33" t="s" s="26">
-        <v>119</v>
       </c>
       <c r="E33" s="31"/>
       <c r="F33" s="31"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" t="s" s="26">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s" s="26">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C34" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D34" t="s" s="26">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E34" s="28"/>
       <c r="F34" s="28"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" t="s" s="26">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s" s="26">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C35" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D35" t="s" s="26">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" t="s" s="26">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B36" t="s" s="26">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C36" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D36" t="s" s="26">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" t="s" s="26">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B37" t="s" s="26">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C37" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D37" t="s" s="26">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" t="s" s="26">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B38" t="s" s="26">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C38" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D38" t="s" s="26">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E38" s="28"/>
       <c r="F38" s="28"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" t="s" s="26">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B39" t="s" s="26">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C39" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D39" t="s" s="26">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E39" s="28"/>
       <c r="F39" s="28"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" t="s" s="26">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B40" t="s" s="26">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C40" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D40" t="s" s="26">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E40" t="s" s="26">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F40" s="31"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" t="s" s="26">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B41" t="s" s="26">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C41" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D41" t="s" s="26">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E41" s="31"/>
       <c r="F41" s="31"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" t="s" s="26">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B42" t="s" s="26">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C42" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D42" t="s" s="26">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E42" s="31"/>
       <c r="F42" s="31"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" t="s" s="26">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B43" t="s" s="26">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C43" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D43" t="s" s="26">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E43" s="31"/>
       <c r="F43" s="31"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" t="s" s="26">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B44" t="s" s="26">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C44" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D44" t="s" s="26">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E44" s="31"/>
       <c r="F44" s="31"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" t="s" s="26">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B45" t="s" s="26">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C45" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D45" t="s" s="26">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E45" s="31"/>
       <c r="F45" s="31"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
       <c r="A46" t="s" s="26">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B46" t="s" s="26">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C46" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D46" t="s" s="26">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E46" s="31"/>
       <c r="F46" s="31"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" t="s" s="26">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B47" t="s" s="26">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C47" t="s" s="26">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D47" t="s" s="26">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E47" s="31"/>
       <c r="F47" s="31"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
+      <c r="A48" t="s" s="26">
+        <v>153</v>
+      </c>
+      <c r="B48" t="s" s="26">
+        <v>154</v>
+      </c>
+      <c r="C48" t="s" s="26">
+        <v>58</v>
+      </c>
+      <c r="D48" t="s" s="26">
+        <v>155</v>
+      </c>
       <c r="E48" s="31"/>
       <c r="F48" s="31"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="A49" s="31"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
+      <c r="A49" t="s" s="26">
+        <v>153</v>
+      </c>
+      <c r="B49" t="s" s="26">
+        <v>156</v>
+      </c>
+      <c r="C49" t="s" s="26">
+        <v>58</v>
+      </c>
+      <c r="D49" t="s" s="26">
+        <v>157</v>
+      </c>
       <c r="E49" s="31"/>
       <c r="F49" s="31"/>
     </row>
     <row r="50" ht="12.75" customHeight="1">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
+      <c r="A50" t="s" s="26">
+        <v>153</v>
+      </c>
+      <c r="B50" t="s" s="26">
+        <v>158</v>
+      </c>
+      <c r="C50" t="s" s="26">
+        <v>58</v>
+      </c>
+      <c r="D50" t="s" s="26">
+        <v>159</v>
+      </c>
       <c r="E50" s="31"/>
       <c r="F50" s="31"/>
     </row>
     <row r="51" ht="12.75" customHeight="1">
-      <c r="A51" s="31"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
+      <c r="A51" t="s" s="26">
+        <v>153</v>
+      </c>
+      <c r="B51" t="s" s="26">
+        <v>160</v>
+      </c>
+      <c r="C51" t="s" s="26">
+        <v>60</v>
+      </c>
+      <c r="D51" t="s" s="26">
+        <v>161</v>
+      </c>
       <c r="E51" s="31"/>
       <c r="F51" s="31"/>
     </row>
     <row r="52" ht="12.75" customHeight="1">
       <c r="A52" t="s" s="26">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B52" t="s" s="26">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C52" t="s" s="26">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D52" t="s" s="26">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="E52" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F52" t="s" s="26">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" ht="12.75" customHeight="1">
       <c r="A53" t="s" s="32">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s" s="32">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C53" t="s" s="32">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D53" t="s" s="32">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="E53" t="s" s="32">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F53" t="s" s="32">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" ht="12.75" customHeight="1">
       <c r="A54" t="s" s="32">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B54" t="s" s="32">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="C54" t="s" s="32">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D54" t="s" s="32">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="E54" t="s" s="32">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F54" t="s" s="32">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" t="s" s="26">
-        <v>151</v>
-      </c>
-      <c r="B55" t="s" s="32">
-        <v>158</v>
-      </c>
-      <c r="C55" t="s" s="26">
-        <v>58</v>
-      </c>
-      <c r="D55" t="s" s="26">
-        <v>159</v>
-      </c>
+      <c r="A55" s="26"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
       <c r="E55" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F55" t="s" s="26">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" t="s" s="26">
-        <v>151</v>
-      </c>
-      <c r="B56" t="s" s="32">
-        <v>160</v>
-      </c>
-      <c r="C56" t="s" s="26">
-        <v>58</v>
-      </c>
-      <c r="D56" t="s" s="32">
-        <v>161</v>
-      </c>
+      <c r="A56" s="26"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="32"/>
       <c r="E56" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F56" t="s" s="26">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" t="s" s="26">
-        <v>151</v>
-      </c>
-      <c r="B57" t="s" s="32">
-        <v>162</v>
-      </c>
-      <c r="C57" t="s" s="26">
-        <v>56</v>
-      </c>
-      <c r="D57" t="s" s="26">
-        <v>163</v>
-      </c>
+      <c r="A57" s="26"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
       <c r="E57" t="s" s="26">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F57" t="s" s="26">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" ht="12.75" customHeight="1">

</xml_diff>

<commit_message>
Added Scripts in HomePage
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="176">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -160,6 +160,24 @@
     <t>nickname=Strat</t>
   </si>
   <si>
+    <t>verifyClickGetMoreData</t>
+  </si>
+  <si>
+    <t>nickname=RealMe</t>
+  </si>
+  <si>
+    <t>verifyClickHamburger</t>
+  </si>
+  <si>
+    <t>nickname=Point</t>
+  </si>
+  <si>
+    <t>verifyClickExpandButtonAnnouncement</t>
+  </si>
+  <si>
+    <t>nickname=Akai</t>
+  </si>
+  <si>
     <t>verifyNotificationBell</t>
   </si>
   <si>
@@ -488,6 +506,12 @@
   </si>
   <si>
     <t>ph.com.globe.mybusiness:id/tv_modem_header</t>
+  </si>
+  <si>
+    <t>btnHamburger</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/drawer</t>
   </si>
   <si>
     <t>NotificationPage</t>
@@ -606,7 +630,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -623,7 +647,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -633,11 +657,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -646,7 +670,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -654,17 +678,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
@@ -681,7 +705,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom/>
@@ -689,12 +713,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -703,59 +738,48 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -763,19 +787,19 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom/>
@@ -783,14 +807,27 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -800,7 +837,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -822,28 +859,28 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -861,20 +898,20 @@
     <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -925,6 +962,12 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -947,8 +990,8 @@
       <rgbColor rgb="015e88b1"/>
       <rgbColor rgb="01eef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
     </indexedColors>
@@ -2015,7 +2058,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2133,16 +2176,19 @@
       <c r="D12" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="E12" s="24"/>
-    </row>
-    <row r="13">
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" ht="13" customHeight="1">
+      <c r="A13" s="7"/>
       <c r="B13" t="s" s="3">
         <v>8</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14">
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" ht="13" customHeight="1">
+      <c r="A14" s="20"/>
       <c r="B14" s="4"/>
       <c r="C14" t="s" s="4">
         <v>5</v>
@@ -2150,6 +2196,7 @@
       <c r="D14" t="s" s="5">
         <v>8</v>
       </c>
+      <c r="E14" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2159,7 +2206,8 @@
   <hyperlinks>
     <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
-    <hyperlink ref="D12" location="'Locators'!R1C1" tooltip="" display="Locators"/>
+    <hyperlink ref="D12" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
+    <hyperlink ref="D14" location="'Locators'!R1C1" tooltip="" display="Locators"/>
     <hyperlink ref="D12" location="'Testdata'!R1C1" tooltip="" display="Testdata"/>
     <hyperlink ref="D14" location="'Locators'!R1C1" tooltip="" display="Locators"/>
   </hyperlinks>
@@ -2173,7 +2221,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2478,82 +2526,112 @@
       <c r="G16" s="28"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" t="s" s="32">
+      <c r="A17" t="s" s="26">
         <v>45</v>
       </c>
-      <c r="B17" t="s" s="29">
+      <c r="B17" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="C17" t="s" s="29">
+      <c r="D17" t="s" s="26">
         <v>18</v>
       </c>
-      <c r="D17" t="s" s="32">
+      <c r="E17" t="s" s="26">
         <v>46</v>
       </c>
-      <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" t="s" s="32">
+      <c r="A18" t="s" s="26">
         <v>47</v>
       </c>
-      <c r="B18" t="s" s="29">
+      <c r="B18" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="C18" t="s" s="29">
+      <c r="D18" t="s" s="26">
         <v>18</v>
       </c>
-      <c r="D18" t="s" s="32">
-        <v>46</v>
-      </c>
-      <c r="E18" s="28"/>
+      <c r="E18" t="s" s="26">
+        <v>48</v>
+      </c>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" t="s" s="32">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s" s="29">
+      <c r="A19" t="s" s="26">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="C19" t="s" s="29">
+      <c r="D19" t="s" s="26">
         <v>18</v>
       </c>
-      <c r="D19" t="s" s="26">
-        <v>46</v>
-      </c>
       <c r="E19" t="s" s="26">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="32"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
+      <c r="A20" t="s" s="32">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s" s="29">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s" s="29">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s" s="32">
+        <v>52</v>
+      </c>
+      <c r="E20" s="28"/>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="32"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
+      <c r="A21" t="s" s="32">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s" s="29">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s" s="29">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s" s="32">
+        <v>52</v>
+      </c>
+      <c r="E21" s="28"/>
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="32"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
+      <c r="A22" t="s" s="32">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s" s="29">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s" s="29">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s" s="26">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s" s="26">
+        <v>55</v>
+      </c>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
     </row>
@@ -2619,6 +2697,33 @@
       <c r="E29" s="26"/>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="32"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="32"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="32"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2634,7 +2739,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2651,1089 +2756,1099 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" t="s" s="26">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s" s="26">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s" s="26">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s" s="26">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s" s="26">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s" s="26">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" t="s" s="26">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s" s="26">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s" s="26">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s" s="26">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s" s="26">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" t="s" s="26">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s" s="26">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s" s="26">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s" s="26">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s" s="26">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s" s="26">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" t="s" s="29">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s" s="29">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s" s="29">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s" s="29">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s" s="29">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s" s="29">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" t="s" s="29">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s" s="29">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s" s="29">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s" s="29">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s" s="29">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s" s="29">
         <v>67</v>
-      </c>
-      <c r="C5" t="s" s="29">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s" s="29">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s" s="29">
-        <v>60</v>
-      </c>
-      <c r="F5" t="s" s="29">
-        <v>61</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" t="s" s="29">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s" s="29">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s" s="29">
         <v>64</v>
       </c>
-      <c r="B6" t="s" s="29">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s" s="29">
-        <v>58</v>
-      </c>
       <c r="D6" t="s" s="29">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s" s="29">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s" s="29">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" t="s" s="29">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s" s="29">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s" s="29">
         <v>64</v>
       </c>
-      <c r="B7" t="s" s="29">
-        <v>71</v>
-      </c>
-      <c r="C7" t="s" s="29">
-        <v>58</v>
-      </c>
       <c r="D7" t="s" s="29">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s" s="29">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s" s="29">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" t="s" s="29">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s" s="29">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s" s="29">
         <v>64</v>
       </c>
-      <c r="B8" t="s" s="29">
-        <v>73</v>
-      </c>
-      <c r="C8" t="s" s="29">
-        <v>58</v>
-      </c>
       <c r="D8" t="s" s="29">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s" s="29">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s" s="29">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" t="s" s="29">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s" s="29">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s" s="29">
         <v>64</v>
       </c>
-      <c r="B9" t="s" s="29">
-        <v>75</v>
-      </c>
-      <c r="C9" t="s" s="29">
-        <v>58</v>
-      </c>
       <c r="D9" t="s" s="29">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s" s="29">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s" s="29">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" t="s" s="29">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s" s="29">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s" s="29">
         <v>64</v>
       </c>
-      <c r="B10" t="s" s="29">
-        <v>77</v>
-      </c>
-      <c r="C10" t="s" s="29">
-        <v>58</v>
-      </c>
       <c r="D10" t="s" s="29">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E10" t="s" s="29">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s" s="29">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" t="s" s="29">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s" s="29">
+        <v>85</v>
+      </c>
+      <c r="C11" t="s" s="29">
         <v>64</v>
       </c>
-      <c r="B11" t="s" s="29">
-        <v>79</v>
-      </c>
-      <c r="C11" t="s" s="29">
-        <v>58</v>
-      </c>
       <c r="D11" t="s" s="29">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s" s="29">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F11" t="s" s="29">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" t="s" s="29">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s" s="29">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s" s="29">
         <v>64</v>
       </c>
-      <c r="B12" t="s" s="29">
-        <v>81</v>
-      </c>
-      <c r="C12" t="s" s="29">
-        <v>58</v>
-      </c>
       <c r="D12" t="s" s="29">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E12" t="s" s="29">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F12" t="s" s="29">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" t="s" s="29">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s" s="29">
+        <v>89</v>
+      </c>
+      <c r="C13" t="s" s="29">
         <v>64</v>
       </c>
-      <c r="B13" t="s" s="29">
-        <v>83</v>
-      </c>
-      <c r="C13" t="s" s="29">
-        <v>58</v>
-      </c>
       <c r="D13" t="s" s="29">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E13" t="s" s="29">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s" s="29">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" t="s" s="29">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s" s="29">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s" s="29">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s" s="29">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s" s="29">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s" s="29">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" t="s" s="32">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s" s="32">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s" s="32">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s" s="32">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E15" t="s" s="32">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F15" t="s" s="32">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" t="s" s="26">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s" s="26">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C16" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s" s="26">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E16" t="s" s="26">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s" s="34">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" t="s" s="26">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s" s="26">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s" s="26">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s" s="26">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E17" t="s" s="35">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F17" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" t="s" s="26">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s" s="26">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s" s="34">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="E18" t="s" s="35">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F18" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" t="s" s="26">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s" s="34">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s" s="35">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s" s="37">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E19" t="s" s="38">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F19" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" t="s" s="35">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B20" t="s" s="37">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s" s="38">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s" s="37">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E20" t="s" s="38">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" t="s" s="26">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s" s="39">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C21" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s" s="39">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E21" t="s" s="35">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F21" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" t="s" s="35">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B22" t="s" s="37">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C22" t="s" s="38">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s" s="37">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s" s="38">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F22" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" t="s" s="26">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s" s="40">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s" s="26">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s" s="40">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E23" t="s" s="35">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F23" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" t="s" s="26">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B24" t="s" s="26">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C24" t="s" s="26">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s" s="26">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E24" t="s" s="35">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F24" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" t="s" s="26">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B25" t="s" s="26">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s" s="26">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s" s="26">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E25" t="s" s="35">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F25" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" t="s" s="26">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B26" t="s" s="26">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C26" t="s" s="26">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D26" t="s" s="26">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E26" t="s" s="35">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F26" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" t="s" s="26">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s" s="26">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s" s="26">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s" s="26">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E27" t="s" s="35">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F27" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" t="s" s="26">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s" s="26">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C28" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s" s="26">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E28" t="s" s="35">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F28" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" t="s" s="26">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s" s="26">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s" s="26">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E29" t="s" s="35">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F29" t="s" s="36">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" t="s" s="26">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B30" t="s" s="26">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s" s="26">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E30" s="31"/>
       <c r="F30" s="41"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" t="s" s="26">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B31" t="s" s="26">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C31" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s" s="26">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E31" s="31"/>
       <c r="F31" s="31"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" t="s" s="26">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B32" t="s" s="26">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C32" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s" s="26">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E32" s="31"/>
       <c r="F32" s="31"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" t="s" s="26">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B33" t="s" s="26">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C33" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s" s="26">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E33" s="31"/>
       <c r="F33" s="31"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" t="s" s="26">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B34" t="s" s="26">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C34" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s" s="26">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="E34" s="28"/>
       <c r="F34" s="28"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" t="s" s="26">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B35" t="s" s="26">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C35" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D35" t="s" s="26">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" t="s" s="26">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B36" t="s" s="26">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C36" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D36" t="s" s="26">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" t="s" s="26">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B37" t="s" s="26">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C37" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D37" t="s" s="26">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" t="s" s="26">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B38" t="s" s="26">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C38" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D38" t="s" s="26">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E38" s="28"/>
       <c r="F38" s="28"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" t="s" s="26">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B39" t="s" s="26">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C39" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D39" t="s" s="26">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E39" s="28"/>
       <c r="F39" s="28"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" t="s" s="26">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s" s="26">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C40" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D40" t="s" s="26">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E40" t="s" s="26">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="F40" s="31"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" t="s" s="26">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B41" t="s" s="26">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C41" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D41" t="s" s="26">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E41" s="31"/>
       <c r="F41" s="31"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" t="s" s="26">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B42" t="s" s="26">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C42" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D42" t="s" s="26">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E42" s="31"/>
       <c r="F42" s="31"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" t="s" s="26">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B43" t="s" s="26">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C43" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D43" t="s" s="26">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E43" s="31"/>
       <c r="F43" s="31"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" t="s" s="26">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B44" t="s" s="26">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C44" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D44" t="s" s="26">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E44" s="31"/>
       <c r="F44" s="31"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" t="s" s="26">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B45" t="s" s="26">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C45" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D45" t="s" s="26">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E45" s="31"/>
       <c r="F45" s="31"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
       <c r="A46" t="s" s="26">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B46" t="s" s="26">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C46" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D46" t="s" s="26">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E46" s="31"/>
       <c r="F46" s="31"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" t="s" s="26">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B47" t="s" s="26">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C47" t="s" s="26">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D47" t="s" s="26">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="E47" s="31"/>
       <c r="F47" s="31"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" t="s" s="26">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s" s="26">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C48" t="s" s="26">
-        <v>58</v>
-      </c>
-      <c r="D48" t="s" s="26">
-        <v>155</v>
-      </c>
-      <c r="E48" s="31"/>
+        <v>64</v>
+      </c>
+      <c r="D48" t="s" s="42">
+        <v>160</v>
+      </c>
+      <c r="E48" t="s" s="43">
+        <v>144</v>
+      </c>
       <c r="F48" s="31"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="A49" t="s" s="26">
-        <v>153</v>
-      </c>
-      <c r="B49" t="s" s="26">
-        <v>156</v>
-      </c>
-      <c r="C49" t="s" s="26">
-        <v>58</v>
-      </c>
-      <c r="D49" t="s" s="26">
-        <v>157</v>
-      </c>
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="40"/>
       <c r="E49" s="31"/>
       <c r="F49" s="31"/>
     </row>
     <row r="50" ht="12.75" customHeight="1">
-      <c r="A50" t="s" s="26">
-        <v>153</v>
-      </c>
-      <c r="B50" t="s" s="26">
-        <v>158</v>
-      </c>
-      <c r="C50" t="s" s="26">
-        <v>58</v>
-      </c>
-      <c r="D50" t="s" s="26">
-        <v>159</v>
-      </c>
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
       <c r="E50" s="31"/>
       <c r="F50" s="31"/>
     </row>
     <row r="51" ht="12.75" customHeight="1">
-      <c r="A51" t="s" s="26">
-        <v>153</v>
-      </c>
-      <c r="B51" t="s" s="26">
-        <v>160</v>
-      </c>
-      <c r="C51" t="s" s="26">
-        <v>60</v>
-      </c>
-      <c r="D51" t="s" s="26">
-        <v>161</v>
-      </c>
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
       <c r="E51" s="31"/>
       <c r="F51" s="31"/>
     </row>
     <row r="52" ht="12.75" customHeight="1">
-      <c r="A52" t="s" s="26">
-        <v>153</v>
-      </c>
-      <c r="B52" t="s" s="26">
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+    </row>
+    <row r="53" ht="12.75" customHeight="1">
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+    </row>
+    <row r="54" ht="12.75" customHeight="1">
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+    </row>
+    <row r="55" ht="12.75" customHeight="1">
+      <c r="A55" t="s" s="26">
+        <v>161</v>
+      </c>
+      <c r="B55" t="s" s="26">
         <v>162</v>
       </c>
-      <c r="C52" t="s" s="26">
-        <v>60</v>
-      </c>
-      <c r="D52" t="s" s="26">
+      <c r="C55" t="s" s="26">
+        <v>64</v>
+      </c>
+      <c r="D55" t="s" s="26">
         <v>163</v>
       </c>
-      <c r="E52" t="s" s="26">
-        <v>60</v>
-      </c>
-      <c r="F52" t="s" s="26">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" t="s" s="32">
-        <v>153</v>
-      </c>
-      <c r="B53" t="s" s="32">
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+    </row>
+    <row r="56" ht="12.75" customHeight="1">
+      <c r="A56" t="s" s="26">
+        <v>161</v>
+      </c>
+      <c r="B56" t="s" s="26">
         <v>164</v>
       </c>
-      <c r="C53" t="s" s="32">
-        <v>58</v>
-      </c>
-      <c r="D53" t="s" s="32">
+      <c r="C56" t="s" s="26">
+        <v>64</v>
+      </c>
+      <c r="D56" t="s" s="26">
         <v>165</v>
       </c>
-      <c r="E53" t="s" s="32">
-        <v>60</v>
-      </c>
-      <c r="F53" t="s" s="32">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" t="s" s="32">
-        <v>153</v>
-      </c>
-      <c r="B54" t="s" s="32">
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+    </row>
+    <row r="57" ht="12.75" customHeight="1">
+      <c r="A57" t="s" s="26">
+        <v>161</v>
+      </c>
+      <c r="B57" t="s" s="26">
         <v>166</v>
       </c>
-      <c r="C54" t="s" s="32">
-        <v>60</v>
-      </c>
-      <c r="D54" t="s" s="32">
+      <c r="C57" t="s" s="26">
+        <v>64</v>
+      </c>
+      <c r="D57" t="s" s="26">
         <v>167</v>
       </c>
-      <c r="E54" t="s" s="32">
-        <v>60</v>
-      </c>
-      <c r="F54" t="s" s="32">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" s="26"/>
-      <c r="B55" s="32"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" t="s" s="26">
-        <v>60</v>
-      </c>
-      <c r="F55" t="s" s="26">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" s="26"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="32"/>
-      <c r="E56" t="s" s="26">
-        <v>60</v>
-      </c>
-      <c r="F56" t="s" s="26">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" s="26"/>
-      <c r="B57" s="32"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" t="s" s="26">
-        <v>60</v>
-      </c>
-      <c r="F57" t="s" s="26">
-        <v>61</v>
-      </c>
+      <c r="E57" s="31"/>
+      <c r="F57" s="31"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
-      <c r="A58" s="31"/>
-      <c r="B58" s="28"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="31"/>
+      <c r="A58" t="s" s="26">
+        <v>161</v>
+      </c>
+      <c r="B58" t="s" s="26">
+        <v>168</v>
+      </c>
+      <c r="C58" t="s" s="26">
+        <v>66</v>
+      </c>
+      <c r="D58" t="s" s="26">
+        <v>169</v>
+      </c>
       <c r="E58" s="31"/>
       <c r="F58" s="31"/>
     </row>
     <row r="59" ht="12.75" customHeight="1">
-      <c r="A59" s="31"/>
-      <c r="B59" s="28"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="31"/>
+      <c r="A59" t="s" s="26">
+        <v>161</v>
+      </c>
+      <c r="B59" t="s" s="26">
+        <v>170</v>
+      </c>
+      <c r="C59" t="s" s="26">
+        <v>66</v>
+      </c>
+      <c r="D59" t="s" s="26">
+        <v>171</v>
+      </c>
+      <c r="E59" t="s" s="26">
+        <v>66</v>
+      </c>
+      <c r="F59" t="s" s="26">
+        <v>67</v>
+      </c>
     </row>
     <row r="60" ht="12.75" customHeight="1">
-      <c r="A60" s="31"/>
-      <c r="B60" s="28"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="31"/>
+      <c r="A60" t="s" s="32">
+        <v>161</v>
+      </c>
+      <c r="B60" t="s" s="32">
+        <v>172</v>
+      </c>
+      <c r="C60" t="s" s="32">
+        <v>64</v>
+      </c>
+      <c r="D60" t="s" s="32">
+        <v>173</v>
+      </c>
+      <c r="E60" t="s" s="32">
+        <v>66</v>
+      </c>
+      <c r="F60" t="s" s="32">
+        <v>67</v>
+      </c>
     </row>
     <row r="61" ht="12.75" customHeight="1">
-      <c r="A61" s="31"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="31"/>
-      <c r="F61" s="31"/>
+      <c r="A61" t="s" s="32">
+        <v>161</v>
+      </c>
+      <c r="B61" t="s" s="32">
+        <v>174</v>
+      </c>
+      <c r="C61" t="s" s="32">
+        <v>66</v>
+      </c>
+      <c r="D61" t="s" s="32">
+        <v>175</v>
+      </c>
+      <c r="E61" t="s" s="32">
+        <v>66</v>
+      </c>
+      <c r="F61" t="s" s="32">
+        <v>67</v>
+      </c>
     </row>
     <row r="62" ht="12.75" customHeight="1">
-      <c r="A62" s="31"/>
-      <c r="B62" s="28"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="31"/>
-      <c r="F62" s="31"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="32"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" t="s" s="26">
+        <v>66</v>
+      </c>
+      <c r="F62" t="s" s="26">
+        <v>67</v>
+      </c>
     </row>
     <row r="63" ht="12.75" customHeight="1">
-      <c r="A63" s="31"/>
-      <c r="B63" s="28"/>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="31"/>
-      <c r="F63" s="31"/>
+      <c r="A63" s="26"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="32"/>
+      <c r="E63" t="s" s="26">
+        <v>66</v>
+      </c>
+      <c r="F63" t="s" s="26">
+        <v>67</v>
+      </c>
     </row>
     <row r="64" ht="12.75" customHeight="1">
-      <c r="A64" s="31"/>
-      <c r="B64" s="28"/>
-      <c r="C64" s="31"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="31"/>
-      <c r="F64" s="31"/>
+      <c r="A64" s="26"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" t="s" s="26">
+        <v>66</v>
+      </c>
+      <c r="F64" t="s" s="26">
+        <v>67</v>
+      </c>
     </row>
     <row r="65" ht="12.75" customHeight="1">
       <c r="A65" s="31"/>
@@ -3862,6 +3977,62 @@
       <c r="D80" s="31"/>
       <c r="E80" s="31"/>
       <c r="F80" s="31"/>
+    </row>
+    <row r="81" ht="12.75" customHeight="1">
+      <c r="A81" s="31"/>
+      <c r="B81" s="28"/>
+      <c r="C81" s="31"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="31"/>
+      <c r="F81" s="31"/>
+    </row>
+    <row r="82" ht="12.75" customHeight="1">
+      <c r="A82" s="31"/>
+      <c r="B82" s="28"/>
+      <c r="C82" s="31"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="31"/>
+      <c r="F82" s="31"/>
+    </row>
+    <row r="83" ht="12.75" customHeight="1">
+      <c r="A83" s="31"/>
+      <c r="B83" s="28"/>
+      <c r="C83" s="31"/>
+      <c r="D83" s="31"/>
+      <c r="E83" s="31"/>
+      <c r="F83" s="31"/>
+    </row>
+    <row r="84" ht="12.75" customHeight="1">
+      <c r="A84" s="31"/>
+      <c r="B84" s="28"/>
+      <c r="C84" s="31"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="31"/>
+      <c r="F84" s="31"/>
+    </row>
+    <row r="85" ht="12.75" customHeight="1">
+      <c r="A85" s="31"/>
+      <c r="B85" s="28"/>
+      <c r="C85" s="31"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="31"/>
+    </row>
+    <row r="86" ht="12.75" customHeight="1">
+      <c r="A86" s="31"/>
+      <c r="B86" s="28"/>
+      <c r="C86" s="31"/>
+      <c r="D86" s="31"/>
+      <c r="E86" s="31"/>
+      <c r="F86" s="31"/>
+    </row>
+    <row r="87" ht="12.75" customHeight="1">
+      <c r="A87" s="31"/>
+      <c r="B87" s="28"/>
+      <c r="C87" s="31"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="31"/>
+      <c r="F87" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Added GetMoreDataPage and VerifyGetMoreData scripts, modified BaseTestcase
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhI1WoFBn/GUxkm7Rp3typR9pznCQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhjgHCz5BEw242x+4ppiaPdnOdisg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="221">
   <si>
     <t>TCName</t>
   </si>
@@ -109,16 +109,40 @@
     <t>nickname=Libertea</t>
   </si>
   <si>
+    <t>verifyClickRefresh</t>
+  </si>
+  <si>
+    <t>nickname=Valir</t>
+  </si>
+  <si>
+    <t>verifyNotificationBell</t>
+  </si>
+  <si>
+    <t>nickname=Gloo</t>
+  </si>
+  <si>
     <t>verifyClickAddModem</t>
   </si>
   <si>
-    <t>nickname=Valir</t>
-  </si>
-  <si>
-    <t>verifyNotificationBell</t>
-  </si>
-  <si>
-    <t>nickname=Gloo</t>
+    <t>nickname=Moana</t>
+  </si>
+  <si>
+    <t>verifyClickHamburger</t>
+  </si>
+  <si>
+    <t>nickname=Asus</t>
+  </si>
+  <si>
+    <t>verifyClickGetMoreData</t>
+  </si>
+  <si>
+    <t>nickname=Mcgee</t>
+  </si>
+  <si>
+    <t>verifyClickExpandButtonAnnouncement</t>
+  </si>
+  <si>
+    <t>nickname=Lebron</t>
   </si>
   <si>
     <t>verifyNotificationPage</t>
@@ -145,6 +169,48 @@
     <t>emptyResultsMsg=Your search is empty.</t>
   </si>
   <si>
+    <t>verifyGetMoreDataPromosPage</t>
+  </si>
+  <si>
+    <t>spiel=Introducing the all-new myBizSURF promos specifically designed for your Prepaid Internet device</t>
+  </si>
+  <si>
+    <t>dataDesc1=myBizSurf 199</t>
+  </si>
+  <si>
+    <t>dataDesc2=myBizSurf 599</t>
+  </si>
+  <si>
+    <t>dataDesc3=myBizSurf 799</t>
+  </si>
+  <si>
+    <t>dataDesc4=myBizSurf 999</t>
+  </si>
+  <si>
+    <t>dataDesc5=myBizSurf 1499</t>
+  </si>
+  <si>
+    <t>verifyGetMoreDataAddOnsPage</t>
+  </si>
+  <si>
+    <t>spielNoSubs=You need to have an active subscription of any myBizSurf promos to purchase add-ons.</t>
+  </si>
+  <si>
+    <t>verifyAccountDetailsPage</t>
+  </si>
+  <si>
+    <t>nickname=Kanex</t>
+  </si>
+  <si>
+    <t>text1=Account Details</t>
+  </si>
+  <si>
+    <t>lblPrepaidNumber=Prepaid Internet Number</t>
+  </si>
+  <si>
+    <t>prepNumber=0927 108 0510</t>
+  </si>
+  <si>
     <t>Page</t>
   </si>
   <si>
@@ -451,6 +517,12 @@
     <t>ph.com.globe.mybusiness:id/tv_modem_header</t>
   </si>
   <si>
+    <t>btnHamburger</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/drawer</t>
+  </si>
+  <si>
     <t>NotificationPage</t>
   </si>
   <si>
@@ -494,17 +566,135 @@
   </si>
   <si>
     <t>//android.widget.TextView[@text='Your search is empty.']</t>
+  </si>
+  <si>
+    <t>GetMoreDataPage</t>
+  </si>
+  <si>
+    <t>hdrGetMoreData</t>
+  </si>
+  <si>
+    <t>//android.widget.TextView[@text='Get more data']</t>
+  </si>
+  <si>
+    <t>spielGetMoreData</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/tv_header</t>
+  </si>
+  <si>
+    <t>btnSubscribe</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/btn_prepaid_data</t>
+  </si>
+  <si>
+    <t>lblPromoDataDesc1</t>
+  </si>
+  <si>
+    <t>//android.widget.TextView[@text='myBizSurf 199']</t>
+  </si>
+  <si>
+    <t>lblPromoDataDesc2</t>
+  </si>
+  <si>
+    <t>//android.widget.TextView[@text='myBizSurf 599']</t>
+  </si>
+  <si>
+    <t>lblPromoDataDesc3</t>
+  </si>
+  <si>
+    <t>//android.widget.TextView[@text='myBizSurf 799']</t>
+  </si>
+  <si>
+    <t>lblPromoDataDesc4</t>
+  </si>
+  <si>
+    <t>//android.widget.TextView[@text='myBizSurf 999']</t>
+  </si>
+  <si>
+    <t>lblPromoDataDesc5</t>
+  </si>
+  <si>
+    <t>//android.widget.TextView[@text='myBizSurf 1499']</t>
+  </si>
+  <si>
+    <t>btnAddOns</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/tv_promos_tackon</t>
+  </si>
+  <si>
+    <t>spielGetMoreDataAddOns</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/tv_header_tackons</t>
+  </si>
+  <si>
+    <t>AccountDetailsPage</t>
+  </si>
+  <si>
+    <t>lnkAccountDetails</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/nav_account_details</t>
+  </si>
+  <si>
+    <t>lblNickname</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/sptxt_account_details_nickname</t>
+  </si>
+  <si>
+    <t>txtTitle</t>
+  </si>
+  <si>
+    <t>iconCamera</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/img_account_details_camera</t>
+  </si>
+  <si>
+    <t>accntImg</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/cimg_account_details_image</t>
+  </si>
+  <si>
+    <t>btnHamburgerAP</t>
+  </si>
+  <si>
+    <t>editNicknameLink</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/sptxt_account_details_edit_nickname</t>
+  </si>
+  <si>
+    <t>lblPrepaidInternetNumber</t>
+  </si>
+  <si>
+    <t>//android.widget.TextView[@text='Prepaid Internet Number']</t>
+  </si>
+  <si>
+    <t>prepaidNumber</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/tv_prepaid_number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -523,6 +713,8 @@
     </font>
     <font>
       <sz val="9.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -533,8 +725,7 @@
     </font>
     <font/>
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -557,45 +748,48 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -605,27 +799,30 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -853,8 +1050,11 @@
     <col customWidth="1" min="2" max="2" width="32.29"/>
     <col customWidth="1" min="3" max="3" width="31.57"/>
     <col customWidth="1" min="4" max="4" width="23.71"/>
-    <col customWidth="1" min="5" max="5" width="24.29"/>
-    <col customWidth="1" min="6" max="6" width="15.0"/>
+    <col customWidth="1" min="5" max="5" width="32.86"/>
+    <col customWidth="1" min="6" max="6" width="35.71"/>
+    <col customWidth="1" min="7" max="7" width="23.57"/>
+    <col customWidth="1" min="8" max="9" width="21.14"/>
+    <col customWidth="1" min="10" max="10" width="22.14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -919,277 +1119,370 @@
       <c r="G4" s="8"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="C12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="D12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="C13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="C14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="D14" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="14" t="s">
+      <c r="B15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="D15" s="17" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>35</v>
+      <c r="D17" s="18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>38</v>
+      <c r="D18" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="17" t="s">
+      <c r="D19" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1"/>
     <row r="30" ht="15.75" customHeight="1"/>
@@ -2166,6 +2459,12 @@
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
     <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
+    <row r="1007" ht="15.75" customHeight="1"/>
+    <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:G1"/>
@@ -2188,7 +2487,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="21.43"/>
-    <col customWidth="1" min="2" max="2" width="19.0"/>
+    <col customWidth="1" min="2" max="2" width="21.57"/>
     <col customWidth="1" min="3" max="3" width="19.29"/>
     <col customWidth="1" min="4" max="4" width="83.86"/>
     <col customWidth="1" min="5" max="5" width="21.29"/>
@@ -2197,1105 +2496,1421 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>47</v>
+      <c r="A1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>53</v>
+      <c r="A2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>53</v>
+      <c r="A3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>53</v>
+      <c r="A15" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>53</v>
+      <c r="A16" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>53</v>
+      <c r="A17" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>53</v>
+      <c r="A18" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>53</v>
+      <c r="A19" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>53</v>
+      <c r="A20" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>53</v>
+      <c r="A21" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>53</v>
+      <c r="A22" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>53</v>
+      <c r="A23" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>53</v>
+      <c r="A24" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>53</v>
+      <c r="A25" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>53</v>
+      <c r="A26" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>53</v>
+      <c r="A27" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>53</v>
+      <c r="A28" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="22" t="s">
-        <v>53</v>
+      <c r="A29" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>53</v>
+      <c r="A30" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F31" s="22" t="s">
-        <v>53</v>
+      <c r="A31" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F32" s="22" t="s">
-        <v>53</v>
+      <c r="A32" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F33" s="22" t="s">
-        <v>53</v>
+      <c r="A33" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>53</v>
+      <c r="A34" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>53</v>
+      <c r="A35" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>53</v>
+      <c r="A36" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>53</v>
+      <c r="A37" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>53</v>
+      <c r="A38" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="15" t="s">
+      <c r="A39" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>53</v>
+      <c r="C39" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F40" s="22" t="s">
-        <v>53</v>
+      <c r="A40" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F41" s="22" t="s">
-        <v>53</v>
+      <c r="A41" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F42" s="22" t="s">
-        <v>53</v>
+      <c r="A42" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F43" s="22" t="s">
-        <v>53</v>
+      <c r="A43" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F44" s="22" t="s">
-        <v>53</v>
+      <c r="A44" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="45" ht="12.75" customHeight="1">
-      <c r="A45" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F45" s="22" t="s">
-        <v>53</v>
+      <c r="A45" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F45" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F46" s="22" t="s">
-        <v>53</v>
+      <c r="A46" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="47" ht="12.75" customHeight="1">
-      <c r="A47" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B47" s="15" t="s">
+      <c r="A47" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F47" s="22" t="s">
-        <v>53</v>
+      <c r="B47" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="48" ht="12.75" customHeight="1">
-      <c r="A48" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B48" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="C48" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D48" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>53</v>
-      </c>
+      <c r="A48" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E48" s="9"/>
+      <c r="F48" s="23"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="A49" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="E49" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="F49" s="23" t="s">
-        <v>53</v>
+      <c r="A49" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="50" ht="12.75" customHeight="1">
-      <c r="A50" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E50" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="F50" s="23" t="s">
-        <v>53</v>
+      <c r="A50" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" s="20" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="51" ht="12.75" customHeight="1">
-      <c r="A51" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C51" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F51" s="17" t="s">
-        <v>53</v>
+      <c r="A51" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="52" ht="12.75" customHeight="1">
-      <c r="A52" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="E52" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F52" s="17" t="s">
-        <v>53</v>
+      <c r="A52" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D53" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="E53" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F53" s="17" t="s">
-        <v>53</v>
+      <c r="A53" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="E53" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B54" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="C54" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="E54" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" ht="12.75" customHeight="1"/>
-    <row r="56" ht="12.75" customHeight="1"/>
-    <row r="57" ht="12.75" customHeight="1"/>
-    <row r="58" ht="12.75" customHeight="1"/>
-    <row r="59" ht="12.75" customHeight="1"/>
-    <row r="60" ht="12.75" customHeight="1"/>
-    <row r="61" ht="12.75" customHeight="1"/>
-    <row r="62" ht="12.75" customHeight="1"/>
-    <row r="63" ht="12.75" customHeight="1"/>
-    <row r="64" ht="12.75" customHeight="1"/>
-    <row r="65" ht="12.75" customHeight="1"/>
-    <row r="66" ht="12.75" customHeight="1"/>
-    <row r="67" ht="12.75" customHeight="1"/>
-    <row r="68" ht="12.75" customHeight="1"/>
-    <row r="69" ht="12.75" customHeight="1"/>
-    <row r="70" ht="12.75" customHeight="1"/>
-    <row r="71" ht="12.75" customHeight="1"/>
-    <row r="72" ht="12.75" customHeight="1"/>
-    <row r="73" ht="12.75" customHeight="1"/>
-    <row r="74" ht="12.75" customHeight="1"/>
+      <c r="A54" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F54" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" ht="12.75" customHeight="1">
+      <c r="A55" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" ht="12.75" customHeight="1">
+      <c r="A56" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F56" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" ht="12.75" customHeight="1">
+      <c r="A57" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F57" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" ht="12.75" customHeight="1">
+      <c r="A58" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" ht="12.75" customHeight="1">
+      <c r="A59" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" ht="12.75" customHeight="1">
+      <c r="A60" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" ht="12.75" customHeight="1">
+      <c r="A61" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C61" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" ht="12.75" customHeight="1">
+      <c r="A62" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C62" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="E62" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F62" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" ht="12.75" customHeight="1">
+      <c r="A63" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E63" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F63" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" ht="12.75" customHeight="1">
+      <c r="A64" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" ht="12.75" customHeight="1">
+      <c r="A65" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="66" ht="12.75" customHeight="1">
+      <c r="A66" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="67" ht="12.75" customHeight="1">
+      <c r="A67" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="68" ht="12.75" customHeight="1">
+      <c r="A68" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" ht="12.75" customHeight="1">
+      <c r="A69" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D69" s="16" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="70" ht="12.75" customHeight="1">
+      <c r="A70" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C70" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D70" s="16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="71" ht="12.75" customHeight="1">
+      <c r="A71" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="72" ht="12.75" customHeight="1">
+      <c r="A72" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D72" s="16" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="73" ht="12.75" customHeight="1">
+      <c r="A73" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B73" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D73" s="16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="74" ht="12.75" customHeight="1">
+      <c r="A74" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C74" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D74" s="16" t="s">
+        <v>220</v>
+      </c>
+    </row>
     <row r="75" ht="12.75" customHeight="1"/>
     <row r="76" ht="12.75" customHeight="1"/>
     <row r="77" ht="12.75" customHeight="1"/>
@@ -4243,6 +4858,17 @@
     <row r="1019" ht="12.75" customHeight="1"/>
     <row r="1020" ht="12.75" customHeight="1"/>
     <row r="1021" ht="12.75" customHeight="1"/>
+    <row r="1022" ht="12.75" customHeight="1"/>
+    <row r="1023" ht="12.75" customHeight="1"/>
+    <row r="1024" ht="12.75" customHeight="1"/>
+    <row r="1025" ht="12.75" customHeight="1"/>
+    <row r="1026" ht="12.75" customHeight="1"/>
+    <row r="1027" ht="12.75" customHeight="1"/>
+    <row r="1028" ht="12.75" customHeight="1"/>
+    <row r="1029" ht="12.75" customHeight="1"/>
+    <row r="1030" ht="12.75" customHeight="1"/>
+    <row r="1031" ht="12.75" customHeight="1"/>
+    <row r="1032" ht="12.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Added Scripts for MyProfilePage
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="392">
   <si>
     <t>TCName</t>
   </si>
@@ -379,6 +379,15 @@
     <t>nickname=Kanex6</t>
   </si>
   <si>
+    <t>personalInfoLbl=Personal Information</t>
+  </si>
+  <si>
+    <t>businessInfoLbl=Business Information</t>
+  </si>
+  <si>
+    <t>btnLbl=EDIT MY PROFILE</t>
+  </si>
+  <si>
     <t>Page</t>
   </si>
   <si>
@@ -1163,6 +1172,27 @@
   </si>
   <si>
     <t>ph.com.globe.mybusiness:id/pb_account_details_done</t>
+  </si>
+  <si>
+    <t>MyProfilePage</t>
+  </si>
+  <si>
+    <t>personalInfoLbl</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/tv_kyc_personal</t>
+  </si>
+  <si>
+    <t>businessInfoLbl</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/tv_kyc_business</t>
+  </si>
+  <si>
+    <t>btnEditProfile</t>
+  </si>
+  <si>
+    <t>ph.com.globe.mybusiness:id/btn_manipulate_profile</t>
   </si>
 </sst>
 </file>
@@ -1199,11 +1229,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
@@ -1229,7 +1259,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1282,26 +1312,26 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1311,9 +1341,6 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -1541,7 +1568,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="31.14"/>
     <col customWidth="1" min="2" max="2" width="32.29"/>
-    <col customWidth="1" min="3" max="3" width="31.57"/>
+    <col customWidth="1" min="3" max="3" width="45.29"/>
     <col customWidth="1" min="4" max="4" width="23.71"/>
     <col customWidth="1" min="5" max="5" width="32.86"/>
     <col customWidth="1" min="6" max="6" width="35.71"/>
@@ -2689,13 +2716,13 @@
       <c r="H29" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="I29" s="22" t="s">
+      <c r="I29" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="J29" s="22" t="s">
+      <c r="J29" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="K29" s="22" t="s">
+      <c r="K29" s="14" t="s">
         <v>113</v>
       </c>
       <c r="L29" s="3"/>
@@ -2718,7 +2745,7 @@
       <c r="AD29" s="3"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="14" t="s">
         <v>114</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -2727,7 +2754,7 @@
       <c r="C30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="22" t="s">
         <v>115</v>
       </c>
       <c r="E30" s="14" t="s">
@@ -2769,7 +2796,7 @@
       <c r="AD30" s="3"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="14" t="s">
         <v>116</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -2778,7 +2805,7 @@
       <c r="C31" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="22" t="s">
         <v>117</v>
       </c>
       <c r="E31" s="14" t="s">
@@ -2820,7 +2847,7 @@
       <c r="AD31" s="3"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="23" t="s">
         <v>118</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -2829,7 +2856,7 @@
       <c r="C32" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="22" t="s">
         <v>119</v>
       </c>
       <c r="E32" s="14" t="s">
@@ -2850,25 +2877,31 @@
       <c r="J32" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="24"/>
-      <c r="S32" s="24"/>
-      <c r="T32" s="24"/>
-      <c r="U32" s="24"/>
-      <c r="V32" s="24"/>
-      <c r="W32" s="24"/>
-      <c r="X32" s="24"/>
-      <c r="Y32" s="24"/>
-      <c r="AA32" s="24"/>
-      <c r="AB32" s="24"/>
-      <c r="AC32" s="24"/>
-      <c r="AD32" s="24"/>
+      <c r="K32" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="L32" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="M32" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="3"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="K33" s="3"/>
@@ -23440,2613 +23473,2652 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="25" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="25" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="25" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F25" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F27" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F29" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F30" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F32" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="11" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F33" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="14" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="14" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F35" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F36" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F37" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F40" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F41" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F42" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F43" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F44" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F45" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" ht="12.75" customHeight="1">
       <c r="A46" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F46" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F47" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="26"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
       <c r="A49" s="17" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" ht="12.75" customHeight="1">
       <c r="A50" s="17" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" ht="12.75" customHeight="1">
       <c r="A51" s="17" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" ht="12.75" customHeight="1">
       <c r="A52" s="17" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F52" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" ht="12.75" customHeight="1">
       <c r="A53" s="17" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" ht="12.75" customHeight="1">
       <c r="A54" s="17" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E54" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" ht="12.75" customHeight="1">
       <c r="A55" s="17" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" ht="12.75" customHeight="1">
       <c r="A56" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E56" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" ht="12.75" customHeight="1">
       <c r="A57" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E57" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" ht="12.75" customHeight="1">
       <c r="A58" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" ht="12.75" customHeight="1">
       <c r="A59" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E59" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" ht="12.75" customHeight="1">
       <c r="A60" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E60" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" ht="12.75" customHeight="1">
       <c r="A61" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E61" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F61" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" ht="12.75" customHeight="1">
       <c r="A62" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="E62" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" ht="12.75" customHeight="1">
       <c r="A63" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" ht="12.75" customHeight="1">
       <c r="A64" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" ht="12.75" customHeight="1">
       <c r="A65" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" ht="12.75" customHeight="1">
       <c r="A66" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="E66" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="67" ht="12.75" customHeight="1">
       <c r="A67" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E67" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" ht="12.75" customHeight="1">
       <c r="A68" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="E68" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" ht="12.75" customHeight="1">
       <c r="A69" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E69" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" ht="12.75" customHeight="1">
       <c r="A70" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E70" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" ht="12.75" customHeight="1">
       <c r="A71" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="E71" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" ht="12.75" customHeight="1">
       <c r="A72" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" ht="12.75" customHeight="1">
       <c r="A73" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" ht="12.75" customHeight="1">
       <c r="A74" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E74" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75" ht="12.75" customHeight="1">
       <c r="A75" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E75" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" ht="12.75" customHeight="1">
       <c r="A76" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E76" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="77" ht="12.75" customHeight="1">
       <c r="A77" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E77" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F77" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" ht="12.75" customHeight="1">
       <c r="A78" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E78" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F78" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" ht="12.75" customHeight="1">
       <c r="A79" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="E79" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F79" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="80" ht="12.75" customHeight="1">
       <c r="A80" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E80" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F80" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" ht="12.75" customHeight="1">
       <c r="A81" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E81" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="82" ht="12.75" customHeight="1">
       <c r="A82" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E82" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" ht="12.75" customHeight="1">
       <c r="A83" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="E83" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" ht="12.75" customHeight="1">
       <c r="A84" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="E84" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="85" ht="12.75" customHeight="1">
       <c r="A85" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="E85" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F85" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="86" ht="12.75" customHeight="1">
       <c r="A86" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="E86" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="87" ht="12.75" customHeight="1">
       <c r="A87" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E87" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F87" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="88" ht="12.75" customHeight="1">
       <c r="A88" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E88" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F88" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="89" ht="12.75" customHeight="1">
       <c r="A89" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="E89" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90" ht="12.75" customHeight="1">
       <c r="A90" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E90" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F90" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="91" ht="12.75" customHeight="1">
       <c r="A91" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E91" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F91" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="92" ht="12.75" customHeight="1">
       <c r="A92" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E92" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F92" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="93" ht="12.75" customHeight="1">
       <c r="A93" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" ht="12.75" customHeight="1">
       <c r="A94" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="E94" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F94" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="95" ht="12.75" customHeight="1">
       <c r="A95" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E95" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F95" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="96" ht="12.75" customHeight="1">
       <c r="A96" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="E96" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F96" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="97" ht="12.75" customHeight="1">
       <c r="A97" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E97" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="98" ht="12.75" customHeight="1">
       <c r="A98" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E98" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="99" ht="12.75" customHeight="1">
       <c r="A99" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E99" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="100" ht="12.75" customHeight="1">
       <c r="A100" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="E100" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F100" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="101" ht="12.75" customHeight="1">
       <c r="A101" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E101" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F101" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="102" ht="12.75" customHeight="1">
-      <c r="A102" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="B102" s="22" t="s">
-        <v>322</v>
-      </c>
-      <c r="C102" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="D102" s="22" t="s">
-        <v>323</v>
-      </c>
-      <c r="E102" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="F102" s="28" t="s">
-        <v>131</v>
+      <c r="A102" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C102" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="E102" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F102" s="17" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="103" ht="12.75" customHeight="1">
-      <c r="A103" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="B103" s="22" t="s">
-        <v>324</v>
-      </c>
-      <c r="C103" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="D103" s="22" t="s">
-        <v>325</v>
-      </c>
-      <c r="E103" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="F103" s="28" t="s">
-        <v>131</v>
+      <c r="A103" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="C103" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="E103" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F103" s="17" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="104" ht="12.75" customHeight="1">
-      <c r="A104" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="B104" s="22" t="s">
-        <v>326</v>
-      </c>
-      <c r="C104" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="D104" s="22" t="s">
-        <v>327</v>
-      </c>
-      <c r="E104" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="F104" s="28" t="s">
-        <v>131</v>
+      <c r="A104" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="C104" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="E104" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F104" s="17" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="105" ht="12.75" customHeight="1">
-      <c r="A105" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="B105" s="22" t="s">
-        <v>328</v>
-      </c>
-      <c r="C105" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="D105" s="22" t="s">
-        <v>329</v>
-      </c>
-      <c r="E105" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="F105" s="28" t="s">
-        <v>131</v>
+      <c r="A105" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="C105" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D105" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="E105" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F105" s="17" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="106" ht="12.75" customHeight="1">
-      <c r="A106" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="B106" s="22" t="s">
-        <v>330</v>
-      </c>
-      <c r="C106" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="D106" s="22" t="s">
-        <v>331</v>
-      </c>
-      <c r="E106" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="F106" s="28" t="s">
-        <v>131</v>
+      <c r="A106" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="C106" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D106" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="E106" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F106" s="17" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="107" ht="12.75" customHeight="1">
       <c r="A107" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="E107" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F107" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="108" ht="12.75" customHeight="1">
       <c r="A108" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F108" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="109" ht="12.75" customHeight="1">
       <c r="A109" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E109" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F109" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="110" ht="12.75" customHeight="1">
       <c r="A110" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D110" s="14" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E110" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F110" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="111" ht="12.75" customHeight="1">
       <c r="A111" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E111" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F111" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="112" ht="12.75" customHeight="1">
       <c r="A112" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D112" s="14" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="E112" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F112" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="113" ht="12.75" customHeight="1">
       <c r="A113" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="E113" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F113" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="114" ht="12.75" customHeight="1">
       <c r="A114" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="E114" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F114" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="115" ht="12.75" customHeight="1">
       <c r="A115" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="E115" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F115" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="116" ht="12.75" customHeight="1">
       <c r="A116" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D116" s="14" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="E116" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F116" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="117" ht="12.75" customHeight="1">
       <c r="A117" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E117" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F117" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="118" ht="12.75" customHeight="1">
       <c r="A118" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D118" s="14" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E118" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F118" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="119" ht="12.75" customHeight="1">
+      <c r="A119" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="C119" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D119" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="E119" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F119" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="120" ht="12.75" customHeight="1">
+      <c r="A120" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C120" s="14" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="119" ht="12.75" customHeight="1">
-      <c r="A119" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="B119" s="22" t="s">
-        <v>351</v>
-      </c>
-      <c r="C119" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="D119" s="22" t="s">
-        <v>352</v>
-      </c>
-      <c r="E119" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="F119" s="17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="120" ht="12.75" customHeight="1">
-      <c r="A120" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="B120" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="C120" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="D120" s="22" t="s">
-        <v>200</v>
+      <c r="D120" s="14" t="s">
+        <v>203</v>
       </c>
       <c r="E120" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F120" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="121" ht="12.75" customHeight="1">
       <c r="A121" s="14" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D121" s="14" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="122" ht="12.75" customHeight="1">
       <c r="A122" s="14" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D122" s="14" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="123" ht="12.75" customHeight="1">
       <c r="A123" s="14" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D123" s="14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="124" ht="12.75" customHeight="1">
       <c r="A124" s="14" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="125" ht="12.75" customHeight="1">
       <c r="A125" s="14" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D125" s="14" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="126" ht="12.75" customHeight="1">
       <c r="A126" s="14" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D126" s="14" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="127" ht="12.75" customHeight="1">
       <c r="A127" s="14" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D127" s="14" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="128" ht="12.75" customHeight="1">
       <c r="A128" s="14" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="129" ht="12.75" customHeight="1">
       <c r="A129" s="14" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D129" s="14" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="130" ht="12.75" customHeight="1">
       <c r="A130" s="14" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D130" s="14" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="131" ht="12.75" customHeight="1">
       <c r="A131" s="14" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D131" s="14" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="132" ht="12.75" customHeight="1">
-      <c r="A132" s="29" t="s">
-        <v>354</v>
+      <c r="A132" s="28" t="s">
+        <v>357</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D132" s="14" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="133" ht="12.75" customHeight="1">
-      <c r="A133" s="29" t="s">
-        <v>354</v>
+      <c r="A133" s="28" t="s">
+        <v>357</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D133" s="14" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="134" ht="12.75" customHeight="1">
-      <c r="A134" s="29" t="s">
-        <v>354</v>
-      </c>
-      <c r="B134" s="22" t="s">
-        <v>378</v>
+      <c r="A134" s="28" t="s">
+        <v>357</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="C134" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D134" s="14" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="135" ht="12.75" customHeight="1">
-      <c r="A135" s="29" t="s">
-        <v>354</v>
+      <c r="A135" s="28" t="s">
+        <v>357</v>
       </c>
       <c r="B135" s="14" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C135" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D135" s="14" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="136" ht="12.75" customHeight="1"/>
-    <row r="137" ht="12.75" customHeight="1"/>
-    <row r="138" ht="12.75" customHeight="1"/>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="136" ht="12.75" customHeight="1">
+      <c r="A136" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="B136" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C136" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D136" s="14" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="137" ht="12.75" customHeight="1">
+      <c r="A137" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="B137" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C137" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D137" s="14" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="138" ht="12.75" customHeight="1">
+      <c r="A138" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="B138" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="C138" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D138" s="14" t="s">
+        <v>391</v>
+      </c>
+    </row>
     <row r="139" ht="12.75" customHeight="1"/>
     <row r="140" ht="12.75" customHeight="1"/>
     <row r="141" ht="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
Upload Photo Test Case Completed (Need for Improvement)
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mig1qZzkGbIIvm8yyVqFrHJdKiBWQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mjDZ2GtIAgnn9x9Q3RpzIez68DtHA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1799" uniqueCount="658">
   <si>
     <t>TCName</t>
   </si>
@@ -1447,6 +1447,24 @@
     <t>ph.com.globe.mybusiness:id/pb_account_details_done</t>
   </si>
   <si>
+    <t>photoObj</t>
+  </si>
+  <si>
+    <t>com.google.android.apps.photos:id/image</t>
+  </si>
+  <si>
+    <t>allowBtn</t>
+  </si>
+  <si>
+    <t>com.android.permissioncontroller:id/permission_allow_button</t>
+  </si>
+  <si>
+    <t>specificPhotoObj</t>
+  </si>
+  <si>
+    <t>//android.view.ViewGroup[@content-desc="Photo taken on May 27, 2021 2:16:16 PM"]</t>
+  </si>
+  <si>
     <t>MyProfilePage</t>
   </si>
   <si>
@@ -72309,76 +72327,64 @@
       </c>
     </row>
     <row r="137" ht="12.75" customHeight="1">
-      <c r="A137" s="50" t="s">
+      <c r="A137" s="53" t="s">
+        <v>446</v>
+      </c>
+      <c r="B137" s="52" t="s">
         <v>476</v>
       </c>
-      <c r="B137" s="50" t="s">
+      <c r="C137" s="52" t="s">
+        <v>220</v>
+      </c>
+      <c r="D137" s="52" t="s">
         <v>477</v>
       </c>
-      <c r="C137" s="50" t="s">
+      <c r="E137" s="51"/>
+      <c r="F137" s="51"/>
+    </row>
+    <row r="138" ht="12.75" customHeight="1">
+      <c r="A138" s="53" t="s">
+        <v>446</v>
+      </c>
+      <c r="B138" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="C138" s="52" t="s">
         <v>220</v>
       </c>
-      <c r="D137" s="50" t="s">
-        <v>478</v>
-      </c>
-      <c r="E137" s="51" t="s">
+      <c r="D138" s="52" t="s">
+        <v>479</v>
+      </c>
+      <c r="E138" s="51"/>
+      <c r="F138" s="51"/>
+    </row>
+    <row r="139" ht="12.75" customHeight="1">
+      <c r="A139" s="53" t="s">
+        <v>446</v>
+      </c>
+      <c r="B139" s="52" t="s">
+        <v>480</v>
+      </c>
+      <c r="C139" s="52" t="s">
         <v>222</v>
       </c>
-      <c r="F137" s="51" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="138" ht="12.75" customHeight="1">
-      <c r="A138" s="50" t="s">
-        <v>476</v>
-      </c>
-      <c r="B138" s="50" t="s">
-        <v>479</v>
-      </c>
-      <c r="C138" s="50" t="s">
-        <v>220</v>
-      </c>
-      <c r="D138" s="50" t="s">
-        <v>480</v>
-      </c>
-      <c r="E138" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="F138" s="51" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="139" ht="12.75" customHeight="1">
-      <c r="A139" s="50" t="s">
-        <v>476</v>
-      </c>
-      <c r="B139" s="50" t="s">
+      <c r="D139" s="52" t="s">
         <v>481</v>
       </c>
-      <c r="C139" s="50" t="s">
-        <v>220</v>
-      </c>
-      <c r="D139" s="50" t="s">
-        <v>482</v>
-      </c>
-      <c r="E139" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="F139" s="51" t="s">
-        <v>223</v>
-      </c>
+      <c r="E139" s="51"/>
+      <c r="F139" s="51"/>
     </row>
     <row r="140" ht="12.75" customHeight="1">
       <c r="A140" s="50" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B140" s="50" t="s">
         <v>483</v>
       </c>
       <c r="C140" s="50" t="s">
-        <v>222</v>
-      </c>
-      <c r="D140" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="D140" s="52" t="s">
         <v>484</v>
       </c>
       <c r="E140" s="51" t="s">
@@ -72390,7 +72396,7 @@
     </row>
     <row r="141" ht="12.75" customHeight="1">
       <c r="A141" s="50" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B141" s="50" t="s">
         <v>485</v>
@@ -72410,13 +72416,13 @@
     </row>
     <row r="142" ht="12.75" customHeight="1">
       <c r="A142" s="50" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B142" s="50" t="s">
         <v>487</v>
       </c>
       <c r="C142" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D142" s="50" t="s">
         <v>488</v>
@@ -72430,13 +72436,13 @@
     </row>
     <row r="143" ht="12.75" customHeight="1">
       <c r="A143" s="50" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B143" s="50" t="s">
         <v>489</v>
       </c>
       <c r="C143" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D143" s="50" t="s">
         <v>490</v>
@@ -72450,13 +72456,13 @@
     </row>
     <row r="144" ht="12.75" customHeight="1">
       <c r="A144" s="50" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B144" s="50" t="s">
         <v>491</v>
       </c>
       <c r="C144" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D144" s="50" t="s">
         <v>492</v>
@@ -72470,13 +72476,13 @@
     </row>
     <row r="145" ht="12.75" customHeight="1">
       <c r="A145" s="50" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B145" s="50" t="s">
         <v>493</v>
       </c>
       <c r="C145" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D145" s="50" t="s">
         <v>494</v>
@@ -72490,13 +72496,13 @@
     </row>
     <row r="146" ht="12.75" customHeight="1">
       <c r="A146" s="50" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B146" s="50" t="s">
         <v>495</v>
       </c>
       <c r="C146" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D146" s="50" t="s">
         <v>496</v>
@@ -72510,13 +72516,13 @@
     </row>
     <row r="147" ht="12.75" customHeight="1">
       <c r="A147" s="50" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B147" s="50" t="s">
         <v>497</v>
       </c>
       <c r="C147" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D147" s="50" t="s">
         <v>498</v>
@@ -72530,13 +72536,13 @@
     </row>
     <row r="148" ht="12.75" customHeight="1">
       <c r="A148" s="50" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B148" s="50" t="s">
         <v>499</v>
       </c>
       <c r="C148" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D148" s="50" t="s">
         <v>500</v>
@@ -72550,13 +72556,13 @@
     </row>
     <row r="149" ht="12.75" customHeight="1">
       <c r="A149" s="50" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B149" s="50" t="s">
         <v>501</v>
       </c>
       <c r="C149" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D149" s="50" t="s">
         <v>502</v>
@@ -72570,13 +72576,13 @@
     </row>
     <row r="150" ht="12.75" customHeight="1">
       <c r="A150" s="50" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B150" s="50" t="s">
         <v>503</v>
       </c>
       <c r="C150" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D150" s="50" t="s">
         <v>504</v>
@@ -72590,13 +72596,13 @@
     </row>
     <row r="151" ht="12.75" customHeight="1">
       <c r="A151" s="50" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B151" s="50" t="s">
         <v>505</v>
       </c>
       <c r="C151" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D151" s="50" t="s">
         <v>506</v>
@@ -72609,62 +72615,74 @@
       </c>
     </row>
     <row r="152" ht="12.75" customHeight="1">
-      <c r="A152" s="52" t="s">
-        <v>476</v>
+      <c r="A152" s="50" t="s">
+        <v>482</v>
       </c>
       <c r="B152" s="50" t="s">
         <v>507</v>
       </c>
       <c r="C152" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D152" s="50" t="s">
         <v>508</v>
       </c>
-      <c r="E152" s="51"/>
-      <c r="F152" s="51"/>
+      <c r="E152" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="F152" s="51" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="153" ht="12.75" customHeight="1">
-      <c r="A153" s="52" t="s">
-        <v>476</v>
+      <c r="A153" s="50" t="s">
+        <v>482</v>
       </c>
       <c r="B153" s="50" t="s">
         <v>509</v>
       </c>
       <c r="C153" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D153" s="50" t="s">
         <v>510</v>
       </c>
-      <c r="E153" s="51"/>
-      <c r="F153" s="51"/>
+      <c r="E153" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="F153" s="51" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="154" ht="12.75" customHeight="1">
-      <c r="A154" s="52" t="s">
-        <v>476</v>
+      <c r="A154" s="50" t="s">
+        <v>482</v>
       </c>
       <c r="B154" s="50" t="s">
         <v>511</v>
       </c>
       <c r="C154" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D154" s="50" t="s">
         <v>512</v>
       </c>
-      <c r="E154" s="51"/>
-      <c r="F154" s="51"/>
+      <c r="E154" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="F154" s="51" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="155" ht="12.75" customHeight="1">
       <c r="A155" s="52" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B155" s="50" t="s">
         <v>513</v>
       </c>
       <c r="C155" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D155" s="50" t="s">
         <v>514</v>
@@ -72674,13 +72692,13 @@
     </row>
     <row r="156" ht="12.75" customHeight="1">
       <c r="A156" s="52" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B156" s="50" t="s">
         <v>515</v>
       </c>
       <c r="C156" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D156" s="50" t="s">
         <v>516</v>
@@ -72690,13 +72708,13 @@
     </row>
     <row r="157" ht="12.75" customHeight="1">
       <c r="A157" s="52" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B157" s="50" t="s">
         <v>517</v>
       </c>
       <c r="C157" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D157" s="50" t="s">
         <v>518</v>
@@ -72706,13 +72724,13 @@
     </row>
     <row r="158" ht="12.75" customHeight="1">
       <c r="A158" s="52" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B158" s="50" t="s">
         <v>519</v>
       </c>
       <c r="C158" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D158" s="50" t="s">
         <v>520</v>
@@ -72722,13 +72740,13 @@
     </row>
     <row r="159" ht="12.75" customHeight="1">
       <c r="A159" s="52" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B159" s="50" t="s">
         <v>521</v>
       </c>
       <c r="C159" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D159" s="50" t="s">
         <v>522</v>
@@ -72738,13 +72756,13 @@
     </row>
     <row r="160" ht="12.75" customHeight="1">
       <c r="A160" s="52" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B160" s="50" t="s">
         <v>523</v>
       </c>
       <c r="C160" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D160" s="50" t="s">
         <v>524</v>
@@ -72754,13 +72772,13 @@
     </row>
     <row r="161" ht="12.75" customHeight="1">
       <c r="A161" s="52" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B161" s="50" t="s">
         <v>525</v>
       </c>
       <c r="C161" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D161" s="50" t="s">
         <v>526</v>
@@ -72769,77 +72787,65 @@
       <c r="F161" s="51"/>
     </row>
     <row r="162" ht="12.75" customHeight="1">
-      <c r="A162" s="50" t="s">
+      <c r="A162" s="52" t="s">
+        <v>482</v>
+      </c>
+      <c r="B162" s="50" t="s">
         <v>527</v>
-      </c>
-      <c r="B162" s="50" t="s">
-        <v>481</v>
       </c>
       <c r="C162" s="50" t="s">
         <v>220</v>
       </c>
       <c r="D162" s="50" t="s">
+        <v>528</v>
+      </c>
+      <c r="E162" s="51"/>
+      <c r="F162" s="51"/>
+    </row>
+    <row r="163" ht="12.75" customHeight="1">
+      <c r="A163" s="52" t="s">
         <v>482</v>
       </c>
-      <c r="E162" s="51" t="s">
+      <c r="B163" s="50" t="s">
+        <v>529</v>
+      </c>
+      <c r="C163" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="F162" s="51" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="163" ht="12.75" customHeight="1">
-      <c r="A163" s="50" t="s">
-        <v>527</v>
-      </c>
-      <c r="B163" s="50" t="s">
-        <v>528</v>
-      </c>
-      <c r="C163" s="50" t="s">
-        <v>220</v>
-      </c>
       <c r="D163" s="50" t="s">
-        <v>283</v>
-      </c>
-      <c r="E163" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="F163" s="51" t="s">
-        <v>223</v>
-      </c>
+        <v>530</v>
+      </c>
+      <c r="E163" s="51"/>
+      <c r="F163" s="51"/>
     </row>
     <row r="164" ht="12.75" customHeight="1">
-      <c r="A164" s="50" t="s">
-        <v>527</v>
+      <c r="A164" s="52" t="s">
+        <v>482</v>
       </c>
       <c r="B164" s="50" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C164" s="50" t="s">
         <v>220</v>
       </c>
       <c r="D164" s="50" t="s">
-        <v>335</v>
-      </c>
-      <c r="E164" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="F164" s="51" t="s">
-        <v>223</v>
-      </c>
+        <v>532</v>
+      </c>
+      <c r="E164" s="51"/>
+      <c r="F164" s="51"/>
     </row>
     <row r="165" ht="12.75" customHeight="1">
       <c r="A165" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B165" s="50" t="s">
-        <v>530</v>
+        <v>487</v>
       </c>
       <c r="C165" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D165" s="50" t="s">
-        <v>531</v>
+        <v>488</v>
       </c>
       <c r="E165" s="51" t="s">
         <v>222</v>
@@ -72850,16 +72856,16 @@
     </row>
     <row r="166" ht="12.75" customHeight="1">
       <c r="A166" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B166" s="50" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="C166" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D166" s="50" t="s">
-        <v>462</v>
+        <v>283</v>
       </c>
       <c r="E166" s="51" t="s">
         <v>222</v>
@@ -72870,16 +72876,16 @@
     </row>
     <row r="167" ht="12.75" customHeight="1">
       <c r="A167" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B167" s="50" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="C167" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D167" s="50" t="s">
-        <v>534</v>
+        <v>335</v>
       </c>
       <c r="E167" s="51" t="s">
         <v>222</v>
@@ -72890,16 +72896,16 @@
     </row>
     <row r="168" ht="12.75" customHeight="1">
       <c r="A168" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B168" s="50" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C168" s="50" t="s">
         <v>222</v>
       </c>
       <c r="D168" s="50" t="s">
-        <v>488</v>
+        <v>537</v>
       </c>
       <c r="E168" s="51" t="s">
         <v>222</v>
@@ -72910,16 +72916,16 @@
     </row>
     <row r="169" ht="12.75" customHeight="1">
       <c r="A169" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B169" s="50" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C169" s="50" t="s">
         <v>222</v>
       </c>
       <c r="D169" s="50" t="s">
-        <v>537</v>
+        <v>462</v>
       </c>
       <c r="E169" s="51" t="s">
         <v>222</v>
@@ -72930,16 +72936,16 @@
     </row>
     <row r="170" ht="12.75" customHeight="1">
       <c r="A170" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B170" s="50" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C170" s="50" t="s">
         <v>222</v>
       </c>
       <c r="D170" s="50" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E170" s="51" t="s">
         <v>222</v>
@@ -72950,16 +72956,16 @@
     </row>
     <row r="171" ht="12.75" customHeight="1">
       <c r="A171" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B171" s="50" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C171" s="50" t="s">
         <v>222</v>
       </c>
       <c r="D171" s="50" t="s">
-        <v>541</v>
+        <v>494</v>
       </c>
       <c r="E171" s="51" t="s">
         <v>222</v>
@@ -72970,7 +72976,7 @@
     </row>
     <row r="172" ht="12.75" customHeight="1">
       <c r="A172" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B172" s="50" t="s">
         <v>542</v>
@@ -72979,7 +72985,7 @@
         <v>222</v>
       </c>
       <c r="D172" s="50" t="s">
-        <v>492</v>
+        <v>543</v>
       </c>
       <c r="E172" s="51" t="s">
         <v>222</v>
@@ -72990,16 +72996,16 @@
     </row>
     <row r="173" ht="12.75" customHeight="1">
       <c r="A173" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B173" s="50" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C173" s="50" t="s">
         <v>222</v>
       </c>
       <c r="D173" s="50" t="s">
-        <v>496</v>
+        <v>545</v>
       </c>
       <c r="E173" s="51" t="s">
         <v>222</v>
@@ -73010,16 +73016,16 @@
     </row>
     <row r="174" ht="12.75" customHeight="1">
       <c r="A174" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B174" s="50" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C174" s="50" t="s">
         <v>222</v>
       </c>
       <c r="D174" s="50" t="s">
-        <v>500</v>
+        <v>547</v>
       </c>
       <c r="E174" s="51" t="s">
         <v>222</v>
@@ -73030,16 +73036,16 @@
     </row>
     <row r="175" ht="12.75" customHeight="1">
       <c r="A175" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B175" s="50" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="C175" s="50" t="s">
         <v>222</v>
       </c>
       <c r="D175" s="50" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="E175" s="51" t="s">
         <v>222</v>
@@ -73050,16 +73056,16 @@
     </row>
     <row r="176" ht="12.75" customHeight="1">
       <c r="A176" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B176" s="50" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="C176" s="50" t="s">
-        <v>220</v>
-      </c>
-      <c r="D176" s="51" t="s">
-        <v>547</v>
+        <v>222</v>
+      </c>
+      <c r="D176" s="50" t="s">
+        <v>502</v>
       </c>
       <c r="E176" s="51" t="s">
         <v>222</v>
@@ -73070,16 +73076,16 @@
     </row>
     <row r="177" ht="12.75" customHeight="1">
       <c r="A177" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B177" s="50" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="C177" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D177" s="50" t="s">
-        <v>549</v>
+        <v>506</v>
       </c>
       <c r="E177" s="51" t="s">
         <v>222</v>
@@ -73090,16 +73096,16 @@
     </row>
     <row r="178" ht="12.75" customHeight="1">
       <c r="A178" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B178" s="50" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C178" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D178" s="50" t="s">
-        <v>551</v>
+        <v>510</v>
       </c>
       <c r="E178" s="51" t="s">
         <v>222</v>
@@ -73110,7 +73116,7 @@
     </row>
     <row r="179" ht="12.75" customHeight="1">
       <c r="A179" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B179" s="50" t="s">
         <v>552</v>
@@ -73118,7 +73124,7 @@
       <c r="C179" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="D179" s="50" t="s">
+      <c r="D179" s="51" t="s">
         <v>553</v>
       </c>
       <c r="E179" s="51" t="s">
@@ -73130,7 +73136,7 @@
     </row>
     <row r="180" ht="12.75" customHeight="1">
       <c r="A180" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B180" s="50" t="s">
         <v>554</v>
@@ -73150,7 +73156,7 @@
     </row>
     <row r="181" ht="12.75" customHeight="1">
       <c r="A181" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B181" s="50" t="s">
         <v>556</v>
@@ -73170,7 +73176,7 @@
     </row>
     <row r="182" ht="12.75" customHeight="1">
       <c r="A182" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B182" s="50" t="s">
         <v>558</v>
@@ -73190,7 +73196,7 @@
     </row>
     <row r="183" ht="12.75" customHeight="1">
       <c r="A183" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B183" s="50" t="s">
         <v>560</v>
@@ -73210,7 +73216,7 @@
     </row>
     <row r="184" ht="12.75" customHeight="1">
       <c r="A184" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B184" s="50" t="s">
         <v>562</v>
@@ -73230,13 +73236,13 @@
     </row>
     <row r="185" ht="12.75" customHeight="1">
       <c r="A185" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B185" s="50" t="s">
         <v>564</v>
       </c>
       <c r="C185" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D185" s="50" t="s">
         <v>565</v>
@@ -73250,7 +73256,7 @@
     </row>
     <row r="186" ht="12.75" customHeight="1">
       <c r="A186" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B186" s="50" t="s">
         <v>566</v>
@@ -73270,13 +73276,13 @@
     </row>
     <row r="187" ht="12.75" customHeight="1">
       <c r="A187" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B187" s="50" t="s">
         <v>568</v>
       </c>
       <c r="C187" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D187" s="50" t="s">
         <v>569</v>
@@ -73290,16 +73296,16 @@
     </row>
     <row r="188" ht="12.75" customHeight="1">
       <c r="A188" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B188" s="50" t="s">
         <v>570</v>
       </c>
       <c r="C188" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D188" s="50" t="s">
-        <v>335</v>
+        <v>571</v>
       </c>
       <c r="E188" s="51" t="s">
         <v>222</v>
@@ -73310,16 +73316,16 @@
     </row>
     <row r="189" ht="12.75" customHeight="1">
       <c r="A189" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B189" s="50" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C189" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D189" s="50" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E189" s="51" t="s">
         <v>222</v>
@@ -73330,16 +73336,16 @@
     </row>
     <row r="190" ht="12.75" customHeight="1">
       <c r="A190" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B190" s="50" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C190" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D190" s="50" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="E190" s="51" t="s">
         <v>222</v>
@@ -73350,16 +73356,16 @@
     </row>
     <row r="191" ht="12.75" customHeight="1">
       <c r="A191" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B191" s="50" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C191" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D191" s="50" t="s">
-        <v>508</v>
+        <v>335</v>
       </c>
       <c r="E191" s="51" t="s">
         <v>222</v>
@@ -73370,16 +73376,16 @@
     </row>
     <row r="192" ht="12.75" customHeight="1">
       <c r="A192" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B192" s="50" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C192" s="50" t="s">
         <v>222</v>
       </c>
       <c r="D192" s="50" t="s">
-        <v>512</v>
+        <v>578</v>
       </c>
       <c r="E192" s="51" t="s">
         <v>222</v>
@@ -73390,16 +73396,16 @@
     </row>
     <row r="193" ht="12.75" customHeight="1">
       <c r="A193" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B193" s="50" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="C193" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D193" s="50" t="s">
-        <v>516</v>
+        <v>580</v>
       </c>
       <c r="E193" s="51" t="s">
         <v>222</v>
@@ -73410,16 +73416,16 @@
     </row>
     <row r="194" ht="12.75" customHeight="1">
       <c r="A194" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B194" s="50" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="C194" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D194" s="50" t="s">
-        <v>579</v>
+        <v>514</v>
       </c>
       <c r="E194" s="51" t="s">
         <v>222</v>
@@ -73430,16 +73436,16 @@
     </row>
     <row r="195" ht="12.75" customHeight="1">
       <c r="A195" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B195" s="50" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C195" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D195" s="50" t="s">
-        <v>581</v>
+        <v>518</v>
       </c>
       <c r="E195" s="51" t="s">
         <v>222</v>
@@ -73450,16 +73456,16 @@
     </row>
     <row r="196" ht="12.75" customHeight="1">
       <c r="A196" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B196" s="50" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C196" s="50" t="s">
         <v>222</v>
       </c>
       <c r="D196" s="50" t="s">
-        <v>565</v>
+        <v>522</v>
       </c>
       <c r="E196" s="51" t="s">
         <v>222</v>
@@ -73470,16 +73476,16 @@
     </row>
     <row r="197" ht="12.75" customHeight="1">
       <c r="A197" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B197" s="50" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C197" s="50" t="s">
         <v>220</v>
       </c>
       <c r="D197" s="50" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="E197" s="51" t="s">
         <v>222</v>
@@ -73490,16 +73496,16 @@
     </row>
     <row r="198" ht="12.75" customHeight="1">
       <c r="A198" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B198" s="50" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C198" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D198" s="50" t="s">
-        <v>569</v>
+        <v>587</v>
       </c>
       <c r="E198" s="51" t="s">
         <v>222</v>
@@ -73510,16 +73516,16 @@
     </row>
     <row r="199" ht="12.75" customHeight="1">
       <c r="A199" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B199" s="50" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C199" s="50" t="s">
         <v>222</v>
       </c>
       <c r="D199" s="50" t="s">
-        <v>587</v>
+        <v>571</v>
       </c>
       <c r="E199" s="51" t="s">
         <v>222</v>
@@ -73530,16 +73536,16 @@
     </row>
     <row r="200" ht="12.75" customHeight="1">
       <c r="A200" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B200" s="50" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C200" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D200" s="50" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="E200" s="51" t="s">
         <v>222</v>
@@ -73550,16 +73556,16 @@
     </row>
     <row r="201" ht="12.75" customHeight="1">
       <c r="A201" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B201" s="50" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C201" s="50" t="s">
         <v>222</v>
       </c>
       <c r="D201" s="50" t="s">
-        <v>591</v>
+        <v>575</v>
       </c>
       <c r="E201" s="51" t="s">
         <v>222</v>
@@ -73570,7 +73576,7 @@
     </row>
     <row r="202" ht="12.75" customHeight="1">
       <c r="A202" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B202" s="50" t="s">
         <v>592</v>
@@ -73590,7 +73596,7 @@
     </row>
     <row r="203" ht="12.75" customHeight="1">
       <c r="A203" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B203" s="50" t="s">
         <v>594</v>
@@ -73610,7 +73616,7 @@
     </row>
     <row r="204" ht="12.75" customHeight="1">
       <c r="A204" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B204" s="50" t="s">
         <v>596</v>
@@ -73630,7 +73636,7 @@
     </row>
     <row r="205" ht="12.75" customHeight="1">
       <c r="A205" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B205" s="50" t="s">
         <v>598</v>
@@ -73650,7 +73656,7 @@
     </row>
     <row r="206" ht="12.75" customHeight="1">
       <c r="A206" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B206" s="50" t="s">
         <v>600</v>
@@ -73670,7 +73676,7 @@
     </row>
     <row r="207" ht="12.75" customHeight="1">
       <c r="A207" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B207" s="50" t="s">
         <v>602</v>
@@ -73690,7 +73696,7 @@
     </row>
     <row r="208" ht="12.75" customHeight="1">
       <c r="A208" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B208" s="50" t="s">
         <v>604</v>
@@ -73710,7 +73716,7 @@
     </row>
     <row r="209" ht="12.75" customHeight="1">
       <c r="A209" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B209" s="50" t="s">
         <v>606</v>
@@ -73719,7 +73725,7 @@
         <v>222</v>
       </c>
       <c r="D209" s="50" t="s">
-        <v>520</v>
+        <v>607</v>
       </c>
       <c r="E209" s="51" t="s">
         <v>222</v>
@@ -73730,16 +73736,16 @@
     </row>
     <row r="210" ht="12.75" customHeight="1">
       <c r="A210" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B210" s="50" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C210" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D210" s="50" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="E210" s="51" t="s">
         <v>222</v>
@@ -73750,16 +73756,16 @@
     </row>
     <row r="211" ht="12.75" customHeight="1">
       <c r="A211" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B211" s="50" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C211" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D211" s="50" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E211" s="51" t="s">
         <v>222</v>
@@ -73770,16 +73776,16 @@
     </row>
     <row r="212" ht="12.75" customHeight="1">
       <c r="A212" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B212" s="50" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C212" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D212" s="50" t="s">
-        <v>612</v>
+        <v>526</v>
       </c>
       <c r="E212" s="51" t="s">
         <v>222</v>
@@ -73790,7 +73796,7 @@
     </row>
     <row r="213" ht="12.75" customHeight="1">
       <c r="A213" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B213" s="50" t="s">
         <v>613</v>
@@ -73810,7 +73816,7 @@
     </row>
     <row r="214" ht="12.75" customHeight="1">
       <c r="A214" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B214" s="50" t="s">
         <v>615</v>
@@ -73830,7 +73836,7 @@
     </row>
     <row r="215" ht="12.75" customHeight="1">
       <c r="A215" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B215" s="50" t="s">
         <v>617</v>
@@ -73850,7 +73856,7 @@
     </row>
     <row r="216" ht="12.75" customHeight="1">
       <c r="A216" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B216" s="50" t="s">
         <v>619</v>
@@ -73870,7 +73876,7 @@
     </row>
     <row r="217" ht="12.75" customHeight="1">
       <c r="A217" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B217" s="50" t="s">
         <v>621</v>
@@ -73890,7 +73896,7 @@
     </row>
     <row r="218" ht="12.75" customHeight="1">
       <c r="A218" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B218" s="50" t="s">
         <v>623</v>
@@ -73910,16 +73916,16 @@
     </row>
     <row r="219" ht="12.75" customHeight="1">
       <c r="A219" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B219" s="50" t="s">
         <v>625</v>
       </c>
       <c r="C219" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D219" s="50" t="s">
-        <v>565</v>
+        <v>626</v>
       </c>
       <c r="E219" s="51" t="s">
         <v>222</v>
@@ -73930,16 +73936,16 @@
     </row>
     <row r="220" ht="12.75" customHeight="1">
       <c r="A220" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B220" s="50" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C220" s="50" t="s">
         <v>220</v>
       </c>
       <c r="D220" s="50" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="E220" s="51" t="s">
         <v>222</v>
@@ -73950,16 +73956,16 @@
     </row>
     <row r="221" ht="12.75" customHeight="1">
       <c r="A221" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B221" s="50" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C221" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D221" s="50" t="s">
-        <v>569</v>
+        <v>630</v>
       </c>
       <c r="E221" s="51" t="s">
         <v>222</v>
@@ -73970,16 +73976,16 @@
     </row>
     <row r="222" ht="12.75" customHeight="1">
       <c r="A222" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B222" s="50" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="C222" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D222" s="50" t="s">
-        <v>630</v>
+        <v>571</v>
       </c>
       <c r="E222" s="51" t="s">
         <v>222</v>
@@ -73990,16 +73996,16 @@
     </row>
     <row r="223" ht="12.75" customHeight="1">
       <c r="A223" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B223" s="50" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="C223" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D223" s="50" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="E223" s="51" t="s">
         <v>222</v>
@@ -74010,16 +74016,16 @@
     </row>
     <row r="224" ht="12.75" customHeight="1">
       <c r="A224" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B224" s="50" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C224" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D224" s="50" t="s">
-        <v>634</v>
+        <v>575</v>
       </c>
       <c r="E224" s="51" t="s">
         <v>222</v>
@@ -74030,7 +74036,7 @@
     </row>
     <row r="225" ht="12.75" customHeight="1">
       <c r="A225" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B225" s="50" t="s">
         <v>635</v>
@@ -74050,13 +74056,13 @@
     </row>
     <row r="226" ht="12.75" customHeight="1">
       <c r="A226" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B226" s="50" t="s">
         <v>637</v>
       </c>
       <c r="C226" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D226" s="50" t="s">
         <v>638</v>
@@ -74070,7 +74076,7 @@
     </row>
     <row r="227" ht="12.75" customHeight="1">
       <c r="A227" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B227" s="50" t="s">
         <v>639</v>
@@ -74090,13 +74096,13 @@
     </row>
     <row r="228" ht="12.75" customHeight="1">
       <c r="A228" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B228" s="50" t="s">
         <v>641</v>
       </c>
       <c r="C228" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D228" s="50" t="s">
         <v>642</v>
@@ -74110,13 +74116,13 @@
     </row>
     <row r="229" ht="12.75" customHeight="1">
       <c r="A229" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B229" s="50" t="s">
         <v>643</v>
       </c>
       <c r="C229" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D229" s="50" t="s">
         <v>644</v>
@@ -74130,7 +74136,7 @@
     </row>
     <row r="230" ht="12.75" customHeight="1">
       <c r="A230" s="50" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B230" s="50" t="s">
         <v>645</v>
@@ -74139,7 +74145,7 @@
         <v>220</v>
       </c>
       <c r="D230" s="50" t="s">
-        <v>283</v>
+        <v>646</v>
       </c>
       <c r="E230" s="51" t="s">
         <v>222</v>
@@ -74149,68 +74155,125 @@
       </c>
     </row>
     <row r="231" ht="12.75" customHeight="1">
-      <c r="A231" s="54" t="s">
-        <v>527</v>
+      <c r="A231" s="50" t="s">
+        <v>533</v>
       </c>
       <c r="B231" s="50" t="s">
-        <v>646</v>
-      </c>
-      <c r="C231" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="C231" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="D231" s="50" t="s">
+        <v>648</v>
+      </c>
+      <c r="E231" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="F231" s="51" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="232" ht="12.75" customHeight="1">
+      <c r="A232" s="50" t="s">
+        <v>533</v>
+      </c>
+      <c r="B232" s="50" t="s">
+        <v>649</v>
+      </c>
+      <c r="C232" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="D232" s="50" t="s">
+        <v>650</v>
+      </c>
+      <c r="E232" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="F232" s="51" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="233" ht="12.75" customHeight="1">
+      <c r="A233" s="50" t="s">
+        <v>533</v>
+      </c>
+      <c r="B233" s="50" t="s">
+        <v>651</v>
+      </c>
+      <c r="C233" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="D231" s="54" t="s">
-        <v>647</v>
-      </c>
-      <c r="E231" s="54" t="s">
+      <c r="D233" s="50" t="s">
+        <v>283</v>
+      </c>
+      <c r="E233" s="51" t="s">
         <v>222</v>
       </c>
-      <c r="F231" s="54" t="s">
+      <c r="F233" s="51" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="232" ht="12.75" customHeight="1">
-      <c r="A232" s="54" t="s">
-        <v>527</v>
-      </c>
-      <c r="B232" s="55" t="s">
-        <v>648</v>
-      </c>
-      <c r="C232" s="54" t="s">
+    <row r="234" ht="12.75" customHeight="1">
+      <c r="A234" s="54" t="s">
+        <v>533</v>
+      </c>
+      <c r="B234" s="50" t="s">
+        <v>652</v>
+      </c>
+      <c r="C234" s="54" t="s">
         <v>220</v>
       </c>
-      <c r="D232" s="54" t="s">
-        <v>649</v>
-      </c>
-      <c r="E232" s="54" t="s">
+      <c r="D234" s="54" t="s">
+        <v>653</v>
+      </c>
+      <c r="E234" s="54" t="s">
         <v>222</v>
       </c>
-      <c r="F232" s="54" t="s">
+      <c r="F234" s="54" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="233" ht="12.75" customHeight="1">
-      <c r="A233" s="54" t="s">
-        <v>527</v>
-      </c>
-      <c r="B233" s="56" t="s">
-        <v>650</v>
-      </c>
-      <c r="C233" s="54" t="s">
+    <row r="235" ht="12.75" customHeight="1">
+      <c r="A235" s="54" t="s">
+        <v>533</v>
+      </c>
+      <c r="B235" s="55" t="s">
+        <v>654</v>
+      </c>
+      <c r="C235" s="54" t="s">
         <v>220</v>
       </c>
-      <c r="D233" s="57" t="s">
-        <v>651</v>
-      </c>
-      <c r="E233" s="54" t="s">
+      <c r="D235" s="54" t="s">
+        <v>655</v>
+      </c>
+      <c r="E235" s="54" t="s">
         <v>222</v>
       </c>
-      <c r="F233" s="54" t="s">
+      <c r="F235" s="54" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="234" ht="12.75" customHeight="1"/>
-    <row r="235" ht="12.75" customHeight="1"/>
-    <row r="236" ht="12.75" customHeight="1"/>
+    <row r="236" ht="12.75" customHeight="1">
+      <c r="A236" s="54" t="s">
+        <v>533</v>
+      </c>
+      <c r="B236" s="56" t="s">
+        <v>656</v>
+      </c>
+      <c r="C236" s="54" t="s">
+        <v>220</v>
+      </c>
+      <c r="D236" s="57" t="s">
+        <v>657</v>
+      </c>
+      <c r="E236" s="54" t="s">
+        <v>222</v>
+      </c>
+      <c r="F236" s="54" t="s">
+        <v>223</v>
+      </c>
+    </row>
     <row r="237" ht="12.75" customHeight="1"/>
     <row r="238" ht="12.75" customHeight="1"/>
     <row r="239" ht="12.75" customHeight="1"/>
@@ -75079,6 +75142,9 @@
     <row r="1102" ht="12.75" customHeight="1"/>
     <row r="1103" ht="12.75" customHeight="1"/>
     <row r="1104" ht="12.75" customHeight="1"/>
+    <row r="1105" ht="12.75" customHeight="1"/>
+    <row r="1106" ht="12.75" customHeight="1"/>
+    <row r="1107" ht="12.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>